<commit_message>
update RP 3 and code
</commit_message>
<xml_diff>
--- a/doc/requirement/RFID_UseCase_v1.0.xlsx
+++ b/doc/requirement/RFID_UseCase_v1.0.xlsx
@@ -1,33 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Normal_User\Desktop\RFID\doc\requirement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lyvam\Desktop\RFID\doc\requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18600" windowHeight="8850" tabRatio="922" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="18600" windowHeight="8850" tabRatio="922" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ChangeHistory" sheetId="1" r:id="rId1"/>
     <sheet name="Cover" sheetId="2" r:id="rId2"/>
-    <sheet name="Đăng kí thẻ" sheetId="3" r:id="rId3"/>
-    <sheet name="Gọi tên" sheetId="4" r:id="rId4"/>
-    <sheet name="Template" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
+    <sheet name="Đăng kí thẻ" sheetId="3" r:id="rId4"/>
+    <sheet name="Gọi tên" sheetId="4" r:id="rId5"/>
+    <sheet name="abc" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_Fill" localSheetId="4" hidden="1">#REF!</definedName>
+    <definedName name="_Fill" localSheetId="5" hidden="1">#REF!</definedName>
     <definedName name="_Fill" hidden="1">#REF!</definedName>
-    <definedName name="_Key1" localSheetId="4" hidden="1">#REF!</definedName>
+    <definedName name="_Key1" localSheetId="5" hidden="1">#REF!</definedName>
     <definedName name="_Key1" hidden="1">#REF!</definedName>
-    <definedName name="_Key2" localSheetId="4" hidden="1">#REF!</definedName>
+    <definedName name="_Key2" localSheetId="5" hidden="1">#REF!</definedName>
     <definedName name="_Key2" hidden="1">#REF!</definedName>
     <definedName name="_Order1" hidden="1">255</definedName>
     <definedName name="_Order2" hidden="1">255</definedName>
-    <definedName name="_Sort" localSheetId="4" hidden="1">#REF!</definedName>
+    <definedName name="_Sort" localSheetId="5" hidden="1">#REF!</definedName>
     <definedName name="_Sort" hidden="1">#REF!</definedName>
     <definedName name="abc" hidden="1">{#N/A,#N/A,TRUE,"商品マスター";#N/A,#N/A,TRUE,"店舗マスター";#N/A,#N/A,TRUE,"在庫マスター";#N/A,#N/A,TRUE,"カレンダーマスター";#N/A,#N/A,TRUE,"分類コード変換マスター";#N/A,#N/A,TRUE,"重点型番マスター";#N/A,#N/A,TRUE,"商品分類コードマスター";#N/A,#N/A,TRUE,"商品分類別店舗型定義";#N/A,#N/A,TRUE,"日別店舗別型別実績 ";#N/A,#N/A,TRUE,"週間店舗別型別実績 ";#N/A,#N/A,TRUE,"月度店舗別型別実績";#N/A,#N/A,TRUE,"四半期店舗別型別実績 ";#N/A,#N/A,TRUE,"年間店舗別型別実績";#N/A,#N/A,TRUE,"日別店舗別小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別小分類実績 ";#N/A,#N/A,TRUE,"月度店舗別小分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別小分類実績 ";#N/A,#N/A,TRUE,"日別店舗別中分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中分類実績 ";#N/A,#N/A,TRUE,"月度店舗別中分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別中分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中分類実績";#N/A,#N/A,TRUE,"日別店舗別中小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中小分類実績";#N/A,#N/A,TRUE,"月度店舗別中小分類実績";#N/A,#N/A,TRUE,"四半期店舗別中小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中小分類実績";#N/A,#N/A,TRUE,"日別店舗別大分類実績";#N/A,#N/A,TRUE,"週間店舗別大分類実績";#N/A,#N/A,TRUE,"月度店舗別大分類実績";#N/A,#N/A,TRUE,"四半期店舗別大分類別実績";#N/A,#N/A,TRUE,"年度店舗別大分類実績 ";#N/A,#N/A,TRUE,"日別店舗別商品群実績 ";#N/A,#N/A,TRUE,"週間店舗別商品群実績 ";#N/A,#N/A,TRUE,"月度店舗別商品群実績";#N/A,#N/A,TRUE,"四半期別商品群実績";#N/A,#N/A,TRUE,"年間店舗別商品群実績";#N/A,#N/A,TRUE,"日別型別実績";#N/A,#N/A,TRUE,"週間型別実績";#N/A,#N/A,TRUE,"月度型別実績";#N/A,#N/A,TRUE,"四半期型別実績";#N/A,#N/A,TRUE,"年間型別実績";#N/A,#N/A,TRUE,"日別小分類実績";#N/A,#N/A,TRUE,"週間小分類実績";#N/A,#N/A,TRUE,"月度小分類実績";#N/A,#N/A,TRUE,"四半期小分類実績";#N/A,#N/A,TRUE,"年度小分類実績";#N/A,#N/A,TRUE,"日別中分類実績";#N/A,#N/A,TRUE,"週間中分類実績";#N/A,#N/A,TRUE,"月度中分類実績";#N/A,#N/A,TRUE,"四半期中分類実績";#N/A,#N/A,TRUE,"年度中分類実績";#N/A,#N/A,TRUE,"日別中小分類実績"}</definedName>
     <definedName name="abcv" hidden="1">{#N/A,#N/A,TRUE,"商品マスター";#N/A,#N/A,TRUE,"店舗マスター";#N/A,#N/A,TRUE,"在庫マスター";#N/A,#N/A,TRUE,"カレンダーマスター";#N/A,#N/A,TRUE,"分類コード変換マスター";#N/A,#N/A,TRUE,"重点型番マスター";#N/A,#N/A,TRUE,"商品分類コードマスター";#N/A,#N/A,TRUE,"商品分類別店舗型定義";#N/A,#N/A,TRUE,"日別店舗別型別実績 ";#N/A,#N/A,TRUE,"週間店舗別型別実績 ";#N/A,#N/A,TRUE,"月度店舗別型別実績";#N/A,#N/A,TRUE,"四半期店舗別型別実績 ";#N/A,#N/A,TRUE,"年間店舗別型別実績";#N/A,#N/A,TRUE,"日別店舗別小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別小分類実績 ";#N/A,#N/A,TRUE,"月度店舗別小分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別小分類実績 ";#N/A,#N/A,TRUE,"日別店舗別中分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中分類実績 ";#N/A,#N/A,TRUE,"月度店舗別中分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別中分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中分類実績";#N/A,#N/A,TRUE,"日別店舗別中小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中小分類実績";#N/A,#N/A,TRUE,"月度店舗別中小分類実績";#N/A,#N/A,TRUE,"四半期店舗別中小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中小分類実績";#N/A,#N/A,TRUE,"日別店舗別大分類実績";#N/A,#N/A,TRUE,"週間店舗別大分類実績";#N/A,#N/A,TRUE,"月度店舗別大分類実績";#N/A,#N/A,TRUE,"四半期店舗別大分類別実績";#N/A,#N/A,TRUE,"年度店舗別大分類実績 ";#N/A,#N/A,TRUE,"日別店舗別商品群実績 ";#N/A,#N/A,TRUE,"週間店舗別商品群実績 ";#N/A,#N/A,TRUE,"月度店舗別商品群実績";#N/A,#N/A,TRUE,"四半期別商品群実績";#N/A,#N/A,TRUE,"年間店舗別商品群実績";#N/A,#N/A,TRUE,"日別型別実績";#N/A,#N/A,TRUE,"週間型別実績";#N/A,#N/A,TRUE,"月度型別実績";#N/A,#N/A,TRUE,"四半期型別実績";#N/A,#N/A,TRUE,"年間型別実績";#N/A,#N/A,TRUE,"日別小分類実績";#N/A,#N/A,TRUE,"週間小分類実績";#N/A,#N/A,TRUE,"月度小分類実績";#N/A,#N/A,TRUE,"四半期小分類実績";#N/A,#N/A,TRUE,"年度小分類実績";#N/A,#N/A,TRUE,"日別中分類実績";#N/A,#N/A,TRUE,"週間中分類実績";#N/A,#N/A,TRUE,"月度中分類実績";#N/A,#N/A,TRUE,"四半期中分類実績";#N/A,#N/A,TRUE,"年度中分類実績";#N/A,#N/A,TRUE,"日別中小分類実績"}</definedName>
@@ -55,20 +56,20 @@
     <definedName name="LDC見積" hidden="1">{#N/A,#N/A,TRUE,"商品マスター";#N/A,#N/A,TRUE,"店舗マスター";#N/A,#N/A,TRUE,"在庫マスター";#N/A,#N/A,TRUE,"カレンダーマスター";#N/A,#N/A,TRUE,"分類コード変換マスター";#N/A,#N/A,TRUE,"重点型番マスター";#N/A,#N/A,TRUE,"商品分類コードマスター";#N/A,#N/A,TRUE,"商品分類別店舗型定義";#N/A,#N/A,TRUE,"日別店舗別型別実績 ";#N/A,#N/A,TRUE,"週間店舗別型別実績 ";#N/A,#N/A,TRUE,"月度店舗別型別実績";#N/A,#N/A,TRUE,"四半期店舗別型別実績 ";#N/A,#N/A,TRUE,"年間店舗別型別実績";#N/A,#N/A,TRUE,"日別店舗別小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別小分類実績 ";#N/A,#N/A,TRUE,"月度店舗別小分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別小分類実績 ";#N/A,#N/A,TRUE,"日別店舗別中分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中分類実績 ";#N/A,#N/A,TRUE,"月度店舗別中分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別中分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中分類実績";#N/A,#N/A,TRUE,"日別店舗別中小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中小分類実績";#N/A,#N/A,TRUE,"月度店舗別中小分類実績";#N/A,#N/A,TRUE,"四半期店舗別中小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中小分類実績";#N/A,#N/A,TRUE,"日別店舗別大分類実績";#N/A,#N/A,TRUE,"週間店舗別大分類実績";#N/A,#N/A,TRUE,"月度店舗別大分類実績";#N/A,#N/A,TRUE,"四半期店舗別大分類別実績";#N/A,#N/A,TRUE,"年度店舗別大分類実績 ";#N/A,#N/A,TRUE,"日別店舗別商品群実績 ";#N/A,#N/A,TRUE,"週間店舗別商品群実績 ";#N/A,#N/A,TRUE,"月度店舗別商品群実績";#N/A,#N/A,TRUE,"四半期別商品群実績";#N/A,#N/A,TRUE,"年間店舗別商品群実績";#N/A,#N/A,TRUE,"日別型別実績";#N/A,#N/A,TRUE,"週間型別実績";#N/A,#N/A,TRUE,"月度型別実績";#N/A,#N/A,TRUE,"四半期型別実績";#N/A,#N/A,TRUE,"年間型別実績";#N/A,#N/A,TRUE,"日別小分類実績";#N/A,#N/A,TRUE,"週間小分類実績";#N/A,#N/A,TRUE,"月度小分類実績";#N/A,#N/A,TRUE,"四半期小分類実績";#N/A,#N/A,TRUE,"年度小分類実績";#N/A,#N/A,TRUE,"日別中分類実績";#N/A,#N/A,TRUE,"週間中分類実績";#N/A,#N/A,TRUE,"月度中分類実績";#N/A,#N/A,TRUE,"四半期中分類実績";#N/A,#N/A,TRUE,"年度中分類実績";#N/A,#N/A,TRUE,"日別中小分類実績"}</definedName>
     <definedName name="ｌｌｌ" hidden="1">{#N/A,#N/A,TRUE,"商品マスター";#N/A,#N/A,TRUE,"店舗マスター";#N/A,#N/A,TRUE,"在庫マスター";#N/A,#N/A,TRUE,"カレンダーマスター";#N/A,#N/A,TRUE,"分類コード変換マスター";#N/A,#N/A,TRUE,"重点型番マスター";#N/A,#N/A,TRUE,"商品分類コードマスター";#N/A,#N/A,TRUE,"商品分類別店舗型定義";#N/A,#N/A,TRUE,"日別店舗別型別実績 ";#N/A,#N/A,TRUE,"週間店舗別型別実績 ";#N/A,#N/A,TRUE,"月度店舗別型別実績";#N/A,#N/A,TRUE,"四半期店舗別型別実績 ";#N/A,#N/A,TRUE,"年間店舗別型別実績";#N/A,#N/A,TRUE,"日別店舗別小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別小分類実績 ";#N/A,#N/A,TRUE,"月度店舗別小分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別小分類実績 ";#N/A,#N/A,TRUE,"日別店舗別中分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中分類実績 ";#N/A,#N/A,TRUE,"月度店舗別中分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別中分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中分類実績";#N/A,#N/A,TRUE,"日別店舗別中小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中小分類実績";#N/A,#N/A,TRUE,"月度店舗別中小分類実績";#N/A,#N/A,TRUE,"四半期店舗別中小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中小分類実績";#N/A,#N/A,TRUE,"日別店舗別大分類実績";#N/A,#N/A,TRUE,"週間店舗別大分類実績";#N/A,#N/A,TRUE,"月度店舗別大分類実績";#N/A,#N/A,TRUE,"四半期店舗別大分類別実績";#N/A,#N/A,TRUE,"年度店舗別大分類実績 ";#N/A,#N/A,TRUE,"日別店舗別商品群実績 ";#N/A,#N/A,TRUE,"週間店舗別商品群実績 ";#N/A,#N/A,TRUE,"月度店舗別商品群実績";#N/A,#N/A,TRUE,"四半期別商品群実績";#N/A,#N/A,TRUE,"年間店舗別商品群実績";#N/A,#N/A,TRUE,"日別型別実績";#N/A,#N/A,TRUE,"週間型別実績";#N/A,#N/A,TRUE,"月度型別実績";#N/A,#N/A,TRUE,"四半期型別実績";#N/A,#N/A,TRUE,"年間型別実績";#N/A,#N/A,TRUE,"日別小分類実績";#N/A,#N/A,TRUE,"週間小分類実績";#N/A,#N/A,TRUE,"月度小分類実績";#N/A,#N/A,TRUE,"四半期小分類実績";#N/A,#N/A,TRUE,"年度小分類実績";#N/A,#N/A,TRUE,"日別中分類実績";#N/A,#N/A,TRUE,"週間中分類実績";#N/A,#N/A,TRUE,"月度中分類実績";#N/A,#N/A,TRUE,"四半期中分類実績";#N/A,#N/A,TRUE,"年度中分類実績";#N/A,#N/A,TRUE,"日別中小分類実績"}</definedName>
     <definedName name="Nam" hidden="1">{#N/A,#N/A,TRUE,"商品マスター";#N/A,#N/A,TRUE,"店舗マスター";#N/A,#N/A,TRUE,"在庫マスター";#N/A,#N/A,TRUE,"カレンダーマスター";#N/A,#N/A,TRUE,"分類コード変換マスター";#N/A,#N/A,TRUE,"重点型番マスター";#N/A,#N/A,TRUE,"商品分類コードマスター";#N/A,#N/A,TRUE,"商品分類別店舗型定義";#N/A,#N/A,TRUE,"日別店舗別型別実績 ";#N/A,#N/A,TRUE,"週間店舗別型別実績 ";#N/A,#N/A,TRUE,"月度店舗別型別実績";#N/A,#N/A,TRUE,"四半期店舗別型別実績 ";#N/A,#N/A,TRUE,"年間店舗別型別実績";#N/A,#N/A,TRUE,"日別店舗別小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別小分類実績 ";#N/A,#N/A,TRUE,"月度店舗別小分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別小分類実績 ";#N/A,#N/A,TRUE,"日別店舗別中分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中分類実績 ";#N/A,#N/A,TRUE,"月度店舗別中分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別中分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中分類実績";#N/A,#N/A,TRUE,"日別店舗別中小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中小分類実績";#N/A,#N/A,TRUE,"月度店舗別中小分類実績";#N/A,#N/A,TRUE,"四半期店舗別中小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中小分類実績";#N/A,#N/A,TRUE,"日別店舗別大分類実績";#N/A,#N/A,TRUE,"週間店舗別大分類実績";#N/A,#N/A,TRUE,"月度店舗別大分類実績";#N/A,#N/A,TRUE,"四半期店舗別大分類別実績";#N/A,#N/A,TRUE,"年度店舗別大分類実績 ";#N/A,#N/A,TRUE,"日別店舗別商品群実績 ";#N/A,#N/A,TRUE,"週間店舗別商品群実績 ";#N/A,#N/A,TRUE,"月度店舗別商品群実績";#N/A,#N/A,TRUE,"四半期別商品群実績";#N/A,#N/A,TRUE,"年間店舗別商品群実績";#N/A,#N/A,TRUE,"日別型別実績";#N/A,#N/A,TRUE,"週間型別実績";#N/A,#N/A,TRUE,"月度型別実績";#N/A,#N/A,TRUE,"四半期型別実績";#N/A,#N/A,TRUE,"年間型別実績";#N/A,#N/A,TRUE,"日別小分類実績";#N/A,#N/A,TRUE,"週間小分類実績";#N/A,#N/A,TRUE,"月度小分類実績";#N/A,#N/A,TRUE,"四半期小分類実績";#N/A,#N/A,TRUE,"年度小分類実績";#N/A,#N/A,TRUE,"日別中分類実績";#N/A,#N/A,TRUE,"週間中分類実績";#N/A,#N/A,TRUE,"月度中分類実績";#N/A,#N/A,TRUE,"四半期中分類実績";#N/A,#N/A,TRUE,"年度中分類実績";#N/A,#N/A,TRUE,"日別中小分類実績"}</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">abc!$A$1:$AR$92</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ChangeHistory!$A$1:$G$39</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Cover!$A$1:$AP$92</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Đăng kí thẻ'!$A$1:$AR$72</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Gọi tên'!$A$1:$AR$97</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">Template!$A$1:$AR$92</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Đăng kí thẻ'!$A$1:$AR$72</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Gọi tên'!$A$1:$AR$97</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="5">abc!$1:4</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Cover!$1:4</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Đăng kí thẻ'!$1:4</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="3">'Gọi tên'!$1:4</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="4">Template!$1:4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">'Đăng kí thẻ'!$1:4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="4">'Gọi tên'!$1:4</definedName>
     <definedName name="qq" hidden="1">{#N/A,#N/A,TRUE,"商品マスター";#N/A,#N/A,TRUE,"店舗マスター";#N/A,#N/A,TRUE,"在庫マスター";#N/A,#N/A,TRUE,"カレンダーマスター";#N/A,#N/A,TRUE,"分類コード変換マスター";#N/A,#N/A,TRUE,"重点型番マスター";#N/A,#N/A,TRUE,"商品分類コードマスター";#N/A,#N/A,TRUE,"商品分類別店舗型定義";#N/A,#N/A,TRUE,"日別店舗別型別実績 ";#N/A,#N/A,TRUE,"週間店舗別型別実績 ";#N/A,#N/A,TRUE,"月度店舗別型別実績";#N/A,#N/A,TRUE,"四半期店舗別型別実績 ";#N/A,#N/A,TRUE,"年間店舗別型別実績";#N/A,#N/A,TRUE,"日別店舗別小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別小分類実績 ";#N/A,#N/A,TRUE,"月度店舗別小分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別小分類実績 ";#N/A,#N/A,TRUE,"日別店舗別中分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中分類実績 ";#N/A,#N/A,TRUE,"月度店舗別中分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別中分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中分類実績";#N/A,#N/A,TRUE,"日別店舗別中小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中小分類実績";#N/A,#N/A,TRUE,"月度店舗別中小分類実績";#N/A,#N/A,TRUE,"四半期店舗別中小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中小分類実績";#N/A,#N/A,TRUE,"日別店舗別大分類実績";#N/A,#N/A,TRUE,"週間店舗別大分類実績";#N/A,#N/A,TRUE,"月度店舗別大分類実績";#N/A,#N/A,TRUE,"四半期店舗別大分類別実績";#N/A,#N/A,TRUE,"年度店舗別大分類実績 ";#N/A,#N/A,TRUE,"日別店舗別商品群実績 ";#N/A,#N/A,TRUE,"週間店舗別商品群実績 ";#N/A,#N/A,TRUE,"月度店舗別商品群実績";#N/A,#N/A,TRUE,"四半期別商品群実績";#N/A,#N/A,TRUE,"年間店舗別商品群実績";#N/A,#N/A,TRUE,"日別型別実績";#N/A,#N/A,TRUE,"週間型別実績";#N/A,#N/A,TRUE,"月度型別実績";#N/A,#N/A,TRUE,"四半期型別実績";#N/A,#N/A,TRUE,"年間型別実績";#N/A,#N/A,TRUE,"日別小分類実績";#N/A,#N/A,TRUE,"週間小分類実績";#N/A,#N/A,TRUE,"月度小分類実績";#N/A,#N/A,TRUE,"四半期小分類実績";#N/A,#N/A,TRUE,"年度小分類実績";#N/A,#N/A,TRUE,"日別中分類実績";#N/A,#N/A,TRUE,"週間中分類実績";#N/A,#N/A,TRUE,"月度中分類実績";#N/A,#N/A,TRUE,"四半期中分類実績";#N/A,#N/A,TRUE,"年度中分類実績";#N/A,#N/A,TRUE,"日別中小分類実績"}</definedName>
     <definedName name="sadasda" hidden="1">{#N/A,#N/A,TRUE,"商品マスター";#N/A,#N/A,TRUE,"店舗マスター";#N/A,#N/A,TRUE,"在庫マスター";#N/A,#N/A,TRUE,"カレンダーマスター";#N/A,#N/A,TRUE,"分類コード変換マスター";#N/A,#N/A,TRUE,"重点型番マスター";#N/A,#N/A,TRUE,"商品分類コードマスター";#N/A,#N/A,TRUE,"商品分類別店舗型定義";#N/A,#N/A,TRUE,"日別店舗別型別実績 ";#N/A,#N/A,TRUE,"週間店舗別型別実績 ";#N/A,#N/A,TRUE,"月度店舗別型別実績";#N/A,#N/A,TRUE,"四半期店舗別型別実績 ";#N/A,#N/A,TRUE,"年間店舗別型別実績";#N/A,#N/A,TRUE,"日別店舗別小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別小分類実績 ";#N/A,#N/A,TRUE,"月度店舗別小分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別小分類実績 ";#N/A,#N/A,TRUE,"日別店舗別中分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中分類実績 ";#N/A,#N/A,TRUE,"月度店舗別中分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別中分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中分類実績";#N/A,#N/A,TRUE,"日別店舗別中小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中小分類実績";#N/A,#N/A,TRUE,"月度店舗別中小分類実績";#N/A,#N/A,TRUE,"四半期店舗別中小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中小分類実績";#N/A,#N/A,TRUE,"日別店舗別大分類実績";#N/A,#N/A,TRUE,"週間店舗別大分類実績";#N/A,#N/A,TRUE,"月度店舗別大分類実績";#N/A,#N/A,TRUE,"四半期店舗別大分類別実績";#N/A,#N/A,TRUE,"年度店舗別大分類実績 ";#N/A,#N/A,TRUE,"日別店舗別商品群実績 ";#N/A,#N/A,TRUE,"週間店舗別商品群実績 ";#N/A,#N/A,TRUE,"月度店舗別商品群実績";#N/A,#N/A,TRUE,"四半期別商品群実績";#N/A,#N/A,TRUE,"年間店舗別商品群実績";#N/A,#N/A,TRUE,"日別型別実績";#N/A,#N/A,TRUE,"週間型別実績";#N/A,#N/A,TRUE,"月度型別実績";#N/A,#N/A,TRUE,"四半期型別実績";#N/A,#N/A,TRUE,"年間型別実績";#N/A,#N/A,TRUE,"日別小分類実績";#N/A,#N/A,TRUE,"週間小分類実績";#N/A,#N/A,TRUE,"月度小分類実績";#N/A,#N/A,TRUE,"四半期小分類実績";#N/A,#N/A,TRUE,"年度小分類実績";#N/A,#N/A,TRUE,"日別中分類実績";#N/A,#N/A,TRUE,"週間中分類実績";#N/A,#N/A,TRUE,"月度中分類実績";#N/A,#N/A,TRUE,"四半期中分類実績";#N/A,#N/A,TRUE,"年度中分類実績";#N/A,#N/A,TRUE,"日別中小分類実績"}</definedName>
     <definedName name="sdddsdsd" hidden="1">{#N/A,#N/A,TRUE,"商品マスター";#N/A,#N/A,TRUE,"店舗マスター";#N/A,#N/A,TRUE,"在庫マスター";#N/A,#N/A,TRUE,"カレンダーマスター";#N/A,#N/A,TRUE,"分類コード変換マスター";#N/A,#N/A,TRUE,"重点型番マスター";#N/A,#N/A,TRUE,"商品分類コードマスター";#N/A,#N/A,TRUE,"商品分類別店舗型定義";#N/A,#N/A,TRUE,"日別店舗別型別実績 ";#N/A,#N/A,TRUE,"週間店舗別型別実績 ";#N/A,#N/A,TRUE,"月度店舗別型別実績";#N/A,#N/A,TRUE,"四半期店舗別型別実績 ";#N/A,#N/A,TRUE,"年間店舗別型別実績";#N/A,#N/A,TRUE,"日別店舗別小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別小分類実績 ";#N/A,#N/A,TRUE,"月度店舗別小分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別小分類実績 ";#N/A,#N/A,TRUE,"日別店舗別中分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中分類実績 ";#N/A,#N/A,TRUE,"月度店舗別中分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別中分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中分類実績";#N/A,#N/A,TRUE,"日別店舗別中小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中小分類実績";#N/A,#N/A,TRUE,"月度店舗別中小分類実績";#N/A,#N/A,TRUE,"四半期店舗別中小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中小分類実績";#N/A,#N/A,TRUE,"日別店舗別大分類実績";#N/A,#N/A,TRUE,"週間店舗別大分類実績";#N/A,#N/A,TRUE,"月度店舗別大分類実績";#N/A,#N/A,TRUE,"四半期店舗別大分類別実績";#N/A,#N/A,TRUE,"年度店舗別大分類実績 ";#N/A,#N/A,TRUE,"日別店舗別商品群実績 ";#N/A,#N/A,TRUE,"週間店舗別商品群実績 ";#N/A,#N/A,TRUE,"月度店舗別商品群実績";#N/A,#N/A,TRUE,"四半期別商品群実績";#N/A,#N/A,TRUE,"年間店舗別商品群実績";#N/A,#N/A,TRUE,"日別型別実績";#N/A,#N/A,TRUE,"週間型別実績";#N/A,#N/A,TRUE,"月度型別実績";#N/A,#N/A,TRUE,"四半期型別実績";#N/A,#N/A,TRUE,"年間型別実績";#N/A,#N/A,TRUE,"日別小分類実績";#N/A,#N/A,TRUE,"週間小分類実績";#N/A,#N/A,TRUE,"月度小分類実績";#N/A,#N/A,TRUE,"四半期小分類実績";#N/A,#N/A,TRUE,"年度小分類実績";#N/A,#N/A,TRUE,"日別中分類実績";#N/A,#N/A,TRUE,"週間中分類実績";#N/A,#N/A,TRUE,"月度中分類実績";#N/A,#N/A,TRUE,"四半期中分類実績";#N/A,#N/A,TRUE,"年度中分類実績";#N/A,#N/A,TRUE,"日別中小分類実績"}</definedName>
     <definedName name="sss" hidden="1">{#N/A,#N/A,FALSE,"Chi tiÆt"}</definedName>
-    <definedName name="UClist" localSheetId="4">#REF!</definedName>
+    <definedName name="UClist" localSheetId="5">#REF!</definedName>
     <definedName name="UClist">#REF!</definedName>
     <definedName name="ưew" hidden="1">{#N/A,#N/A,TRUE,"商品マスター";#N/A,#N/A,TRUE,"店舗マスター";#N/A,#N/A,TRUE,"在庫マスター";#N/A,#N/A,TRUE,"カレンダーマスター";#N/A,#N/A,TRUE,"分類コード変換マスター";#N/A,#N/A,TRUE,"重点型番マスター";#N/A,#N/A,TRUE,"商品分類コードマスター";#N/A,#N/A,TRUE,"商品分類別店舗型定義";#N/A,#N/A,TRUE,"日別店舗別型別実績 ";#N/A,#N/A,TRUE,"週間店舗別型別実績 ";#N/A,#N/A,TRUE,"月度店舗別型別実績";#N/A,#N/A,TRUE,"四半期店舗別型別実績 ";#N/A,#N/A,TRUE,"年間店舗別型別実績";#N/A,#N/A,TRUE,"日別店舗別小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別小分類実績 ";#N/A,#N/A,TRUE,"月度店舗別小分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別小分類実績 ";#N/A,#N/A,TRUE,"日別店舗別中分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中分類実績 ";#N/A,#N/A,TRUE,"月度店舗別中分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別中分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中分類実績";#N/A,#N/A,TRUE,"日別店舗別中小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中小分類実績";#N/A,#N/A,TRUE,"月度店舗別中小分類実績";#N/A,#N/A,TRUE,"四半期店舗別中小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中小分類実績";#N/A,#N/A,TRUE,"日別店舗別大分類実績";#N/A,#N/A,TRUE,"週間店舗別大分類実績";#N/A,#N/A,TRUE,"月度店舗別大分類実績";#N/A,#N/A,TRUE,"四半期店舗別大分類別実績";#N/A,#N/A,TRUE,"年度店舗別大分類実績 ";#N/A,#N/A,TRUE,"日別店舗別商品群実績 ";#N/A,#N/A,TRUE,"週間店舗別商品群実績 ";#N/A,#N/A,TRUE,"月度店舗別商品群実績";#N/A,#N/A,TRUE,"四半期別商品群実績";#N/A,#N/A,TRUE,"年間店舗別商品群実績";#N/A,#N/A,TRUE,"日別型別実績";#N/A,#N/A,TRUE,"週間型別実績";#N/A,#N/A,TRUE,"月度型別実績";#N/A,#N/A,TRUE,"四半期型別実績";#N/A,#N/A,TRUE,"年間型別実績";#N/A,#N/A,TRUE,"日別小分類実績";#N/A,#N/A,TRUE,"週間小分類実績";#N/A,#N/A,TRUE,"月度小分類実績";#N/A,#N/A,TRUE,"四半期小分類実績";#N/A,#N/A,TRUE,"年度小分類実績";#N/A,#N/A,TRUE,"日別中分類実績";#N/A,#N/A,TRUE,"週間中分類実績";#N/A,#N/A,TRUE,"月度中分類実績";#N/A,#N/A,TRUE,"四半期中分類実績";#N/A,#N/A,TRUE,"年度中分類実績";#N/A,#N/A,TRUE,"日別中小分類実績"}</definedName>
     <definedName name="w" hidden="1">{#N/A,#N/A,TRUE,"商品マスター";#N/A,#N/A,TRUE,"店舗マスター";#N/A,#N/A,TRUE,"在庫マスター";#N/A,#N/A,TRUE,"カレンダーマスター";#N/A,#N/A,TRUE,"分類コード変換マスター";#N/A,#N/A,TRUE,"重点型番マスター";#N/A,#N/A,TRUE,"商品分類コードマスター";#N/A,#N/A,TRUE,"商品分類別店舗型定義";#N/A,#N/A,TRUE,"日別店舗別型別実績 ";#N/A,#N/A,TRUE,"週間店舗別型別実績 ";#N/A,#N/A,TRUE,"月度店舗別型別実績";#N/A,#N/A,TRUE,"四半期店舗別型別実績 ";#N/A,#N/A,TRUE,"年間店舗別型別実績";#N/A,#N/A,TRUE,"日別店舗別小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別小分類実績 ";#N/A,#N/A,TRUE,"月度店舗別小分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別小分類実績 ";#N/A,#N/A,TRUE,"日別店舗別中分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中分類実績 ";#N/A,#N/A,TRUE,"月度店舗別中分類実績 ";#N/A,#N/A,TRUE,"四半期店舗別中分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中分類実績";#N/A,#N/A,TRUE,"日別店舗別中小分類実績 ";#N/A,#N/A,TRUE,"週間店舗別中小分類実績";#N/A,#N/A,TRUE,"月度店舗別中小分類実績";#N/A,#N/A,TRUE,"四半期店舗別中小分類実績 ";#N/A,#N/A,TRUE,"年度店舗別中小分類実績";#N/A,#N/A,TRUE,"日別店舗別大分類実績";#N/A,#N/A,TRUE,"週間店舗別大分類実績";#N/A,#N/A,TRUE,"月度店舗別大分類実績";#N/A,#N/A,TRUE,"四半期店舗別大分類別実績";#N/A,#N/A,TRUE,"年度店舗別大分類実績 ";#N/A,#N/A,TRUE,"日別店舗別商品群実績 ";#N/A,#N/A,TRUE,"週間店舗別商品群実績 ";#N/A,#N/A,TRUE,"月度店舗別商品群実績";#N/A,#N/A,TRUE,"四半期別商品群実績";#N/A,#N/A,TRUE,"年間店舗別商品群実績";#N/A,#N/A,TRUE,"日別型別実績";#N/A,#N/A,TRUE,"週間型別実績";#N/A,#N/A,TRUE,"月度型別実績";#N/A,#N/A,TRUE,"四半期型別実績";#N/A,#N/A,TRUE,"年間型別実績";#N/A,#N/A,TRUE,"日別小分類実績";#N/A,#N/A,TRUE,"週間小分類実績";#N/A,#N/A,TRUE,"月度小分類実績";#N/A,#N/A,TRUE,"四半期小分類実績";#N/A,#N/A,TRUE,"年度小分類実績";#N/A,#N/A,TRUE,"日別中分類実績";#N/A,#N/A,TRUE,"週間中分類実績";#N/A,#N/A,TRUE,"月度中分類実績";#N/A,#N/A,TRUE,"四半期中分類実績";#N/A,#N/A,TRUE,"年度中分類実績";#N/A,#N/A,TRUE,"日別中小分類実績"}</definedName>
@@ -303,7 +304,7 @@
         <b/>
         <sz val="10"/>
         <rFont val="Tahoma"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>Security matrix</t>
     </r>
@@ -477,32 +478,32 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -510,7 +511,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -518,12 +519,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Wingdings 3"/>
+      <family val="1"/>
       <charset val="2"/>
     </font>
     <font>
@@ -533,133 +535,134 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Webdings"/>
+      <family val="1"/>
       <charset val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Tahoma"/>
-      <charset val="128"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="0"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="10"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="10"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
       <color indexed="56"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color indexed="52"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color indexed="9"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="17"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="9"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="20"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color indexed="56"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -671,39 +674,39 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="62"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color indexed="23"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color indexed="63"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="13"/>
       <color indexed="56"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="13"/>
@@ -714,7 +717,7 @@
       <sz val="11"/>
       <color indexed="60"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -725,14 +728,14 @@
       <sz val="11"/>
       <color indexed="52"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color indexed="56"/>
       <name val="Cambria"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="14"/>
@@ -802,7 +805,7 @@
       <b/>
       <sz val="12"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -823,7 +826,7 @@
       <b/>
       <sz val="9"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -838,7 +841,7 @@
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -850,7 +853,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="128"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -5369,6 +5372,76 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="1882" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="3633" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="64" fillId="2" borderId="0" xfId="3633" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="6" borderId="1" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="6" borderId="2" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="6" borderId="3" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="6" borderId="9" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="3" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="9" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="3" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="9" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -5414,18 +5487,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5456,76 +5517,19 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="3" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="9" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="3" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="9" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="6" borderId="1" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="6" borderId="2" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="6" borderId="3" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="6" borderId="9" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="174" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5540,7 +5544,6 @@
     <xf numFmtId="174" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="64" fillId="2" borderId="0" xfId="3633" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3719">
     <cellStyle name="??" xfId="392"/>
@@ -10407,7 +10410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="AC74" sqref="AC74"/>
     </sheetView>
   </sheetViews>
@@ -10425,156 +10428,156 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="163" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="165" t="s">
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="166"/>
-      <c r="L1" s="166"/>
-      <c r="M1" s="166"/>
-      <c r="N1" s="166"/>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="166"/>
-      <c r="R1" s="166"/>
-      <c r="S1" s="166"/>
-      <c r="T1" s="166"/>
-      <c r="U1" s="166"/>
-      <c r="V1" s="166"/>
-      <c r="W1" s="166"/>
-      <c r="X1" s="166"/>
-      <c r="Y1" s="166"/>
-      <c r="Z1" s="166"/>
-      <c r="AA1" s="166"/>
-      <c r="AB1" s="166"/>
-      <c r="AC1" s="166"/>
-      <c r="AD1" s="167"/>
-      <c r="AE1" s="165" t="s">
+      <c r="H1" s="126"/>
+      <c r="I1" s="126"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="126"/>
+      <c r="L1" s="126"/>
+      <c r="M1" s="126"/>
+      <c r="N1" s="126"/>
+      <c r="O1" s="126"/>
+      <c r="P1" s="126"/>
+      <c r="Q1" s="126"/>
+      <c r="R1" s="126"/>
+      <c r="S1" s="126"/>
+      <c r="T1" s="126"/>
+      <c r="U1" s="126"/>
+      <c r="V1" s="126"/>
+      <c r="W1" s="126"/>
+      <c r="X1" s="126"/>
+      <c r="Y1" s="126"/>
+      <c r="Z1" s="126"/>
+      <c r="AA1" s="126"/>
+      <c r="AB1" s="126"/>
+      <c r="AC1" s="126"/>
+      <c r="AD1" s="127"/>
+      <c r="AE1" s="125" t="s">
         <v>13</v>
       </c>
-      <c r="AF1" s="166"/>
-      <c r="AG1" s="166"/>
-      <c r="AH1" s="167"/>
-      <c r="AI1" s="166" t="s">
+      <c r="AF1" s="126"/>
+      <c r="AG1" s="126"/>
+      <c r="AH1" s="127"/>
+      <c r="AI1" s="126" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="166"/>
-      <c r="AK1" s="166"/>
-      <c r="AL1" s="167"/>
-      <c r="AM1" s="165" t="s">
+      <c r="AJ1" s="126"/>
+      <c r="AK1" s="126"/>
+      <c r="AL1" s="127"/>
+      <c r="AM1" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="AN1" s="166"/>
-      <c r="AO1" s="166"/>
-      <c r="AP1" s="167"/>
+      <c r="AN1" s="126"/>
+      <c r="AO1" s="126"/>
+      <c r="AP1" s="127"/>
     </row>
     <row r="2" spans="1:42" ht="15" customHeight="1">
-      <c r="A2" s="143"/>
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="143"/>
-      <c r="G2" s="144" t="s">
+      <c r="A2" s="163"/>
+      <c r="B2" s="163"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="163"/>
+      <c r="F2" s="163"/>
+      <c r="G2" s="164" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="145"/>
-      <c r="I2" s="145"/>
-      <c r="J2" s="145"/>
-      <c r="K2" s="145"/>
-      <c r="L2" s="145"/>
-      <c r="M2" s="145"/>
-      <c r="N2" s="145"/>
-      <c r="O2" s="145"/>
-      <c r="P2" s="145"/>
-      <c r="Q2" s="145"/>
-      <c r="R2" s="145"/>
-      <c r="S2" s="145"/>
-      <c r="T2" s="145"/>
-      <c r="U2" s="145"/>
-      <c r="V2" s="145"/>
-      <c r="W2" s="145"/>
-      <c r="X2" s="145"/>
-      <c r="Y2" s="145"/>
-      <c r="Z2" s="145"/>
-      <c r="AA2" s="145"/>
-      <c r="AB2" s="145"/>
-      <c r="AC2" s="145"/>
-      <c r="AD2" s="146"/>
-      <c r="AE2" s="133" t="s">
+      <c r="H2" s="165"/>
+      <c r="I2" s="165"/>
+      <c r="J2" s="165"/>
+      <c r="K2" s="165"/>
+      <c r="L2" s="165"/>
+      <c r="M2" s="165"/>
+      <c r="N2" s="165"/>
+      <c r="O2" s="165"/>
+      <c r="P2" s="165"/>
+      <c r="Q2" s="165"/>
+      <c r="R2" s="165"/>
+      <c r="S2" s="165"/>
+      <c r="T2" s="165"/>
+      <c r="U2" s="165"/>
+      <c r="V2" s="165"/>
+      <c r="W2" s="165"/>
+      <c r="X2" s="165"/>
+      <c r="Y2" s="165"/>
+      <c r="Z2" s="165"/>
+      <c r="AA2" s="165"/>
+      <c r="AB2" s="165"/>
+      <c r="AC2" s="165"/>
+      <c r="AD2" s="166"/>
+      <c r="AE2" s="157" t="s">
         <v>7</v>
       </c>
-      <c r="AF2" s="134"/>
-      <c r="AG2" s="134"/>
-      <c r="AH2" s="135"/>
-      <c r="AI2" s="139">
+      <c r="AF2" s="158"/>
+      <c r="AG2" s="158"/>
+      <c r="AH2" s="159"/>
+      <c r="AI2" s="132">
         <f>DATE(2017,1,30)</f>
         <v>42765</v>
       </c>
-      <c r="AJ2" s="139"/>
-      <c r="AK2" s="139"/>
-      <c r="AL2" s="140"/>
-      <c r="AM2" s="139">
+      <c r="AJ2" s="132"/>
+      <c r="AK2" s="132"/>
+      <c r="AL2" s="133"/>
+      <c r="AM2" s="132">
         <f>DATE(2017,2,2)</f>
         <v>42768</v>
       </c>
-      <c r="AN2" s="139"/>
-      <c r="AO2" s="139"/>
-      <c r="AP2" s="140"/>
+      <c r="AN2" s="132"/>
+      <c r="AO2" s="132"/>
+      <c r="AP2" s="133"/>
     </row>
     <row r="3" spans="1:42">
-      <c r="A3" s="143"/>
-      <c r="B3" s="143"/>
-      <c r="C3" s="143"/>
-      <c r="D3" s="143"/>
-      <c r="E3" s="143"/>
-      <c r="F3" s="143"/>
-      <c r="G3" s="147"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
-      <c r="K3" s="148"/>
-      <c r="L3" s="148"/>
-      <c r="M3" s="148"/>
-      <c r="N3" s="148"/>
-      <c r="O3" s="148"/>
-      <c r="P3" s="148"/>
-      <c r="Q3" s="148"/>
-      <c r="R3" s="148"/>
-      <c r="S3" s="148"/>
-      <c r="T3" s="148"/>
-      <c r="U3" s="148"/>
-      <c r="V3" s="148"/>
-      <c r="W3" s="148"/>
-      <c r="X3" s="148"/>
-      <c r="Y3" s="148"/>
-      <c r="Z3" s="148"/>
-      <c r="AA3" s="148"/>
-      <c r="AB3" s="148"/>
-      <c r="AC3" s="148"/>
-      <c r="AD3" s="149"/>
-      <c r="AE3" s="136"/>
-      <c r="AF3" s="137"/>
-      <c r="AG3" s="137"/>
-      <c r="AH3" s="138"/>
-      <c r="AI3" s="141"/>
-      <c r="AJ3" s="141"/>
-      <c r="AK3" s="141"/>
-      <c r="AL3" s="142"/>
-      <c r="AM3" s="141"/>
-      <c r="AN3" s="141"/>
-      <c r="AO3" s="141"/>
-      <c r="AP3" s="142"/>
+      <c r="A3" s="163"/>
+      <c r="B3" s="163"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="163"/>
+      <c r="G3" s="167"/>
+      <c r="H3" s="168"/>
+      <c r="I3" s="168"/>
+      <c r="J3" s="168"/>
+      <c r="K3" s="168"/>
+      <c r="L3" s="168"/>
+      <c r="M3" s="168"/>
+      <c r="N3" s="168"/>
+      <c r="O3" s="168"/>
+      <c r="P3" s="168"/>
+      <c r="Q3" s="168"/>
+      <c r="R3" s="168"/>
+      <c r="S3" s="168"/>
+      <c r="T3" s="168"/>
+      <c r="U3" s="168"/>
+      <c r="V3" s="168"/>
+      <c r="W3" s="168"/>
+      <c r="X3" s="168"/>
+      <c r="Y3" s="168"/>
+      <c r="Z3" s="168"/>
+      <c r="AA3" s="168"/>
+      <c r="AB3" s="168"/>
+      <c r="AC3" s="168"/>
+      <c r="AD3" s="169"/>
+      <c r="AE3" s="160"/>
+      <c r="AF3" s="161"/>
+      <c r="AG3" s="161"/>
+      <c r="AH3" s="162"/>
+      <c r="AI3" s="134"/>
+      <c r="AJ3" s="134"/>
+      <c r="AK3" s="134"/>
+      <c r="AL3" s="135"/>
+      <c r="AM3" s="134"/>
+      <c r="AN3" s="134"/>
+      <c r="AO3" s="134"/>
+      <c r="AP3" s="135"/>
     </row>
     <row r="4" spans="1:42">
       <c r="A4" s="54"/>
@@ -10712,181 +10715,181 @@
     </row>
     <row r="7" spans="1:42" ht="12.75" customHeight="1">
       <c r="A7" s="54"/>
-      <c r="B7" s="150" t="s">
+      <c r="B7" s="170" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="151"/>
-      <c r="D7" s="151"/>
-      <c r="E7" s="151"/>
-      <c r="F7" s="151"/>
-      <c r="G7" s="151"/>
-      <c r="H7" s="151"/>
-      <c r="I7" s="151"/>
-      <c r="J7" s="151"/>
-      <c r="K7" s="151"/>
-      <c r="L7" s="151"/>
-      <c r="M7" s="151"/>
-      <c r="N7" s="151"/>
-      <c r="O7" s="151"/>
-      <c r="P7" s="151"/>
-      <c r="Q7" s="151"/>
-      <c r="R7" s="151"/>
-      <c r="S7" s="151"/>
-      <c r="T7" s="151"/>
-      <c r="U7" s="151"/>
-      <c r="V7" s="151"/>
-      <c r="W7" s="151"/>
-      <c r="X7" s="151"/>
-      <c r="Y7" s="151"/>
-      <c r="Z7" s="151"/>
-      <c r="AA7" s="151"/>
-      <c r="AB7" s="151"/>
-      <c r="AC7" s="151"/>
-      <c r="AD7" s="151"/>
-      <c r="AE7" s="151"/>
-      <c r="AF7" s="151"/>
-      <c r="AG7" s="151"/>
-      <c r="AH7" s="151"/>
-      <c r="AI7" s="151"/>
-      <c r="AJ7" s="151"/>
-      <c r="AK7" s="151"/>
-      <c r="AL7" s="151"/>
-      <c r="AM7" s="151"/>
-      <c r="AN7" s="151"/>
-      <c r="AO7" s="151"/>
-      <c r="AP7" s="152"/>
+      <c r="C7" s="171"/>
+      <c r="D7" s="171"/>
+      <c r="E7" s="171"/>
+      <c r="F7" s="171"/>
+      <c r="G7" s="171"/>
+      <c r="H7" s="171"/>
+      <c r="I7" s="171"/>
+      <c r="J7" s="171"/>
+      <c r="K7" s="171"/>
+      <c r="L7" s="171"/>
+      <c r="M7" s="171"/>
+      <c r="N7" s="171"/>
+      <c r="O7" s="171"/>
+      <c r="P7" s="171"/>
+      <c r="Q7" s="171"/>
+      <c r="R7" s="171"/>
+      <c r="S7" s="171"/>
+      <c r="T7" s="171"/>
+      <c r="U7" s="171"/>
+      <c r="V7" s="171"/>
+      <c r="W7" s="171"/>
+      <c r="X7" s="171"/>
+      <c r="Y7" s="171"/>
+      <c r="Z7" s="171"/>
+      <c r="AA7" s="171"/>
+      <c r="AB7" s="171"/>
+      <c r="AC7" s="171"/>
+      <c r="AD7" s="171"/>
+      <c r="AE7" s="171"/>
+      <c r="AF7" s="171"/>
+      <c r="AG7" s="171"/>
+      <c r="AH7" s="171"/>
+      <c r="AI7" s="171"/>
+      <c r="AJ7" s="171"/>
+      <c r="AK7" s="171"/>
+      <c r="AL7" s="171"/>
+      <c r="AM7" s="171"/>
+      <c r="AN7" s="171"/>
+      <c r="AO7" s="171"/>
+      <c r="AP7" s="172"/>
     </row>
     <row r="8" spans="1:42" ht="12.75" customHeight="1">
       <c r="A8" s="54"/>
-      <c r="B8" s="151"/>
-      <c r="C8" s="151"/>
-      <c r="D8" s="151"/>
-      <c r="E8" s="151"/>
-      <c r="F8" s="151"/>
-      <c r="G8" s="151"/>
-      <c r="H8" s="151"/>
-      <c r="I8" s="151"/>
-      <c r="J8" s="151"/>
-      <c r="K8" s="151"/>
-      <c r="L8" s="151"/>
-      <c r="M8" s="151"/>
-      <c r="N8" s="151"/>
-      <c r="O8" s="151"/>
-      <c r="P8" s="151"/>
-      <c r="Q8" s="151"/>
-      <c r="R8" s="151"/>
-      <c r="S8" s="151"/>
-      <c r="T8" s="151"/>
-      <c r="U8" s="151"/>
-      <c r="V8" s="151"/>
-      <c r="W8" s="151"/>
-      <c r="X8" s="151"/>
-      <c r="Y8" s="151"/>
-      <c r="Z8" s="151"/>
-      <c r="AA8" s="151"/>
-      <c r="AB8" s="151"/>
-      <c r="AC8" s="151"/>
-      <c r="AD8" s="151"/>
-      <c r="AE8" s="151"/>
-      <c r="AF8" s="151"/>
-      <c r="AG8" s="151"/>
-      <c r="AH8" s="151"/>
-      <c r="AI8" s="151"/>
-      <c r="AJ8" s="151"/>
-      <c r="AK8" s="151"/>
-      <c r="AL8" s="151"/>
-      <c r="AM8" s="151"/>
-      <c r="AN8" s="151"/>
-      <c r="AO8" s="151"/>
-      <c r="AP8" s="152"/>
+      <c r="B8" s="171"/>
+      <c r="C8" s="171"/>
+      <c r="D8" s="171"/>
+      <c r="E8" s="171"/>
+      <c r="F8" s="171"/>
+      <c r="G8" s="171"/>
+      <c r="H8" s="171"/>
+      <c r="I8" s="171"/>
+      <c r="J8" s="171"/>
+      <c r="K8" s="171"/>
+      <c r="L8" s="171"/>
+      <c r="M8" s="171"/>
+      <c r="N8" s="171"/>
+      <c r="O8" s="171"/>
+      <c r="P8" s="171"/>
+      <c r="Q8" s="171"/>
+      <c r="R8" s="171"/>
+      <c r="S8" s="171"/>
+      <c r="T8" s="171"/>
+      <c r="U8" s="171"/>
+      <c r="V8" s="171"/>
+      <c r="W8" s="171"/>
+      <c r="X8" s="171"/>
+      <c r="Y8" s="171"/>
+      <c r="Z8" s="171"/>
+      <c r="AA8" s="171"/>
+      <c r="AB8" s="171"/>
+      <c r="AC8" s="171"/>
+      <c r="AD8" s="171"/>
+      <c r="AE8" s="171"/>
+      <c r="AF8" s="171"/>
+      <c r="AG8" s="171"/>
+      <c r="AH8" s="171"/>
+      <c r="AI8" s="171"/>
+      <c r="AJ8" s="171"/>
+      <c r="AK8" s="171"/>
+      <c r="AL8" s="171"/>
+      <c r="AM8" s="171"/>
+      <c r="AN8" s="171"/>
+      <c r="AO8" s="171"/>
+      <c r="AP8" s="172"/>
     </row>
     <row r="9" spans="1:42" ht="12.75" customHeight="1">
       <c r="A9" s="54"/>
-      <c r="B9" s="151"/>
-      <c r="C9" s="151"/>
-      <c r="D9" s="151"/>
-      <c r="E9" s="151"/>
-      <c r="F9" s="151"/>
-      <c r="G9" s="151"/>
-      <c r="H9" s="151"/>
-      <c r="I9" s="151"/>
-      <c r="J9" s="151"/>
-      <c r="K9" s="151"/>
-      <c r="L9" s="151"/>
-      <c r="M9" s="151"/>
-      <c r="N9" s="151"/>
-      <c r="O9" s="151"/>
-      <c r="P9" s="151"/>
-      <c r="Q9" s="151"/>
-      <c r="R9" s="151"/>
-      <c r="S9" s="151"/>
-      <c r="T9" s="151"/>
-      <c r="U9" s="151"/>
-      <c r="V9" s="151"/>
-      <c r="W9" s="151"/>
-      <c r="X9" s="151"/>
-      <c r="Y9" s="151"/>
-      <c r="Z9" s="151"/>
-      <c r="AA9" s="151"/>
-      <c r="AB9" s="151"/>
-      <c r="AC9" s="151"/>
-      <c r="AD9" s="151"/>
-      <c r="AE9" s="151"/>
-      <c r="AF9" s="151"/>
-      <c r="AG9" s="151"/>
-      <c r="AH9" s="151"/>
-      <c r="AI9" s="151"/>
-      <c r="AJ9" s="151"/>
-      <c r="AK9" s="151"/>
-      <c r="AL9" s="151"/>
-      <c r="AM9" s="151"/>
-      <c r="AN9" s="151"/>
-      <c r="AO9" s="151"/>
-      <c r="AP9" s="152"/>
+      <c r="B9" s="171"/>
+      <c r="C9" s="171"/>
+      <c r="D9" s="171"/>
+      <c r="E9" s="171"/>
+      <c r="F9" s="171"/>
+      <c r="G9" s="171"/>
+      <c r="H9" s="171"/>
+      <c r="I9" s="171"/>
+      <c r="J9" s="171"/>
+      <c r="K9" s="171"/>
+      <c r="L9" s="171"/>
+      <c r="M9" s="171"/>
+      <c r="N9" s="171"/>
+      <c r="O9" s="171"/>
+      <c r="P9" s="171"/>
+      <c r="Q9" s="171"/>
+      <c r="R9" s="171"/>
+      <c r="S9" s="171"/>
+      <c r="T9" s="171"/>
+      <c r="U9" s="171"/>
+      <c r="V9" s="171"/>
+      <c r="W9" s="171"/>
+      <c r="X9" s="171"/>
+      <c r="Y9" s="171"/>
+      <c r="Z9" s="171"/>
+      <c r="AA9" s="171"/>
+      <c r="AB9" s="171"/>
+      <c r="AC9" s="171"/>
+      <c r="AD9" s="171"/>
+      <c r="AE9" s="171"/>
+      <c r="AF9" s="171"/>
+      <c r="AG9" s="171"/>
+      <c r="AH9" s="171"/>
+      <c r="AI9" s="171"/>
+      <c r="AJ9" s="171"/>
+      <c r="AK9" s="171"/>
+      <c r="AL9" s="171"/>
+      <c r="AM9" s="171"/>
+      <c r="AN9" s="171"/>
+      <c r="AO9" s="171"/>
+      <c r="AP9" s="172"/>
     </row>
     <row r="10" spans="1:42" ht="12.75" customHeight="1">
       <c r="A10" s="54"/>
-      <c r="B10" s="151"/>
-      <c r="C10" s="151"/>
-      <c r="D10" s="151"/>
-      <c r="E10" s="151"/>
-      <c r="F10" s="151"/>
-      <c r="G10" s="151"/>
-      <c r="H10" s="151"/>
-      <c r="I10" s="151"/>
-      <c r="J10" s="151"/>
-      <c r="K10" s="151"/>
-      <c r="L10" s="151"/>
-      <c r="M10" s="151"/>
-      <c r="N10" s="151"/>
-      <c r="O10" s="151"/>
-      <c r="P10" s="151"/>
-      <c r="Q10" s="151"/>
-      <c r="R10" s="151"/>
-      <c r="S10" s="151"/>
-      <c r="T10" s="151"/>
-      <c r="U10" s="151"/>
-      <c r="V10" s="151"/>
-      <c r="W10" s="151"/>
-      <c r="X10" s="151"/>
-      <c r="Y10" s="151"/>
-      <c r="Z10" s="151"/>
-      <c r="AA10" s="151"/>
-      <c r="AB10" s="151"/>
-      <c r="AC10" s="151"/>
-      <c r="AD10" s="151"/>
-      <c r="AE10" s="151"/>
-      <c r="AF10" s="151"/>
-      <c r="AG10" s="151"/>
-      <c r="AH10" s="151"/>
-      <c r="AI10" s="151"/>
-      <c r="AJ10" s="151"/>
-      <c r="AK10" s="151"/>
-      <c r="AL10" s="151"/>
-      <c r="AM10" s="151"/>
-      <c r="AN10" s="151"/>
-      <c r="AO10" s="151"/>
-      <c r="AP10" s="152"/>
+      <c r="B10" s="171"/>
+      <c r="C10" s="171"/>
+      <c r="D10" s="171"/>
+      <c r="E10" s="171"/>
+      <c r="F10" s="171"/>
+      <c r="G10" s="171"/>
+      <c r="H10" s="171"/>
+      <c r="I10" s="171"/>
+      <c r="J10" s="171"/>
+      <c r="K10" s="171"/>
+      <c r="L10" s="171"/>
+      <c r="M10" s="171"/>
+      <c r="N10" s="171"/>
+      <c r="O10" s="171"/>
+      <c r="P10" s="171"/>
+      <c r="Q10" s="171"/>
+      <c r="R10" s="171"/>
+      <c r="S10" s="171"/>
+      <c r="T10" s="171"/>
+      <c r="U10" s="171"/>
+      <c r="V10" s="171"/>
+      <c r="W10" s="171"/>
+      <c r="X10" s="171"/>
+      <c r="Y10" s="171"/>
+      <c r="Z10" s="171"/>
+      <c r="AA10" s="171"/>
+      <c r="AB10" s="171"/>
+      <c r="AC10" s="171"/>
+      <c r="AD10" s="171"/>
+      <c r="AE10" s="171"/>
+      <c r="AF10" s="171"/>
+      <c r="AG10" s="171"/>
+      <c r="AH10" s="171"/>
+      <c r="AI10" s="171"/>
+      <c r="AJ10" s="171"/>
+      <c r="AK10" s="171"/>
+      <c r="AL10" s="171"/>
+      <c r="AM10" s="171"/>
+      <c r="AN10" s="171"/>
+      <c r="AO10" s="171"/>
+      <c r="AP10" s="172"/>
     </row>
     <row r="11" spans="1:42">
       <c r="A11" s="54"/>
@@ -12708,46 +12711,46 @@
       <c r="C52" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="D52" s="168" t="s">
+      <c r="D52" s="128" t="s">
         <v>24</v>
       </c>
-      <c r="E52" s="168"/>
-      <c r="F52" s="168"/>
-      <c r="G52" s="168"/>
-      <c r="H52" s="168" t="s">
+      <c r="E52" s="128"/>
+      <c r="F52" s="128"/>
+      <c r="G52" s="128"/>
+      <c r="H52" s="128" t="s">
         <v>25</v>
       </c>
-      <c r="I52" s="168"/>
-      <c r="J52" s="168"/>
-      <c r="K52" s="168"/>
-      <c r="L52" s="168"/>
-      <c r="M52" s="168"/>
-      <c r="N52" s="168"/>
-      <c r="O52" s="168"/>
-      <c r="P52" s="168"/>
-      <c r="Q52" s="168"/>
-      <c r="R52" s="168"/>
-      <c r="S52" s="168"/>
-      <c r="T52" s="168"/>
-      <c r="U52" s="168"/>
-      <c r="V52" s="168"/>
-      <c r="W52" s="169" t="s">
+      <c r="I52" s="128"/>
+      <c r="J52" s="128"/>
+      <c r="K52" s="128"/>
+      <c r="L52" s="128"/>
+      <c r="M52" s="128"/>
+      <c r="N52" s="128"/>
+      <c r="O52" s="128"/>
+      <c r="P52" s="128"/>
+      <c r="Q52" s="128"/>
+      <c r="R52" s="128"/>
+      <c r="S52" s="128"/>
+      <c r="T52" s="128"/>
+      <c r="U52" s="128"/>
+      <c r="V52" s="128"/>
+      <c r="W52" s="129" t="s">
         <v>26</v>
       </c>
-      <c r="X52" s="170"/>
-      <c r="Y52" s="170"/>
-      <c r="Z52" s="170"/>
-      <c r="AA52" s="170"/>
-      <c r="AB52" s="170"/>
-      <c r="AC52" s="170"/>
-      <c r="AD52" s="170"/>
-      <c r="AE52" s="170"/>
-      <c r="AF52" s="170"/>
-      <c r="AG52" s="170"/>
-      <c r="AH52" s="170"/>
-      <c r="AI52" s="170"/>
-      <c r="AJ52" s="170"/>
-      <c r="AK52" s="171"/>
+      <c r="X52" s="130"/>
+      <c r="Y52" s="130"/>
+      <c r="Z52" s="130"/>
+      <c r="AA52" s="130"/>
+      <c r="AB52" s="130"/>
+      <c r="AC52" s="130"/>
+      <c r="AD52" s="130"/>
+      <c r="AE52" s="130"/>
+      <c r="AF52" s="130"/>
+      <c r="AG52" s="130"/>
+      <c r="AH52" s="130"/>
+      <c r="AI52" s="130"/>
+      <c r="AJ52" s="130"/>
+      <c r="AK52" s="131"/>
       <c r="AL52" s="5"/>
       <c r="AM52" s="5"/>
       <c r="AN52" s="5"/>
@@ -12760,46 +12763,46 @@
       <c r="C53" s="80">
         <v>1</v>
       </c>
-      <c r="D53" s="157" t="s">
+      <c r="D53" s="136" t="s">
         <v>27</v>
       </c>
-      <c r="E53" s="157"/>
-      <c r="F53" s="157"/>
-      <c r="G53" s="157"/>
-      <c r="H53" s="162" t="s">
+      <c r="E53" s="136"/>
+      <c r="F53" s="136"/>
+      <c r="G53" s="136"/>
+      <c r="H53" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="I53" s="163"/>
-      <c r="J53" s="163"/>
-      <c r="K53" s="163"/>
-      <c r="L53" s="163"/>
-      <c r="M53" s="163"/>
-      <c r="N53" s="163"/>
-      <c r="O53" s="163"/>
-      <c r="P53" s="163"/>
-      <c r="Q53" s="163"/>
-      <c r="R53" s="163"/>
-      <c r="S53" s="163"/>
-      <c r="T53" s="163"/>
-      <c r="U53" s="163"/>
-      <c r="V53" s="164"/>
-      <c r="W53" s="158" t="s">
+      <c r="I53" s="138"/>
+      <c r="J53" s="138"/>
+      <c r="K53" s="138"/>
+      <c r="L53" s="138"/>
+      <c r="M53" s="138"/>
+      <c r="N53" s="138"/>
+      <c r="O53" s="138"/>
+      <c r="P53" s="138"/>
+      <c r="Q53" s="138"/>
+      <c r="R53" s="138"/>
+      <c r="S53" s="138"/>
+      <c r="T53" s="138"/>
+      <c r="U53" s="138"/>
+      <c r="V53" s="139"/>
+      <c r="W53" s="140" t="s">
         <v>29</v>
       </c>
-      <c r="X53" s="159"/>
-      <c r="Y53" s="159"/>
-      <c r="Z53" s="159"/>
-      <c r="AA53" s="159"/>
-      <c r="AB53" s="159"/>
-      <c r="AC53" s="159"/>
-      <c r="AD53" s="159"/>
-      <c r="AE53" s="159"/>
-      <c r="AF53" s="159"/>
-      <c r="AG53" s="159"/>
-      <c r="AH53" s="159"/>
-      <c r="AI53" s="159"/>
-      <c r="AJ53" s="159"/>
-      <c r="AK53" s="160"/>
+      <c r="X53" s="141"/>
+      <c r="Y53" s="141"/>
+      <c r="Z53" s="141"/>
+      <c r="AA53" s="141"/>
+      <c r="AB53" s="141"/>
+      <c r="AC53" s="141"/>
+      <c r="AD53" s="141"/>
+      <c r="AE53" s="141"/>
+      <c r="AF53" s="141"/>
+      <c r="AG53" s="141"/>
+      <c r="AH53" s="141"/>
+      <c r="AI53" s="141"/>
+      <c r="AJ53" s="141"/>
+      <c r="AK53" s="142"/>
       <c r="AL53" s="5"/>
       <c r="AM53" s="5"/>
       <c r="AN53" s="5"/>
@@ -12812,46 +12815,46 @@
       <c r="C54" s="80">
         <v>2</v>
       </c>
-      <c r="D54" s="156" t="s">
+      <c r="D54" s="143" t="s">
         <v>30</v>
       </c>
-      <c r="E54" s="157"/>
-      <c r="F54" s="157"/>
-      <c r="G54" s="157"/>
-      <c r="H54" s="162" t="s">
+      <c r="E54" s="136"/>
+      <c r="F54" s="136"/>
+      <c r="G54" s="136"/>
+      <c r="H54" s="137" t="s">
         <v>31</v>
       </c>
-      <c r="I54" s="163"/>
-      <c r="J54" s="163"/>
-      <c r="K54" s="163"/>
-      <c r="L54" s="163"/>
-      <c r="M54" s="163"/>
-      <c r="N54" s="163"/>
-      <c r="O54" s="163"/>
-      <c r="P54" s="163"/>
-      <c r="Q54" s="163"/>
-      <c r="R54" s="163"/>
-      <c r="S54" s="163"/>
-      <c r="T54" s="163"/>
-      <c r="U54" s="163"/>
-      <c r="V54" s="164"/>
-      <c r="W54" s="158" t="s">
+      <c r="I54" s="138"/>
+      <c r="J54" s="138"/>
+      <c r="K54" s="138"/>
+      <c r="L54" s="138"/>
+      <c r="M54" s="138"/>
+      <c r="N54" s="138"/>
+      <c r="O54" s="138"/>
+      <c r="P54" s="138"/>
+      <c r="Q54" s="138"/>
+      <c r="R54" s="138"/>
+      <c r="S54" s="138"/>
+      <c r="T54" s="138"/>
+      <c r="U54" s="138"/>
+      <c r="V54" s="139"/>
+      <c r="W54" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="X54" s="159"/>
-      <c r="Y54" s="159"/>
-      <c r="Z54" s="159"/>
-      <c r="AA54" s="159"/>
-      <c r="AB54" s="159"/>
-      <c r="AC54" s="159"/>
-      <c r="AD54" s="159"/>
-      <c r="AE54" s="159"/>
-      <c r="AF54" s="159"/>
-      <c r="AG54" s="159"/>
-      <c r="AH54" s="159"/>
-      <c r="AI54" s="159"/>
-      <c r="AJ54" s="159"/>
-      <c r="AK54" s="160"/>
+      <c r="X54" s="141"/>
+      <c r="Y54" s="141"/>
+      <c r="Z54" s="141"/>
+      <c r="AA54" s="141"/>
+      <c r="AB54" s="141"/>
+      <c r="AC54" s="141"/>
+      <c r="AD54" s="141"/>
+      <c r="AE54" s="141"/>
+      <c r="AF54" s="141"/>
+      <c r="AG54" s="141"/>
+      <c r="AH54" s="141"/>
+      <c r="AI54" s="141"/>
+      <c r="AJ54" s="141"/>
+      <c r="AK54" s="142"/>
       <c r="AL54" s="5"/>
       <c r="AM54" s="5"/>
       <c r="AN54" s="5"/>
@@ -12864,46 +12867,46 @@
       <c r="C55" s="80">
         <v>3</v>
       </c>
-      <c r="D55" s="156" t="s">
+      <c r="D55" s="143" t="s">
         <v>33</v>
       </c>
-      <c r="E55" s="157"/>
-      <c r="F55" s="157"/>
-      <c r="G55" s="157"/>
-      <c r="H55" s="162" t="s">
+      <c r="E55" s="136"/>
+      <c r="F55" s="136"/>
+      <c r="G55" s="136"/>
+      <c r="H55" s="137" t="s">
         <v>34</v>
       </c>
-      <c r="I55" s="163"/>
-      <c r="J55" s="163"/>
-      <c r="K55" s="163"/>
-      <c r="L55" s="163"/>
-      <c r="M55" s="163"/>
-      <c r="N55" s="163"/>
-      <c r="O55" s="163"/>
-      <c r="P55" s="163"/>
-      <c r="Q55" s="163"/>
-      <c r="R55" s="163"/>
-      <c r="S55" s="163"/>
-      <c r="T55" s="163"/>
-      <c r="U55" s="163"/>
-      <c r="V55" s="164"/>
-      <c r="W55" s="158" t="s">
+      <c r="I55" s="138"/>
+      <c r="J55" s="138"/>
+      <c r="K55" s="138"/>
+      <c r="L55" s="138"/>
+      <c r="M55" s="138"/>
+      <c r="N55" s="138"/>
+      <c r="O55" s="138"/>
+      <c r="P55" s="138"/>
+      <c r="Q55" s="138"/>
+      <c r="R55" s="138"/>
+      <c r="S55" s="138"/>
+      <c r="T55" s="138"/>
+      <c r="U55" s="138"/>
+      <c r="V55" s="139"/>
+      <c r="W55" s="140" t="s">
         <v>35</v>
       </c>
-      <c r="X55" s="159"/>
-      <c r="Y55" s="159"/>
-      <c r="Z55" s="159"/>
-      <c r="AA55" s="159"/>
-      <c r="AB55" s="159"/>
-      <c r="AC55" s="159"/>
-      <c r="AD55" s="159"/>
-      <c r="AE55" s="159"/>
-      <c r="AF55" s="159"/>
-      <c r="AG55" s="159"/>
-      <c r="AH55" s="159"/>
-      <c r="AI55" s="159"/>
-      <c r="AJ55" s="159"/>
-      <c r="AK55" s="160"/>
+      <c r="X55" s="141"/>
+      <c r="Y55" s="141"/>
+      <c r="Z55" s="141"/>
+      <c r="AA55" s="141"/>
+      <c r="AB55" s="141"/>
+      <c r="AC55" s="141"/>
+      <c r="AD55" s="141"/>
+      <c r="AE55" s="141"/>
+      <c r="AF55" s="141"/>
+      <c r="AG55" s="141"/>
+      <c r="AH55" s="141"/>
+      <c r="AI55" s="141"/>
+      <c r="AJ55" s="141"/>
+      <c r="AK55" s="142"/>
       <c r="AL55" s="5"/>
       <c r="AM55" s="5"/>
       <c r="AN55" s="5"/>
@@ -12916,46 +12919,46 @@
       <c r="C56" s="80">
         <v>4</v>
       </c>
-      <c r="D56" s="156" t="s">
+      <c r="D56" s="143" t="s">
         <v>36</v>
       </c>
-      <c r="E56" s="157"/>
-      <c r="F56" s="157"/>
-      <c r="G56" s="157"/>
-      <c r="H56" s="162" t="s">
+      <c r="E56" s="136"/>
+      <c r="F56" s="136"/>
+      <c r="G56" s="136"/>
+      <c r="H56" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="I56" s="163"/>
-      <c r="J56" s="163"/>
-      <c r="K56" s="163"/>
-      <c r="L56" s="163"/>
-      <c r="M56" s="163"/>
-      <c r="N56" s="163"/>
-      <c r="O56" s="163"/>
-      <c r="P56" s="163"/>
-      <c r="Q56" s="163"/>
-      <c r="R56" s="163"/>
-      <c r="S56" s="163"/>
-      <c r="T56" s="163"/>
-      <c r="U56" s="163"/>
-      <c r="V56" s="164"/>
-      <c r="W56" s="158" t="s">
+      <c r="I56" s="138"/>
+      <c r="J56" s="138"/>
+      <c r="K56" s="138"/>
+      <c r="L56" s="138"/>
+      <c r="M56" s="138"/>
+      <c r="N56" s="138"/>
+      <c r="O56" s="138"/>
+      <c r="P56" s="138"/>
+      <c r="Q56" s="138"/>
+      <c r="R56" s="138"/>
+      <c r="S56" s="138"/>
+      <c r="T56" s="138"/>
+      <c r="U56" s="138"/>
+      <c r="V56" s="139"/>
+      <c r="W56" s="140" t="s">
         <v>38</v>
       </c>
-      <c r="X56" s="159"/>
-      <c r="Y56" s="159"/>
-      <c r="Z56" s="159"/>
-      <c r="AA56" s="159"/>
-      <c r="AB56" s="159"/>
-      <c r="AC56" s="159"/>
-      <c r="AD56" s="159"/>
-      <c r="AE56" s="159"/>
-      <c r="AF56" s="159"/>
-      <c r="AG56" s="159"/>
-      <c r="AH56" s="159"/>
-      <c r="AI56" s="159"/>
-      <c r="AJ56" s="159"/>
-      <c r="AK56" s="160"/>
+      <c r="X56" s="141"/>
+      <c r="Y56" s="141"/>
+      <c r="Z56" s="141"/>
+      <c r="AA56" s="141"/>
+      <c r="AB56" s="141"/>
+      <c r="AC56" s="141"/>
+      <c r="AD56" s="141"/>
+      <c r="AE56" s="141"/>
+      <c r="AF56" s="141"/>
+      <c r="AG56" s="141"/>
+      <c r="AH56" s="141"/>
+      <c r="AI56" s="141"/>
+      <c r="AJ56" s="141"/>
+      <c r="AK56" s="142"/>
       <c r="AL56" s="5"/>
       <c r="AM56" s="5"/>
       <c r="AN56" s="5"/>
@@ -12968,46 +12971,46 @@
       <c r="C57" s="80">
         <v>5</v>
       </c>
-      <c r="D57" s="156" t="s">
+      <c r="D57" s="143" t="s">
         <v>39</v>
       </c>
-      <c r="E57" s="157"/>
-      <c r="F57" s="157"/>
-      <c r="G57" s="157"/>
-      <c r="H57" s="158" t="s">
+      <c r="E57" s="136"/>
+      <c r="F57" s="136"/>
+      <c r="G57" s="136"/>
+      <c r="H57" s="140" t="s">
         <v>40</v>
       </c>
-      <c r="I57" s="159"/>
-      <c r="J57" s="159"/>
-      <c r="K57" s="159"/>
-      <c r="L57" s="159"/>
-      <c r="M57" s="159"/>
-      <c r="N57" s="159"/>
-      <c r="O57" s="159"/>
-      <c r="P57" s="159"/>
-      <c r="Q57" s="159"/>
-      <c r="R57" s="159"/>
-      <c r="S57" s="159"/>
-      <c r="T57" s="159"/>
-      <c r="U57" s="159"/>
-      <c r="V57" s="160"/>
-      <c r="W57" s="158" t="s">
+      <c r="I57" s="141"/>
+      <c r="J57" s="141"/>
+      <c r="K57" s="141"/>
+      <c r="L57" s="141"/>
+      <c r="M57" s="141"/>
+      <c r="N57" s="141"/>
+      <c r="O57" s="141"/>
+      <c r="P57" s="141"/>
+      <c r="Q57" s="141"/>
+      <c r="R57" s="141"/>
+      <c r="S57" s="141"/>
+      <c r="T57" s="141"/>
+      <c r="U57" s="141"/>
+      <c r="V57" s="142"/>
+      <c r="W57" s="140" t="s">
         <v>41</v>
       </c>
-      <c r="X57" s="159"/>
-      <c r="Y57" s="159"/>
-      <c r="Z57" s="159"/>
-      <c r="AA57" s="159"/>
-      <c r="AB57" s="159"/>
-      <c r="AC57" s="159"/>
-      <c r="AD57" s="159"/>
-      <c r="AE57" s="159"/>
-      <c r="AF57" s="159"/>
-      <c r="AG57" s="159"/>
-      <c r="AH57" s="159"/>
-      <c r="AI57" s="159"/>
-      <c r="AJ57" s="159"/>
-      <c r="AK57" s="160"/>
+      <c r="X57" s="141"/>
+      <c r="Y57" s="141"/>
+      <c r="Z57" s="141"/>
+      <c r="AA57" s="141"/>
+      <c r="AB57" s="141"/>
+      <c r="AC57" s="141"/>
+      <c r="AD57" s="141"/>
+      <c r="AE57" s="141"/>
+      <c r="AF57" s="141"/>
+      <c r="AG57" s="141"/>
+      <c r="AH57" s="141"/>
+      <c r="AI57" s="141"/>
+      <c r="AJ57" s="141"/>
+      <c r="AK57" s="142"/>
       <c r="AL57" s="5"/>
       <c r="AM57" s="5"/>
       <c r="AN57" s="5"/>
@@ -13109,45 +13112,45 @@
       <c r="B60" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="161" t="s">
+      <c r="C60" s="144" t="s">
         <v>43</v>
       </c>
-      <c r="D60" s="161"/>
-      <c r="E60" s="161"/>
-      <c r="F60" s="161"/>
-      <c r="G60" s="161"/>
-      <c r="H60" s="161" t="s">
+      <c r="D60" s="144"/>
+      <c r="E60" s="144"/>
+      <c r="F60" s="144"/>
+      <c r="G60" s="144"/>
+      <c r="H60" s="144" t="s">
         <v>44</v>
       </c>
-      <c r="I60" s="161"/>
-      <c r="J60" s="161"/>
-      <c r="K60" s="161"/>
-      <c r="L60" s="161"/>
-      <c r="M60" s="161"/>
-      <c r="N60" s="161"/>
-      <c r="O60" s="161"/>
-      <c r="P60" s="161"/>
-      <c r="Q60" s="161"/>
-      <c r="R60" s="161" t="s">
+      <c r="I60" s="144"/>
+      <c r="J60" s="144"/>
+      <c r="K60" s="144"/>
+      <c r="L60" s="144"/>
+      <c r="M60" s="144"/>
+      <c r="N60" s="144"/>
+      <c r="O60" s="144"/>
+      <c r="P60" s="144"/>
+      <c r="Q60" s="144"/>
+      <c r="R60" s="144" t="s">
         <v>45</v>
       </c>
-      <c r="S60" s="161"/>
-      <c r="T60" s="161"/>
-      <c r="U60" s="161"/>
-      <c r="V60" s="161"/>
-      <c r="W60" s="161"/>
-      <c r="X60" s="161"/>
-      <c r="Y60" s="161"/>
-      <c r="Z60" s="161"/>
-      <c r="AA60" s="161"/>
-      <c r="AB60" s="161"/>
-      <c r="AC60" s="161"/>
-      <c r="AD60" s="161"/>
-      <c r="AE60" s="161"/>
-      <c r="AF60" s="161"/>
-      <c r="AG60" s="161"/>
-      <c r="AH60" s="161"/>
-      <c r="AI60" s="161"/>
+      <c r="S60" s="144"/>
+      <c r="T60" s="144"/>
+      <c r="U60" s="144"/>
+      <c r="V60" s="144"/>
+      <c r="W60" s="144"/>
+      <c r="X60" s="144"/>
+      <c r="Y60" s="144"/>
+      <c r="Z60" s="144"/>
+      <c r="AA60" s="144"/>
+      <c r="AB60" s="144"/>
+      <c r="AC60" s="144"/>
+      <c r="AD60" s="144"/>
+      <c r="AE60" s="144"/>
+      <c r="AF60" s="144"/>
+      <c r="AG60" s="144"/>
+      <c r="AH60" s="144"/>
+      <c r="AI60" s="144"/>
       <c r="AJ60" s="64"/>
       <c r="AK60" s="64"/>
       <c r="AL60" s="64"/>
@@ -13161,13 +13164,13 @@
       <c r="B61" s="83">
         <v>1</v>
       </c>
-      <c r="C61" s="124" t="s">
+      <c r="C61" s="148" t="s">
         <v>46</v>
       </c>
-      <c r="D61" s="125"/>
-      <c r="E61" s="125"/>
-      <c r="F61" s="125"/>
-      <c r="G61" s="126"/>
+      <c r="D61" s="149"/>
+      <c r="E61" s="149"/>
+      <c r="F61" s="149"/>
+      <c r="G61" s="150"/>
       <c r="H61" s="84" t="s">
         <v>47</v>
       </c>
@@ -13180,26 +13183,26 @@
       <c r="O61" s="88"/>
       <c r="P61" s="88"/>
       <c r="Q61" s="88"/>
-      <c r="R61" s="153" t="s">
+      <c r="R61" s="145" t="s">
         <v>48</v>
       </c>
-      <c r="S61" s="154"/>
-      <c r="T61" s="154"/>
-      <c r="U61" s="154"/>
-      <c r="V61" s="154"/>
-      <c r="W61" s="154"/>
-      <c r="X61" s="154"/>
-      <c r="Y61" s="154"/>
-      <c r="Z61" s="154"/>
-      <c r="AA61" s="154"/>
-      <c r="AB61" s="154"/>
-      <c r="AC61" s="154"/>
-      <c r="AD61" s="154"/>
-      <c r="AE61" s="154"/>
-      <c r="AF61" s="154"/>
-      <c r="AG61" s="154"/>
-      <c r="AH61" s="154"/>
-      <c r="AI61" s="155"/>
+      <c r="S61" s="146"/>
+      <c r="T61" s="146"/>
+      <c r="U61" s="146"/>
+      <c r="V61" s="146"/>
+      <c r="W61" s="146"/>
+      <c r="X61" s="146"/>
+      <c r="Y61" s="146"/>
+      <c r="Z61" s="146"/>
+      <c r="AA61" s="146"/>
+      <c r="AB61" s="146"/>
+      <c r="AC61" s="146"/>
+      <c r="AD61" s="146"/>
+      <c r="AE61" s="146"/>
+      <c r="AF61" s="146"/>
+      <c r="AG61" s="146"/>
+      <c r="AH61" s="146"/>
+      <c r="AI61" s="147"/>
       <c r="AJ61" s="5"/>
       <c r="AK61" s="5"/>
       <c r="AL61" s="5"/>
@@ -13213,13 +13216,13 @@
       <c r="B62" s="86">
         <v>2</v>
       </c>
-      <c r="C62" s="124" t="s">
+      <c r="C62" s="148" t="s">
         <v>49</v>
       </c>
-      <c r="D62" s="125"/>
-      <c r="E62" s="125"/>
-      <c r="F62" s="125"/>
-      <c r="G62" s="126"/>
+      <c r="D62" s="149"/>
+      <c r="E62" s="149"/>
+      <c r="F62" s="149"/>
+      <c r="G62" s="150"/>
       <c r="H62" s="87" t="s">
         <v>50</v>
       </c>
@@ -13232,26 +13235,26 @@
       <c r="O62" s="90"/>
       <c r="P62" s="90"/>
       <c r="Q62" s="90"/>
-      <c r="R62" s="127" t="s">
+      <c r="R62" s="151" t="s">
         <v>51</v>
       </c>
-      <c r="S62" s="128"/>
-      <c r="T62" s="128"/>
-      <c r="U62" s="128"/>
-      <c r="V62" s="128"/>
-      <c r="W62" s="128"/>
-      <c r="X62" s="128"/>
-      <c r="Y62" s="128"/>
-      <c r="Z62" s="128"/>
-      <c r="AA62" s="128"/>
-      <c r="AB62" s="128"/>
-      <c r="AC62" s="128"/>
-      <c r="AD62" s="128"/>
-      <c r="AE62" s="128"/>
-      <c r="AF62" s="128"/>
-      <c r="AG62" s="128"/>
-      <c r="AH62" s="128"/>
-      <c r="AI62" s="129"/>
+      <c r="S62" s="152"/>
+      <c r="T62" s="152"/>
+      <c r="U62" s="152"/>
+      <c r="V62" s="152"/>
+      <c r="W62" s="152"/>
+      <c r="X62" s="152"/>
+      <c r="Y62" s="152"/>
+      <c r="Z62" s="152"/>
+      <c r="AA62" s="152"/>
+      <c r="AB62" s="152"/>
+      <c r="AC62" s="152"/>
+      <c r="AD62" s="152"/>
+      <c r="AE62" s="152"/>
+      <c r="AF62" s="152"/>
+      <c r="AG62" s="152"/>
+      <c r="AH62" s="152"/>
+      <c r="AI62" s="153"/>
       <c r="AJ62" s="55"/>
       <c r="AK62" s="55"/>
       <c r="AL62" s="55"/>
@@ -13265,13 +13268,13 @@
       <c r="B63" s="86">
         <v>3</v>
       </c>
-      <c r="C63" s="124" t="s">
+      <c r="C63" s="148" t="s">
         <v>52</v>
       </c>
-      <c r="D63" s="125"/>
-      <c r="E63" s="125"/>
-      <c r="F63" s="125"/>
-      <c r="G63" s="126"/>
+      <c r="D63" s="149"/>
+      <c r="E63" s="149"/>
+      <c r="F63" s="149"/>
+      <c r="G63" s="150"/>
       <c r="H63" s="87" t="s">
         <v>53</v>
       </c>
@@ -13284,26 +13287,26 @@
       <c r="O63" s="90"/>
       <c r="P63" s="90"/>
       <c r="Q63" s="90"/>
-      <c r="R63" s="127" t="s">
+      <c r="R63" s="151" t="s">
         <v>54</v>
       </c>
-      <c r="S63" s="128"/>
-      <c r="T63" s="128"/>
-      <c r="U63" s="128"/>
-      <c r="V63" s="128"/>
-      <c r="W63" s="128"/>
-      <c r="X63" s="128"/>
-      <c r="Y63" s="128"/>
-      <c r="Z63" s="128"/>
-      <c r="AA63" s="128"/>
-      <c r="AB63" s="128"/>
-      <c r="AC63" s="128"/>
-      <c r="AD63" s="128"/>
-      <c r="AE63" s="128"/>
-      <c r="AF63" s="128"/>
-      <c r="AG63" s="128"/>
-      <c r="AH63" s="128"/>
-      <c r="AI63" s="129"/>
+      <c r="S63" s="152"/>
+      <c r="T63" s="152"/>
+      <c r="U63" s="152"/>
+      <c r="V63" s="152"/>
+      <c r="W63" s="152"/>
+      <c r="X63" s="152"/>
+      <c r="Y63" s="152"/>
+      <c r="Z63" s="152"/>
+      <c r="AA63" s="152"/>
+      <c r="AB63" s="152"/>
+      <c r="AC63" s="152"/>
+      <c r="AD63" s="152"/>
+      <c r="AE63" s="152"/>
+      <c r="AF63" s="152"/>
+      <c r="AG63" s="152"/>
+      <c r="AH63" s="152"/>
+      <c r="AI63" s="153"/>
       <c r="AJ63" s="55"/>
       <c r="AK63" s="55"/>
       <c r="AL63" s="55"/>
@@ -13323,13 +13326,13 @@
       <c r="B64" s="86">
         <v>4</v>
       </c>
-      <c r="C64" s="124" t="s">
+      <c r="C64" s="148" t="s">
         <v>55</v>
       </c>
-      <c r="D64" s="125"/>
-      <c r="E64" s="125"/>
-      <c r="F64" s="125"/>
-      <c r="G64" s="126"/>
+      <c r="D64" s="149"/>
+      <c r="E64" s="149"/>
+      <c r="F64" s="149"/>
+      <c r="G64" s="150"/>
       <c r="H64" s="87" t="s">
         <v>56</v>
       </c>
@@ -13342,26 +13345,26 @@
       <c r="O64" s="90"/>
       <c r="P64" s="90"/>
       <c r="Q64" s="90"/>
-      <c r="R64" s="127" t="s">
+      <c r="R64" s="151" t="s">
         <v>57</v>
       </c>
-      <c r="S64" s="128"/>
-      <c r="T64" s="128"/>
-      <c r="U64" s="128"/>
-      <c r="V64" s="128"/>
-      <c r="W64" s="128"/>
-      <c r="X64" s="128"/>
-      <c r="Y64" s="128"/>
-      <c r="Z64" s="128"/>
-      <c r="AA64" s="128"/>
-      <c r="AB64" s="128"/>
-      <c r="AC64" s="128"/>
-      <c r="AD64" s="128"/>
-      <c r="AE64" s="128"/>
-      <c r="AF64" s="128"/>
-      <c r="AG64" s="128"/>
-      <c r="AH64" s="128"/>
-      <c r="AI64" s="129"/>
+      <c r="S64" s="152"/>
+      <c r="T64" s="152"/>
+      <c r="U64" s="152"/>
+      <c r="V64" s="152"/>
+      <c r="W64" s="152"/>
+      <c r="X64" s="152"/>
+      <c r="Y64" s="152"/>
+      <c r="Z64" s="152"/>
+      <c r="AA64" s="152"/>
+      <c r="AB64" s="152"/>
+      <c r="AC64" s="152"/>
+      <c r="AD64" s="152"/>
+      <c r="AE64" s="152"/>
+      <c r="AF64" s="152"/>
+      <c r="AG64" s="152"/>
+      <c r="AH64" s="152"/>
+      <c r="AI64" s="153"/>
       <c r="AJ64" s="55"/>
       <c r="AK64" s="55"/>
       <c r="AL64" s="55"/>
@@ -13381,13 +13384,13 @@
       <c r="B65" s="86">
         <v>5</v>
       </c>
-      <c r="C65" s="124" t="s">
+      <c r="C65" s="148" t="s">
         <v>58</v>
       </c>
-      <c r="D65" s="125"/>
-      <c r="E65" s="125"/>
-      <c r="F65" s="125"/>
-      <c r="G65" s="126"/>
+      <c r="D65" s="149"/>
+      <c r="E65" s="149"/>
+      <c r="F65" s="149"/>
+      <c r="G65" s="150"/>
       <c r="H65" s="87" t="s">
         <v>59</v>
       </c>
@@ -13400,26 +13403,26 @@
       <c r="O65" s="90"/>
       <c r="P65" s="90"/>
       <c r="Q65" s="90"/>
-      <c r="R65" s="127" t="s">
+      <c r="R65" s="151" t="s">
         <v>60</v>
       </c>
-      <c r="S65" s="128"/>
-      <c r="T65" s="128"/>
-      <c r="U65" s="128"/>
-      <c r="V65" s="128"/>
-      <c r="W65" s="128"/>
-      <c r="X65" s="128"/>
-      <c r="Y65" s="128"/>
-      <c r="Z65" s="128"/>
-      <c r="AA65" s="128"/>
-      <c r="AB65" s="128"/>
-      <c r="AC65" s="128"/>
-      <c r="AD65" s="128"/>
-      <c r="AE65" s="128"/>
-      <c r="AF65" s="128"/>
-      <c r="AG65" s="128"/>
-      <c r="AH65" s="128"/>
-      <c r="AI65" s="129"/>
+      <c r="S65" s="152"/>
+      <c r="T65" s="152"/>
+      <c r="U65" s="152"/>
+      <c r="V65" s="152"/>
+      <c r="W65" s="152"/>
+      <c r="X65" s="152"/>
+      <c r="Y65" s="152"/>
+      <c r="Z65" s="152"/>
+      <c r="AA65" s="152"/>
+      <c r="AB65" s="152"/>
+      <c r="AC65" s="152"/>
+      <c r="AD65" s="152"/>
+      <c r="AE65" s="152"/>
+      <c r="AF65" s="152"/>
+      <c r="AG65" s="152"/>
+      <c r="AH65" s="152"/>
+      <c r="AI65" s="153"/>
       <c r="AJ65" s="55"/>
       <c r="AK65" s="55"/>
       <c r="AL65" s="55"/>
@@ -13439,13 +13442,13 @@
       <c r="B66" s="86">
         <v>6</v>
       </c>
-      <c r="C66" s="124" t="s">
+      <c r="C66" s="148" t="s">
         <v>61</v>
       </c>
-      <c r="D66" s="125"/>
-      <c r="E66" s="125"/>
-      <c r="F66" s="125"/>
-      <c r="G66" s="126"/>
+      <c r="D66" s="149"/>
+      <c r="E66" s="149"/>
+      <c r="F66" s="149"/>
+      <c r="G66" s="150"/>
       <c r="H66" s="87" t="s">
         <v>62</v>
       </c>
@@ -13458,26 +13461,26 @@
       <c r="O66" s="90"/>
       <c r="P66" s="90"/>
       <c r="Q66" s="90"/>
-      <c r="R66" s="127" t="s">
+      <c r="R66" s="151" t="s">
         <v>63</v>
       </c>
-      <c r="S66" s="128"/>
-      <c r="T66" s="128"/>
-      <c r="U66" s="128"/>
-      <c r="V66" s="128"/>
-      <c r="W66" s="128"/>
-      <c r="X66" s="128"/>
-      <c r="Y66" s="128"/>
-      <c r="Z66" s="128"/>
-      <c r="AA66" s="128"/>
-      <c r="AB66" s="128"/>
-      <c r="AC66" s="128"/>
-      <c r="AD66" s="128"/>
-      <c r="AE66" s="128"/>
-      <c r="AF66" s="128"/>
-      <c r="AG66" s="128"/>
-      <c r="AH66" s="128"/>
-      <c r="AI66" s="129"/>
+      <c r="S66" s="152"/>
+      <c r="T66" s="152"/>
+      <c r="U66" s="152"/>
+      <c r="V66" s="152"/>
+      <c r="W66" s="152"/>
+      <c r="X66" s="152"/>
+      <c r="Y66" s="152"/>
+      <c r="Z66" s="152"/>
+      <c r="AA66" s="152"/>
+      <c r="AB66" s="152"/>
+      <c r="AC66" s="152"/>
+      <c r="AD66" s="152"/>
+      <c r="AE66" s="152"/>
+      <c r="AF66" s="152"/>
+      <c r="AG66" s="152"/>
+      <c r="AH66" s="152"/>
+      <c r="AI66" s="153"/>
       <c r="AJ66" s="55"/>
       <c r="AK66" s="55"/>
       <c r="AL66" s="55"/>
@@ -13497,11 +13500,11 @@
       <c r="B67" s="86">
         <v>7</v>
       </c>
-      <c r="C67" s="124"/>
-      <c r="D67" s="125"/>
-      <c r="E67" s="125"/>
-      <c r="F67" s="125"/>
-      <c r="G67" s="126"/>
+      <c r="C67" s="148"/>
+      <c r="D67" s="149"/>
+      <c r="E67" s="149"/>
+      <c r="F67" s="149"/>
+      <c r="G67" s="150"/>
       <c r="H67" s="87"/>
       <c r="I67" s="90"/>
       <c r="J67" s="90"/>
@@ -13512,24 +13515,24 @@
       <c r="O67" s="90"/>
       <c r="P67" s="90"/>
       <c r="Q67" s="90"/>
-      <c r="R67" s="127"/>
-      <c r="S67" s="128"/>
-      <c r="T67" s="128"/>
-      <c r="U67" s="128"/>
-      <c r="V67" s="128"/>
-      <c r="W67" s="128"/>
-      <c r="X67" s="128"/>
-      <c r="Y67" s="128"/>
-      <c r="Z67" s="128"/>
-      <c r="AA67" s="128"/>
-      <c r="AB67" s="128"/>
-      <c r="AC67" s="128"/>
-      <c r="AD67" s="128"/>
-      <c r="AE67" s="128"/>
-      <c r="AF67" s="128"/>
-      <c r="AG67" s="128"/>
-      <c r="AH67" s="128"/>
-      <c r="AI67" s="129"/>
+      <c r="R67" s="151"/>
+      <c r="S67" s="152"/>
+      <c r="T67" s="152"/>
+      <c r="U67" s="152"/>
+      <c r="V67" s="152"/>
+      <c r="W67" s="152"/>
+      <c r="X67" s="152"/>
+      <c r="Y67" s="152"/>
+      <c r="Z67" s="152"/>
+      <c r="AA67" s="152"/>
+      <c r="AB67" s="152"/>
+      <c r="AC67" s="152"/>
+      <c r="AD67" s="152"/>
+      <c r="AE67" s="152"/>
+      <c r="AF67" s="152"/>
+      <c r="AG67" s="152"/>
+      <c r="AH67" s="152"/>
+      <c r="AI67" s="153"/>
       <c r="AJ67" s="55"/>
       <c r="AK67" s="55"/>
       <c r="AL67" s="55"/>
@@ -13549,11 +13552,11 @@
       <c r="B68" s="97">
         <v>8</v>
       </c>
-      <c r="C68" s="124"/>
-      <c r="D68" s="125"/>
-      <c r="E68" s="125"/>
-      <c r="F68" s="125"/>
-      <c r="G68" s="126"/>
+      <c r="C68" s="148"/>
+      <c r="D68" s="149"/>
+      <c r="E68" s="149"/>
+      <c r="F68" s="149"/>
+      <c r="G68" s="150"/>
       <c r="H68" s="98"/>
       <c r="I68" s="99"/>
       <c r="J68" s="99"/>
@@ -13564,24 +13567,24 @@
       <c r="O68" s="99"/>
       <c r="P68" s="99"/>
       <c r="Q68" s="99"/>
-      <c r="R68" s="130"/>
-      <c r="S68" s="131"/>
-      <c r="T68" s="131"/>
-      <c r="U68" s="131"/>
-      <c r="V68" s="131"/>
-      <c r="W68" s="131"/>
-      <c r="X68" s="131"/>
-      <c r="Y68" s="131"/>
-      <c r="Z68" s="131"/>
-      <c r="AA68" s="131"/>
-      <c r="AB68" s="131"/>
-      <c r="AC68" s="131"/>
-      <c r="AD68" s="131"/>
-      <c r="AE68" s="131"/>
-      <c r="AF68" s="131"/>
-      <c r="AG68" s="131"/>
-      <c r="AH68" s="131"/>
-      <c r="AI68" s="132"/>
+      <c r="R68" s="154"/>
+      <c r="S68" s="155"/>
+      <c r="T68" s="155"/>
+      <c r="U68" s="155"/>
+      <c r="V68" s="155"/>
+      <c r="W68" s="155"/>
+      <c r="X68" s="155"/>
+      <c r="Y68" s="155"/>
+      <c r="Z68" s="155"/>
+      <c r="AA68" s="155"/>
+      <c r="AB68" s="155"/>
+      <c r="AC68" s="155"/>
+      <c r="AD68" s="155"/>
+      <c r="AE68" s="155"/>
+      <c r="AF68" s="155"/>
+      <c r="AG68" s="155"/>
+      <c r="AH68" s="155"/>
+      <c r="AI68" s="156"/>
       <c r="AJ68" s="55"/>
       <c r="AK68" s="55"/>
       <c r="AL68" s="55"/>
@@ -14829,37 +14832,6 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="G1:AD1"/>
-    <mergeCell ref="AE1:AH1"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="AM1:AP1"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="H52:V52"/>
-    <mergeCell ref="W52:AK52"/>
-    <mergeCell ref="AM2:AP3"/>
-    <mergeCell ref="D53:G53"/>
-    <mergeCell ref="H53:V53"/>
-    <mergeCell ref="W53:AK53"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="H54:V54"/>
-    <mergeCell ref="W54:AK54"/>
-    <mergeCell ref="D55:G55"/>
-    <mergeCell ref="H55:V55"/>
-    <mergeCell ref="W55:AK55"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="H56:V56"/>
-    <mergeCell ref="W56:AK56"/>
-    <mergeCell ref="D57:G57"/>
-    <mergeCell ref="H57:V57"/>
-    <mergeCell ref="W57:AK57"/>
-    <mergeCell ref="C60:G60"/>
-    <mergeCell ref="H60:Q60"/>
-    <mergeCell ref="R60:AI60"/>
-    <mergeCell ref="R61:AI61"/>
-    <mergeCell ref="C62:G62"/>
-    <mergeCell ref="R62:AI62"/>
-    <mergeCell ref="C63:G63"/>
-    <mergeCell ref="R63:AI63"/>
     <mergeCell ref="C67:G67"/>
     <mergeCell ref="R67:AI67"/>
     <mergeCell ref="C68:G68"/>
@@ -14876,6 +14848,37 @@
     <mergeCell ref="C66:G66"/>
     <mergeCell ref="R66:AI66"/>
     <mergeCell ref="C61:G61"/>
+    <mergeCell ref="R61:AI61"/>
+    <mergeCell ref="C62:G62"/>
+    <mergeCell ref="R62:AI62"/>
+    <mergeCell ref="C63:G63"/>
+    <mergeCell ref="R63:AI63"/>
+    <mergeCell ref="D57:G57"/>
+    <mergeCell ref="H57:V57"/>
+    <mergeCell ref="W57:AK57"/>
+    <mergeCell ref="C60:G60"/>
+    <mergeCell ref="H60:Q60"/>
+    <mergeCell ref="R60:AI60"/>
+    <mergeCell ref="D55:G55"/>
+    <mergeCell ref="H55:V55"/>
+    <mergeCell ref="W55:AK55"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="H56:V56"/>
+    <mergeCell ref="W56:AK56"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="H53:V53"/>
+    <mergeCell ref="W53:AK53"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="H54:V54"/>
+    <mergeCell ref="W54:AK54"/>
+    <mergeCell ref="G1:AD1"/>
+    <mergeCell ref="AE1:AH1"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="AM1:AP1"/>
+    <mergeCell ref="D52:G52"/>
+    <mergeCell ref="H52:V52"/>
+    <mergeCell ref="W52:AK52"/>
+    <mergeCell ref="AM2:AP3"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="77" orientation="landscape"/>
@@ -14891,12 +14894,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AR72"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="AX61" sqref="AX61"/>
     </sheetView>
   </sheetViews>
@@ -14909,173 +14924,173 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" s="1" customFormat="1">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="163" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="165" t="s">
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="125" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="167"/>
-      <c r="L1" s="176" t="s">
+      <c r="H1" s="126"/>
+      <c r="I1" s="126"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="127"/>
+      <c r="L1" s="174" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="176"/>
-      <c r="N1" s="176"/>
-      <c r="O1" s="176"/>
-      <c r="P1" s="176"/>
-      <c r="Q1" s="176"/>
-      <c r="R1" s="176"/>
-      <c r="S1" s="176"/>
-      <c r="T1" s="176" t="s">
+      <c r="M1" s="174"/>
+      <c r="N1" s="174"/>
+      <c r="O1" s="174"/>
+      <c r="P1" s="174"/>
+      <c r="Q1" s="174"/>
+      <c r="R1" s="174"/>
+      <c r="S1" s="174"/>
+      <c r="T1" s="174" t="s">
         <v>71</v>
       </c>
-      <c r="U1" s="176"/>
-      <c r="V1" s="176"/>
-      <c r="W1" s="176"/>
-      <c r="X1" s="176"/>
-      <c r="Y1" s="176"/>
-      <c r="Z1" s="176"/>
-      <c r="AA1" s="176"/>
-      <c r="AB1" s="176"/>
-      <c r="AC1" s="176"/>
-      <c r="AD1" s="176"/>
-      <c r="AE1" s="176"/>
-      <c r="AF1" s="176"/>
-      <c r="AG1" s="165" t="s">
+      <c r="U1" s="174"/>
+      <c r="V1" s="174"/>
+      <c r="W1" s="174"/>
+      <c r="X1" s="174"/>
+      <c r="Y1" s="174"/>
+      <c r="Z1" s="174"/>
+      <c r="AA1" s="174"/>
+      <c r="AB1" s="174"/>
+      <c r="AC1" s="174"/>
+      <c r="AD1" s="174"/>
+      <c r="AE1" s="174"/>
+      <c r="AF1" s="174"/>
+      <c r="AG1" s="125" t="s">
         <v>13</v>
       </c>
-      <c r="AH1" s="166"/>
-      <c r="AI1" s="166"/>
-      <c r="AJ1" s="167"/>
-      <c r="AK1" s="166" t="s">
+      <c r="AH1" s="126"/>
+      <c r="AI1" s="126"/>
+      <c r="AJ1" s="127"/>
+      <c r="AK1" s="126" t="s">
         <v>14</v>
       </c>
-      <c r="AL1" s="166"/>
-      <c r="AM1" s="166"/>
-      <c r="AN1" s="167"/>
-      <c r="AO1" s="165" t="s">
+      <c r="AL1" s="126"/>
+      <c r="AM1" s="126"/>
+      <c r="AN1" s="127"/>
+      <c r="AO1" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="AP1" s="166"/>
-      <c r="AQ1" s="166"/>
-      <c r="AR1" s="167"/>
+      <c r="AP1" s="126"/>
+      <c r="AQ1" s="126"/>
+      <c r="AR1" s="127"/>
     </row>
     <row r="2" spans="1:44" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="143"/>
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="143"/>
-      <c r="G2" s="133" t="str">
+      <c r="A2" s="163"/>
+      <c r="B2" s="163"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="163"/>
+      <c r="F2" s="163"/>
+      <c r="G2" s="157" t="str">
         <f>T2</f>
         <v>Đăng kí thẻ</v>
       </c>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="135"/>
-      <c r="L2" s="175" t="str">
+      <c r="H2" s="158"/>
+      <c r="I2" s="158"/>
+      <c r="J2" s="158"/>
+      <c r="K2" s="159"/>
+      <c r="L2" s="173" t="str">
         <f>Cover!C61</f>
         <v>UC_001</v>
       </c>
-      <c r="M2" s="175"/>
-      <c r="N2" s="175"/>
-      <c r="O2" s="175"/>
-      <c r="P2" s="175"/>
-      <c r="Q2" s="175"/>
-      <c r="R2" s="175"/>
-      <c r="S2" s="175"/>
-      <c r="T2" s="175" t="str">
+      <c r="M2" s="173"/>
+      <c r="N2" s="173"/>
+      <c r="O2" s="173"/>
+      <c r="P2" s="173"/>
+      <c r="Q2" s="173"/>
+      <c r="R2" s="173"/>
+      <c r="S2" s="173"/>
+      <c r="T2" s="173" t="str">
         <f>Cover!H61</f>
         <v>Đăng kí thẻ</v>
       </c>
-      <c r="U2" s="175"/>
-      <c r="V2" s="175"/>
-      <c r="W2" s="175"/>
-      <c r="X2" s="175"/>
-      <c r="Y2" s="175"/>
-      <c r="Z2" s="175"/>
-      <c r="AA2" s="175"/>
-      <c r="AB2" s="175"/>
-      <c r="AC2" s="175"/>
-      <c r="AD2" s="175"/>
-      <c r="AE2" s="175"/>
-      <c r="AF2" s="175"/>
-      <c r="AG2" s="133" t="s">
+      <c r="U2" s="173"/>
+      <c r="V2" s="173"/>
+      <c r="W2" s="173"/>
+      <c r="X2" s="173"/>
+      <c r="Y2" s="173"/>
+      <c r="Z2" s="173"/>
+      <c r="AA2" s="173"/>
+      <c r="AB2" s="173"/>
+      <c r="AC2" s="173"/>
+      <c r="AD2" s="173"/>
+      <c r="AE2" s="173"/>
+      <c r="AF2" s="173"/>
+      <c r="AG2" s="157" t="s">
         <v>7</v>
       </c>
-      <c r="AH2" s="134"/>
-      <c r="AI2" s="134"/>
-      <c r="AJ2" s="135"/>
-      <c r="AK2" s="139">
+      <c r="AH2" s="158"/>
+      <c r="AI2" s="158"/>
+      <c r="AJ2" s="159"/>
+      <c r="AK2" s="132">
         <f>DATE(2016,2,3)</f>
         <v>42403</v>
       </c>
-      <c r="AL2" s="139"/>
-      <c r="AM2" s="139"/>
-      <c r="AN2" s="140"/>
-      <c r="AO2" s="139">
+      <c r="AL2" s="132"/>
+      <c r="AM2" s="132"/>
+      <c r="AN2" s="133"/>
+      <c r="AO2" s="132">
         <f>DATE(2017,2,12)</f>
         <v>42778</v>
       </c>
-      <c r="AP2" s="139"/>
-      <c r="AQ2" s="139"/>
-      <c r="AR2" s="140"/>
+      <c r="AP2" s="132"/>
+      <c r="AQ2" s="132"/>
+      <c r="AR2" s="133"/>
     </row>
     <row r="3" spans="1:44" s="1" customFormat="1">
-      <c r="A3" s="143"/>
-      <c r="B3" s="143"/>
-      <c r="C3" s="143"/>
-      <c r="D3" s="143"/>
-      <c r="E3" s="143"/>
-      <c r="F3" s="143"/>
-      <c r="G3" s="136"/>
-      <c r="H3" s="137"/>
-      <c r="I3" s="137"/>
-      <c r="J3" s="137"/>
-      <c r="K3" s="138"/>
-      <c r="L3" s="175"/>
-      <c r="M3" s="175"/>
-      <c r="N3" s="175"/>
-      <c r="O3" s="175"/>
-      <c r="P3" s="175"/>
-      <c r="Q3" s="175"/>
-      <c r="R3" s="175"/>
-      <c r="S3" s="175"/>
-      <c r="T3" s="175"/>
-      <c r="U3" s="175"/>
-      <c r="V3" s="175"/>
-      <c r="W3" s="175"/>
-      <c r="X3" s="175"/>
-      <c r="Y3" s="175"/>
-      <c r="Z3" s="175"/>
-      <c r="AA3" s="175"/>
-      <c r="AB3" s="175"/>
-      <c r="AC3" s="175"/>
-      <c r="AD3" s="175"/>
-      <c r="AE3" s="175"/>
-      <c r="AF3" s="175"/>
-      <c r="AG3" s="136"/>
-      <c r="AH3" s="137"/>
-      <c r="AI3" s="137"/>
-      <c r="AJ3" s="138"/>
-      <c r="AK3" s="141"/>
-      <c r="AL3" s="141"/>
-      <c r="AM3" s="141"/>
-      <c r="AN3" s="142"/>
-      <c r="AO3" s="141"/>
-      <c r="AP3" s="141"/>
-      <c r="AQ3" s="141"/>
-      <c r="AR3" s="142"/>
+      <c r="A3" s="163"/>
+      <c r="B3" s="163"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="163"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="161"/>
+      <c r="K3" s="162"/>
+      <c r="L3" s="173"/>
+      <c r="M3" s="173"/>
+      <c r="N3" s="173"/>
+      <c r="O3" s="173"/>
+      <c r="P3" s="173"/>
+      <c r="Q3" s="173"/>
+      <c r="R3" s="173"/>
+      <c r="S3" s="173"/>
+      <c r="T3" s="173"/>
+      <c r="U3" s="173"/>
+      <c r="V3" s="173"/>
+      <c r="W3" s="173"/>
+      <c r="X3" s="173"/>
+      <c r="Y3" s="173"/>
+      <c r="Z3" s="173"/>
+      <c r="AA3" s="173"/>
+      <c r="AB3" s="173"/>
+      <c r="AC3" s="173"/>
+      <c r="AD3" s="173"/>
+      <c r="AE3" s="173"/>
+      <c r="AF3" s="173"/>
+      <c r="AG3" s="160"/>
+      <c r="AH3" s="161"/>
+      <c r="AI3" s="161"/>
+      <c r="AJ3" s="162"/>
+      <c r="AK3" s="134"/>
+      <c r="AL3" s="134"/>
+      <c r="AM3" s="134"/>
+      <c r="AN3" s="135"/>
+      <c r="AO3" s="134"/>
+      <c r="AP3" s="134"/>
+      <c r="AQ3" s="134"/>
+      <c r="AR3" s="135"/>
     </row>
     <row r="4" spans="1:44">
       <c r="A4" s="4"/>
@@ -16745,22 +16760,22 @@
       <c r="E39" s="42"/>
       <c r="F39" s="42"/>
       <c r="G39" s="28"/>
-      <c r="H39" s="174"/>
-      <c r="I39" s="174"/>
-      <c r="J39" s="174"/>
-      <c r="K39" s="174"/>
-      <c r="L39" s="174"/>
-      <c r="M39" s="174"/>
-      <c r="N39" s="174"/>
-      <c r="O39" s="174"/>
-      <c r="P39" s="174"/>
-      <c r="Q39" s="174"/>
-      <c r="R39" s="174"/>
-      <c r="S39" s="174"/>
-      <c r="T39" s="174"/>
-      <c r="U39" s="174"/>
-      <c r="V39" s="174"/>
-      <c r="W39" s="174"/>
+      <c r="H39" s="175"/>
+      <c r="I39" s="175"/>
+      <c r="J39" s="175"/>
+      <c r="K39" s="175"/>
+      <c r="L39" s="175"/>
+      <c r="M39" s="175"/>
+      <c r="N39" s="175"/>
+      <c r="O39" s="175"/>
+      <c r="P39" s="175"/>
+      <c r="Q39" s="175"/>
+      <c r="R39" s="175"/>
+      <c r="S39" s="175"/>
+      <c r="T39" s="175"/>
+      <c r="U39" s="175"/>
+      <c r="V39" s="175"/>
+      <c r="W39" s="175"/>
       <c r="X39" s="49"/>
       <c r="Y39" s="49"/>
       <c r="Z39" s="44"/>
@@ -16776,9 +16791,9 @@
       <c r="AJ39" s="28"/>
       <c r="AK39" s="28"/>
       <c r="AL39" s="28"/>
-      <c r="AM39" s="172"/>
-      <c r="AN39" s="172"/>
-      <c r="AO39" s="172"/>
+      <c r="AM39" s="176"/>
+      <c r="AN39" s="176"/>
+      <c r="AO39" s="176"/>
       <c r="AP39" s="28"/>
       <c r="AQ39" s="5"/>
       <c r="AR39" s="23"/>
@@ -16791,22 +16806,22 @@
       <c r="E40" s="42"/>
       <c r="F40" s="42"/>
       <c r="G40" s="28"/>
-      <c r="H40" s="174"/>
-      <c r="I40" s="174"/>
-      <c r="J40" s="174"/>
-      <c r="K40" s="174"/>
-      <c r="L40" s="174"/>
-      <c r="M40" s="174"/>
-      <c r="N40" s="174"/>
-      <c r="O40" s="174"/>
-      <c r="P40" s="174"/>
-      <c r="Q40" s="174"/>
-      <c r="R40" s="174"/>
-      <c r="S40" s="174"/>
-      <c r="T40" s="174"/>
-      <c r="U40" s="174"/>
-      <c r="V40" s="174"/>
-      <c r="W40" s="174"/>
+      <c r="H40" s="175"/>
+      <c r="I40" s="175"/>
+      <c r="J40" s="175"/>
+      <c r="K40" s="175"/>
+      <c r="L40" s="175"/>
+      <c r="M40" s="175"/>
+      <c r="N40" s="175"/>
+      <c r="O40" s="175"/>
+      <c r="P40" s="175"/>
+      <c r="Q40" s="175"/>
+      <c r="R40" s="175"/>
+      <c r="S40" s="175"/>
+      <c r="T40" s="175"/>
+      <c r="U40" s="175"/>
+      <c r="V40" s="175"/>
+      <c r="W40" s="175"/>
       <c r="X40" s="49"/>
       <c r="Y40" s="49"/>
       <c r="Z40" s="44"/>
@@ -16822,9 +16837,9 @@
       <c r="AJ40" s="28"/>
       <c r="AK40" s="28"/>
       <c r="AL40" s="28"/>
-      <c r="AM40" s="172"/>
-      <c r="AN40" s="172"/>
-      <c r="AO40" s="172"/>
+      <c r="AM40" s="176"/>
+      <c r="AN40" s="176"/>
+      <c r="AO40" s="176"/>
       <c r="AP40" s="28"/>
       <c r="AQ40" s="5"/>
       <c r="AR40" s="23"/>
@@ -16929,33 +16944,33 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="173"/>
-      <c r="I43" s="173"/>
-      <c r="J43" s="173"/>
-      <c r="K43" s="173"/>
-      <c r="L43" s="173"/>
-      <c r="M43" s="173"/>
-      <c r="N43" s="173"/>
-      <c r="O43" s="173"/>
-      <c r="P43" s="173"/>
-      <c r="Q43" s="173"/>
-      <c r="R43" s="173"/>
-      <c r="S43" s="173"/>
-      <c r="T43" s="173"/>
-      <c r="U43" s="173"/>
-      <c r="V43" s="173"/>
-      <c r="W43" s="173"/>
-      <c r="X43" s="173"/>
-      <c r="Y43" s="173"/>
-      <c r="Z43" s="173"/>
-      <c r="AA43" s="173"/>
-      <c r="AB43" s="173"/>
-      <c r="AC43" s="173"/>
-      <c r="AD43" s="173"/>
-      <c r="AE43" s="173"/>
-      <c r="AF43" s="173"/>
-      <c r="AG43" s="173"/>
-      <c r="AH43" s="173"/>
+      <c r="H43" s="177"/>
+      <c r="I43" s="177"/>
+      <c r="J43" s="177"/>
+      <c r="K43" s="177"/>
+      <c r="L43" s="177"/>
+      <c r="M43" s="177"/>
+      <c r="N43" s="177"/>
+      <c r="O43" s="177"/>
+      <c r="P43" s="177"/>
+      <c r="Q43" s="177"/>
+      <c r="R43" s="177"/>
+      <c r="S43" s="177"/>
+      <c r="T43" s="177"/>
+      <c r="U43" s="177"/>
+      <c r="V43" s="177"/>
+      <c r="W43" s="177"/>
+      <c r="X43" s="177"/>
+      <c r="Y43" s="177"/>
+      <c r="Z43" s="177"/>
+      <c r="AA43" s="177"/>
+      <c r="AB43" s="177"/>
+      <c r="AC43" s="177"/>
+      <c r="AD43" s="177"/>
+      <c r="AE43" s="177"/>
+      <c r="AF43" s="177"/>
+      <c r="AG43" s="177"/>
+      <c r="AH43" s="177"/>
       <c r="AI43" s="53"/>
       <c r="AJ43" s="28"/>
       <c r="AK43" s="28"/>
@@ -16975,33 +16990,33 @@
       <c r="E44" s="28"/>
       <c r="F44" s="28"/>
       <c r="G44" s="28"/>
-      <c r="H44" s="173"/>
-      <c r="I44" s="173"/>
-      <c r="J44" s="173"/>
-      <c r="K44" s="173"/>
-      <c r="L44" s="173"/>
-      <c r="M44" s="173"/>
-      <c r="N44" s="173"/>
-      <c r="O44" s="173"/>
-      <c r="P44" s="173"/>
-      <c r="Q44" s="173"/>
-      <c r="R44" s="173"/>
-      <c r="S44" s="173"/>
-      <c r="T44" s="173"/>
-      <c r="U44" s="173"/>
-      <c r="V44" s="173"/>
-      <c r="W44" s="173"/>
-      <c r="X44" s="173"/>
-      <c r="Y44" s="173"/>
-      <c r="Z44" s="173"/>
-      <c r="AA44" s="173"/>
-      <c r="AB44" s="173"/>
-      <c r="AC44" s="173"/>
-      <c r="AD44" s="173"/>
-      <c r="AE44" s="173"/>
-      <c r="AF44" s="173"/>
-      <c r="AG44" s="173"/>
-      <c r="AH44" s="173"/>
+      <c r="H44" s="177"/>
+      <c r="I44" s="177"/>
+      <c r="J44" s="177"/>
+      <c r="K44" s="177"/>
+      <c r="L44" s="177"/>
+      <c r="M44" s="177"/>
+      <c r="N44" s="177"/>
+      <c r="O44" s="177"/>
+      <c r="P44" s="177"/>
+      <c r="Q44" s="177"/>
+      <c r="R44" s="177"/>
+      <c r="S44" s="177"/>
+      <c r="T44" s="177"/>
+      <c r="U44" s="177"/>
+      <c r="V44" s="177"/>
+      <c r="W44" s="177"/>
+      <c r="X44" s="177"/>
+      <c r="Y44" s="177"/>
+      <c r="Z44" s="177"/>
+      <c r="AA44" s="177"/>
+      <c r="AB44" s="177"/>
+      <c r="AC44" s="177"/>
+      <c r="AD44" s="177"/>
+      <c r="AE44" s="177"/>
+      <c r="AF44" s="177"/>
+      <c r="AG44" s="177"/>
+      <c r="AH44" s="177"/>
       <c r="AI44" s="28"/>
       <c r="AJ44" s="28"/>
       <c r="AK44" s="28"/>
@@ -18303,6 +18318,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="AM39:AO40"/>
+    <mergeCell ref="H43:K44"/>
+    <mergeCell ref="L43:O44"/>
+    <mergeCell ref="P43:T44"/>
+    <mergeCell ref="U43:Y44"/>
+    <mergeCell ref="Z43:AD44"/>
+    <mergeCell ref="AE43:AH44"/>
+    <mergeCell ref="A1:F3"/>
+    <mergeCell ref="H39:K40"/>
+    <mergeCell ref="L39:O40"/>
+    <mergeCell ref="P39:S40"/>
+    <mergeCell ref="T39:W40"/>
     <mergeCell ref="AO1:AR1"/>
     <mergeCell ref="AG2:AJ3"/>
     <mergeCell ref="AK2:AN3"/>
@@ -18315,18 +18342,6 @@
     <mergeCell ref="T1:AF1"/>
     <mergeCell ref="AG1:AJ1"/>
     <mergeCell ref="AK1:AN1"/>
-    <mergeCell ref="A1:F3"/>
-    <mergeCell ref="H39:K40"/>
-    <mergeCell ref="L39:O40"/>
-    <mergeCell ref="P39:S40"/>
-    <mergeCell ref="T39:W40"/>
-    <mergeCell ref="AM39:AO40"/>
-    <mergeCell ref="H43:K44"/>
-    <mergeCell ref="L43:O44"/>
-    <mergeCell ref="P43:T44"/>
-    <mergeCell ref="U43:Y44"/>
-    <mergeCell ref="Z43:AD44"/>
-    <mergeCell ref="AE43:AH44"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="80" fitToHeight="0" orientation="landscape"/>
@@ -18337,14 +18352,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AR97"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="AX1" sqref="AX1"/>
     </sheetView>
   </sheetViews>
@@ -18357,170 +18372,170 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" s="1" customFormat="1">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="163" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="165" t="s">
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="125" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="167"/>
-      <c r="L1" s="176" t="s">
+      <c r="H1" s="126"/>
+      <c r="I1" s="126"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="127"/>
+      <c r="L1" s="174" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="176"/>
-      <c r="N1" s="176"/>
-      <c r="O1" s="176"/>
-      <c r="P1" s="176"/>
-      <c r="Q1" s="176"/>
-      <c r="R1" s="176"/>
-      <c r="S1" s="176"/>
-      <c r="T1" s="176" t="s">
+      <c r="M1" s="174"/>
+      <c r="N1" s="174"/>
+      <c r="O1" s="174"/>
+      <c r="P1" s="174"/>
+      <c r="Q1" s="174"/>
+      <c r="R1" s="174"/>
+      <c r="S1" s="174"/>
+      <c r="T1" s="174" t="s">
         <v>71</v>
       </c>
-      <c r="U1" s="176"/>
-      <c r="V1" s="176"/>
-      <c r="W1" s="176"/>
-      <c r="X1" s="176"/>
-      <c r="Y1" s="176"/>
-      <c r="Z1" s="176"/>
-      <c r="AA1" s="176"/>
-      <c r="AB1" s="176"/>
-      <c r="AC1" s="176"/>
-      <c r="AD1" s="176"/>
-      <c r="AE1" s="176"/>
-      <c r="AF1" s="176"/>
-      <c r="AG1" s="165" t="s">
+      <c r="U1" s="174"/>
+      <c r="V1" s="174"/>
+      <c r="W1" s="174"/>
+      <c r="X1" s="174"/>
+      <c r="Y1" s="174"/>
+      <c r="Z1" s="174"/>
+      <c r="AA1" s="174"/>
+      <c r="AB1" s="174"/>
+      <c r="AC1" s="174"/>
+      <c r="AD1" s="174"/>
+      <c r="AE1" s="174"/>
+      <c r="AF1" s="174"/>
+      <c r="AG1" s="125" t="s">
         <v>13</v>
       </c>
-      <c r="AH1" s="166"/>
-      <c r="AI1" s="166"/>
-      <c r="AJ1" s="167"/>
-      <c r="AK1" s="166" t="s">
+      <c r="AH1" s="126"/>
+      <c r="AI1" s="126"/>
+      <c r="AJ1" s="127"/>
+      <c r="AK1" s="126" t="s">
         <v>14</v>
       </c>
-      <c r="AL1" s="166"/>
-      <c r="AM1" s="166"/>
-      <c r="AN1" s="167"/>
-      <c r="AO1" s="165" t="s">
+      <c r="AL1" s="126"/>
+      <c r="AM1" s="126"/>
+      <c r="AN1" s="127"/>
+      <c r="AO1" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="AP1" s="166"/>
-      <c r="AQ1" s="166"/>
-      <c r="AR1" s="167"/>
+      <c r="AP1" s="126"/>
+      <c r="AQ1" s="126"/>
+      <c r="AR1" s="127"/>
     </row>
     <row r="2" spans="1:44" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="143"/>
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="143"/>
-      <c r="G2" s="133" t="str">
+      <c r="A2" s="163"/>
+      <c r="B2" s="163"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="163"/>
+      <c r="F2" s="163"/>
+      <c r="G2" s="157" t="str">
         <f>T2</f>
         <v>Đọc tên</v>
       </c>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="135"/>
-      <c r="L2" s="175" t="str">
+      <c r="H2" s="158"/>
+      <c r="I2" s="158"/>
+      <c r="J2" s="158"/>
+      <c r="K2" s="159"/>
+      <c r="L2" s="173" t="str">
         <f>Cover!C62</f>
         <v>UC_002</v>
       </c>
-      <c r="M2" s="175"/>
-      <c r="N2" s="175"/>
-      <c r="O2" s="175"/>
-      <c r="P2" s="175"/>
-      <c r="Q2" s="175"/>
-      <c r="R2" s="175"/>
-      <c r="S2" s="175"/>
-      <c r="T2" s="175" t="str">
+      <c r="M2" s="173"/>
+      <c r="N2" s="173"/>
+      <c r="O2" s="173"/>
+      <c r="P2" s="173"/>
+      <c r="Q2" s="173"/>
+      <c r="R2" s="173"/>
+      <c r="S2" s="173"/>
+      <c r="T2" s="173" t="str">
         <f>Cover!H62</f>
         <v>Đọc tên</v>
       </c>
-      <c r="U2" s="175"/>
-      <c r="V2" s="175"/>
-      <c r="W2" s="175"/>
-      <c r="X2" s="175"/>
-      <c r="Y2" s="175"/>
-      <c r="Z2" s="175"/>
-      <c r="AA2" s="175"/>
-      <c r="AB2" s="175"/>
-      <c r="AC2" s="175"/>
-      <c r="AD2" s="175"/>
-      <c r="AE2" s="175"/>
-      <c r="AF2" s="175"/>
-      <c r="AG2" s="133" t="s">
+      <c r="U2" s="173"/>
+      <c r="V2" s="173"/>
+      <c r="W2" s="173"/>
+      <c r="X2" s="173"/>
+      <c r="Y2" s="173"/>
+      <c r="Z2" s="173"/>
+      <c r="AA2" s="173"/>
+      <c r="AB2" s="173"/>
+      <c r="AC2" s="173"/>
+      <c r="AD2" s="173"/>
+      <c r="AE2" s="173"/>
+      <c r="AF2" s="173"/>
+      <c r="AG2" s="157" t="s">
         <v>7</v>
       </c>
-      <c r="AH2" s="134"/>
-      <c r="AI2" s="134"/>
-      <c r="AJ2" s="135"/>
-      <c r="AK2" s="139">
+      <c r="AH2" s="158"/>
+      <c r="AI2" s="158"/>
+      <c r="AJ2" s="159"/>
+      <c r="AK2" s="132">
         <f>DATE(2017,2,12)</f>
         <v>42778</v>
       </c>
-      <c r="AL2" s="139"/>
-      <c r="AM2" s="139"/>
-      <c r="AN2" s="140"/>
-      <c r="AO2" s="139"/>
-      <c r="AP2" s="139"/>
-      <c r="AQ2" s="139"/>
-      <c r="AR2" s="140"/>
+      <c r="AL2" s="132"/>
+      <c r="AM2" s="132"/>
+      <c r="AN2" s="133"/>
+      <c r="AO2" s="132"/>
+      <c r="AP2" s="132"/>
+      <c r="AQ2" s="132"/>
+      <c r="AR2" s="133"/>
     </row>
     <row r="3" spans="1:44" s="1" customFormat="1">
-      <c r="A3" s="143"/>
-      <c r="B3" s="143"/>
-      <c r="C3" s="143"/>
-      <c r="D3" s="143"/>
-      <c r="E3" s="143"/>
-      <c r="F3" s="143"/>
-      <c r="G3" s="136"/>
-      <c r="H3" s="137"/>
-      <c r="I3" s="137"/>
-      <c r="J3" s="137"/>
-      <c r="K3" s="138"/>
-      <c r="L3" s="175"/>
-      <c r="M3" s="175"/>
-      <c r="N3" s="175"/>
-      <c r="O3" s="175"/>
-      <c r="P3" s="175"/>
-      <c r="Q3" s="175"/>
-      <c r="R3" s="175"/>
-      <c r="S3" s="175"/>
-      <c r="T3" s="175"/>
-      <c r="U3" s="175"/>
-      <c r="V3" s="175"/>
-      <c r="W3" s="175"/>
-      <c r="X3" s="175"/>
-      <c r="Y3" s="175"/>
-      <c r="Z3" s="175"/>
-      <c r="AA3" s="175"/>
-      <c r="AB3" s="175"/>
-      <c r="AC3" s="175"/>
-      <c r="AD3" s="175"/>
-      <c r="AE3" s="175"/>
-      <c r="AF3" s="175"/>
-      <c r="AG3" s="136"/>
-      <c r="AH3" s="137"/>
-      <c r="AI3" s="137"/>
-      <c r="AJ3" s="138"/>
-      <c r="AK3" s="141"/>
-      <c r="AL3" s="141"/>
-      <c r="AM3" s="141"/>
-      <c r="AN3" s="142"/>
-      <c r="AO3" s="141"/>
-      <c r="AP3" s="141"/>
-      <c r="AQ3" s="141"/>
-      <c r="AR3" s="142"/>
+      <c r="A3" s="163"/>
+      <c r="B3" s="163"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="163"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="161"/>
+      <c r="K3" s="162"/>
+      <c r="L3" s="173"/>
+      <c r="M3" s="173"/>
+      <c r="N3" s="173"/>
+      <c r="O3" s="173"/>
+      <c r="P3" s="173"/>
+      <c r="Q3" s="173"/>
+      <c r="R3" s="173"/>
+      <c r="S3" s="173"/>
+      <c r="T3" s="173"/>
+      <c r="U3" s="173"/>
+      <c r="V3" s="173"/>
+      <c r="W3" s="173"/>
+      <c r="X3" s="173"/>
+      <c r="Y3" s="173"/>
+      <c r="Z3" s="173"/>
+      <c r="AA3" s="173"/>
+      <c r="AB3" s="173"/>
+      <c r="AC3" s="173"/>
+      <c r="AD3" s="173"/>
+      <c r="AE3" s="173"/>
+      <c r="AF3" s="173"/>
+      <c r="AG3" s="160"/>
+      <c r="AH3" s="161"/>
+      <c r="AI3" s="161"/>
+      <c r="AJ3" s="162"/>
+      <c r="AK3" s="134"/>
+      <c r="AL3" s="134"/>
+      <c r="AM3" s="134"/>
+      <c r="AN3" s="135"/>
+      <c r="AO3" s="134"/>
+      <c r="AP3" s="134"/>
+      <c r="AQ3" s="134"/>
+      <c r="AR3" s="135"/>
     </row>
     <row r="4" spans="1:44">
       <c r="A4" s="4"/>
@@ -19894,7 +19909,7 @@
     </row>
     <row r="33" spans="1:44">
       <c r="A33" s="4"/>
-      <c r="B33" s="181" t="s">
+      <c r="B33" s="124" t="s">
         <v>106</v>
       </c>
       <c r="C33" s="5"/>
@@ -20494,7 +20509,7 @@
     </row>
     <row r="46" spans="1:44">
       <c r="A46" s="4"/>
-      <c r="B46" s="181" t="s">
+      <c r="B46" s="124" t="s">
         <v>107</v>
       </c>
       <c r="C46" s="5"/>
@@ -22911,176 +22926,174 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AR92"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:W38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="3"/>
-    <col min="2" max="3" width="3.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="3.42578125" style="3"/>
+    <col min="1" max="44" width="3.28515625" style="3" customWidth="1"/>
+    <col min="45" max="16384" width="3.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" s="1" customFormat="1">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="163" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="165" t="s">
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="125" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="167"/>
-      <c r="L1" s="176" t="s">
+      <c r="H1" s="126"/>
+      <c r="I1" s="126"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="127"/>
+      <c r="L1" s="174" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="176"/>
-      <c r="N1" s="176"/>
-      <c r="O1" s="176"/>
-      <c r="P1" s="176"/>
-      <c r="Q1" s="176"/>
-      <c r="R1" s="176"/>
-      <c r="S1" s="176"/>
-      <c r="T1" s="176" t="s">
+      <c r="M1" s="174"/>
+      <c r="N1" s="174"/>
+      <c r="O1" s="174"/>
+      <c r="P1" s="174"/>
+      <c r="Q1" s="174"/>
+      <c r="R1" s="174"/>
+      <c r="S1" s="174"/>
+      <c r="T1" s="174" t="s">
         <v>71</v>
       </c>
-      <c r="U1" s="176"/>
-      <c r="V1" s="176"/>
-      <c r="W1" s="176"/>
-      <c r="X1" s="176"/>
-      <c r="Y1" s="176"/>
-      <c r="Z1" s="176"/>
-      <c r="AA1" s="176"/>
-      <c r="AB1" s="176"/>
-      <c r="AC1" s="176"/>
-      <c r="AD1" s="176"/>
-      <c r="AE1" s="176"/>
-      <c r="AF1" s="176"/>
-      <c r="AG1" s="165" t="s">
+      <c r="U1" s="174"/>
+      <c r="V1" s="174"/>
+      <c r="W1" s="174"/>
+      <c r="X1" s="174"/>
+      <c r="Y1" s="174"/>
+      <c r="Z1" s="174"/>
+      <c r="AA1" s="174"/>
+      <c r="AB1" s="174"/>
+      <c r="AC1" s="174"/>
+      <c r="AD1" s="174"/>
+      <c r="AE1" s="174"/>
+      <c r="AF1" s="174"/>
+      <c r="AG1" s="125" t="s">
         <v>13</v>
       </c>
-      <c r="AH1" s="166"/>
-      <c r="AI1" s="166"/>
-      <c r="AJ1" s="167"/>
-      <c r="AK1" s="166" t="s">
+      <c r="AH1" s="126"/>
+      <c r="AI1" s="126"/>
+      <c r="AJ1" s="127"/>
+      <c r="AK1" s="126" t="s">
         <v>14</v>
       </c>
-      <c r="AL1" s="166"/>
-      <c r="AM1" s="166"/>
-      <c r="AN1" s="167"/>
-      <c r="AO1" s="165" t="s">
+      <c r="AL1" s="126"/>
+      <c r="AM1" s="126"/>
+      <c r="AN1" s="127"/>
+      <c r="AO1" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="AP1" s="166"/>
-      <c r="AQ1" s="166"/>
-      <c r="AR1" s="167"/>
+      <c r="AP1" s="126"/>
+      <c r="AQ1" s="126"/>
+      <c r="AR1" s="127"/>
     </row>
     <row r="2" spans="1:44" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="143"/>
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="143"/>
-      <c r="G2" s="133"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="135"/>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175"/>
-      <c r="N2" s="175"/>
-      <c r="O2" s="175"/>
-      <c r="P2" s="175"/>
-      <c r="Q2" s="175"/>
-      <c r="R2" s="175"/>
-      <c r="S2" s="175"/>
-      <c r="T2" s="175"/>
-      <c r="U2" s="175"/>
-      <c r="V2" s="175"/>
-      <c r="W2" s="175"/>
-      <c r="X2" s="175"/>
-      <c r="Y2" s="175"/>
-      <c r="Z2" s="175"/>
-      <c r="AA2" s="175"/>
-      <c r="AB2" s="175"/>
-      <c r="AC2" s="175"/>
-      <c r="AD2" s="175"/>
-      <c r="AE2" s="175"/>
-      <c r="AF2" s="175"/>
-      <c r="AG2" s="133"/>
-      <c r="AH2" s="134"/>
-      <c r="AI2" s="134"/>
-      <c r="AJ2" s="135"/>
-      <c r="AK2" s="177"/>
-      <c r="AL2" s="177"/>
-      <c r="AM2" s="177"/>
-      <c r="AN2" s="178"/>
-      <c r="AO2" s="177"/>
-      <c r="AP2" s="177"/>
-      <c r="AQ2" s="177"/>
-      <c r="AR2" s="178"/>
+      <c r="A2" s="163"/>
+      <c r="B2" s="163"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="163"/>
+      <c r="F2" s="163"/>
+      <c r="G2" s="157"/>
+      <c r="H2" s="158"/>
+      <c r="I2" s="158"/>
+      <c r="J2" s="158"/>
+      <c r="K2" s="159"/>
+      <c r="L2" s="173"/>
+      <c r="M2" s="173"/>
+      <c r="N2" s="173"/>
+      <c r="O2" s="173"/>
+      <c r="P2" s="173"/>
+      <c r="Q2" s="173"/>
+      <c r="R2" s="173"/>
+      <c r="S2" s="173"/>
+      <c r="T2" s="173"/>
+      <c r="U2" s="173"/>
+      <c r="V2" s="173"/>
+      <c r="W2" s="173"/>
+      <c r="X2" s="173"/>
+      <c r="Y2" s="173"/>
+      <c r="Z2" s="173"/>
+      <c r="AA2" s="173"/>
+      <c r="AB2" s="173"/>
+      <c r="AC2" s="173"/>
+      <c r="AD2" s="173"/>
+      <c r="AE2" s="173"/>
+      <c r="AF2" s="173"/>
+      <c r="AG2" s="157"/>
+      <c r="AH2" s="158"/>
+      <c r="AI2" s="158"/>
+      <c r="AJ2" s="159"/>
+      <c r="AK2" s="178"/>
+      <c r="AL2" s="178"/>
+      <c r="AM2" s="178"/>
+      <c r="AN2" s="179"/>
+      <c r="AO2" s="178"/>
+      <c r="AP2" s="178"/>
+      <c r="AQ2" s="178"/>
+      <c r="AR2" s="179"/>
     </row>
     <row r="3" spans="1:44" s="1" customFormat="1">
-      <c r="A3" s="143"/>
-      <c r="B3" s="143"/>
-      <c r="C3" s="143"/>
-      <c r="D3" s="143"/>
-      <c r="E3" s="143"/>
-      <c r="F3" s="143"/>
-      <c r="G3" s="136"/>
-      <c r="H3" s="137"/>
-      <c r="I3" s="137"/>
-      <c r="J3" s="137"/>
-      <c r="K3" s="138"/>
-      <c r="L3" s="175"/>
-      <c r="M3" s="175"/>
-      <c r="N3" s="175"/>
-      <c r="O3" s="175"/>
-      <c r="P3" s="175"/>
-      <c r="Q3" s="175"/>
-      <c r="R3" s="175"/>
-      <c r="S3" s="175"/>
-      <c r="T3" s="175"/>
-      <c r="U3" s="175"/>
-      <c r="V3" s="175"/>
-      <c r="W3" s="175"/>
-      <c r="X3" s="175"/>
-      <c r="Y3" s="175"/>
-      <c r="Z3" s="175"/>
-      <c r="AA3" s="175"/>
-      <c r="AB3" s="175"/>
-      <c r="AC3" s="175"/>
-      <c r="AD3" s="175"/>
-      <c r="AE3" s="175"/>
-      <c r="AF3" s="175"/>
-      <c r="AG3" s="136"/>
-      <c r="AH3" s="137"/>
-      <c r="AI3" s="137"/>
-      <c r="AJ3" s="138"/>
-      <c r="AK3" s="179"/>
-      <c r="AL3" s="179"/>
-      <c r="AM3" s="179"/>
-      <c r="AN3" s="180"/>
-      <c r="AO3" s="179"/>
-      <c r="AP3" s="179"/>
-      <c r="AQ3" s="179"/>
-      <c r="AR3" s="180"/>
+      <c r="A3" s="163"/>
+      <c r="B3" s="163"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="163"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="161"/>
+      <c r="K3" s="162"/>
+      <c r="L3" s="173"/>
+      <c r="M3" s="173"/>
+      <c r="N3" s="173"/>
+      <c r="O3" s="173"/>
+      <c r="P3" s="173"/>
+      <c r="Q3" s="173"/>
+      <c r="R3" s="173"/>
+      <c r="S3" s="173"/>
+      <c r="T3" s="173"/>
+      <c r="U3" s="173"/>
+      <c r="V3" s="173"/>
+      <c r="W3" s="173"/>
+      <c r="X3" s="173"/>
+      <c r="Y3" s="173"/>
+      <c r="Z3" s="173"/>
+      <c r="AA3" s="173"/>
+      <c r="AB3" s="173"/>
+      <c r="AC3" s="173"/>
+      <c r="AD3" s="173"/>
+      <c r="AE3" s="173"/>
+      <c r="AF3" s="173"/>
+      <c r="AG3" s="160"/>
+      <c r="AH3" s="161"/>
+      <c r="AI3" s="161"/>
+      <c r="AJ3" s="162"/>
+      <c r="AK3" s="180"/>
+      <c r="AL3" s="180"/>
+      <c r="AM3" s="180"/>
+      <c r="AN3" s="181"/>
+      <c r="AO3" s="180"/>
+      <c r="AP3" s="180"/>
+      <c r="AQ3" s="180"/>
+      <c r="AR3" s="181"/>
     </row>
     <row r="4" spans="1:44">
       <c r="A4" s="4"/>

</xml_diff>

<commit_message>
spec UC doc ten
</commit_message>
<xml_diff>
--- a/doc/requirement/RFID_UseCase_v1.0.xlsx
+++ b/doc/requirement/RFID_UseCase_v1.0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="18600" windowHeight="8850" tabRatio="922" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18600" windowHeight="8850" tabRatio="922" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ChangeHistory" sheetId="1" r:id="rId1"/>
@@ -5373,75 +5373,6 @@
     <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="1882" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="3633" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="64" fillId="2" borderId="0" xfId="3633" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="6" borderId="1" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="6" borderId="2" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="6" borderId="3" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="6" borderId="9" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="3" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="9" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="3" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="9" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -5487,6 +5418,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5517,19 +5460,76 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="3" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="9" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="3" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="9" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="6" borderId="1" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="6" borderId="2" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="6" borderId="3" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="6" borderId="9" xfId="3633" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="174" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -10428,156 +10428,156 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="144" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="125" t="s">
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
+      <c r="G1" s="166" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="126"/>
-      <c r="N1" s="126"/>
-      <c r="O1" s="126"/>
-      <c r="P1" s="126"/>
-      <c r="Q1" s="126"/>
-      <c r="R1" s="126"/>
-      <c r="S1" s="126"/>
-      <c r="T1" s="126"/>
-      <c r="U1" s="126"/>
-      <c r="V1" s="126"/>
-      <c r="W1" s="126"/>
-      <c r="X1" s="126"/>
-      <c r="Y1" s="126"/>
-      <c r="Z1" s="126"/>
-      <c r="AA1" s="126"/>
-      <c r="AB1" s="126"/>
-      <c r="AC1" s="126"/>
-      <c r="AD1" s="127"/>
-      <c r="AE1" s="125" t="s">
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
+      <c r="P1" s="167"/>
+      <c r="Q1" s="167"/>
+      <c r="R1" s="167"/>
+      <c r="S1" s="167"/>
+      <c r="T1" s="167"/>
+      <c r="U1" s="167"/>
+      <c r="V1" s="167"/>
+      <c r="W1" s="167"/>
+      <c r="X1" s="167"/>
+      <c r="Y1" s="167"/>
+      <c r="Z1" s="167"/>
+      <c r="AA1" s="167"/>
+      <c r="AB1" s="167"/>
+      <c r="AC1" s="167"/>
+      <c r="AD1" s="168"/>
+      <c r="AE1" s="166" t="s">
         <v>13</v>
       </c>
-      <c r="AF1" s="126"/>
-      <c r="AG1" s="126"/>
-      <c r="AH1" s="127"/>
-      <c r="AI1" s="126" t="s">
+      <c r="AF1" s="167"/>
+      <c r="AG1" s="167"/>
+      <c r="AH1" s="168"/>
+      <c r="AI1" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="126"/>
-      <c r="AK1" s="126"/>
-      <c r="AL1" s="127"/>
-      <c r="AM1" s="125" t="s">
+      <c r="AJ1" s="167"/>
+      <c r="AK1" s="167"/>
+      <c r="AL1" s="168"/>
+      <c r="AM1" s="166" t="s">
         <v>15</v>
       </c>
-      <c r="AN1" s="126"/>
-      <c r="AO1" s="126"/>
-      <c r="AP1" s="127"/>
+      <c r="AN1" s="167"/>
+      <c r="AO1" s="167"/>
+      <c r="AP1" s="168"/>
     </row>
     <row r="2" spans="1:42" ht="15" customHeight="1">
-      <c r="A2" s="163"/>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="164" t="s">
+      <c r="A2" s="144"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="145" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="165"/>
-      <c r="I2" s="165"/>
-      <c r="J2" s="165"/>
-      <c r="K2" s="165"/>
-      <c r="L2" s="165"/>
-      <c r="M2" s="165"/>
-      <c r="N2" s="165"/>
-      <c r="O2" s="165"/>
-      <c r="P2" s="165"/>
-      <c r="Q2" s="165"/>
-      <c r="R2" s="165"/>
-      <c r="S2" s="165"/>
-      <c r="T2" s="165"/>
-      <c r="U2" s="165"/>
-      <c r="V2" s="165"/>
-      <c r="W2" s="165"/>
-      <c r="X2" s="165"/>
-      <c r="Y2" s="165"/>
-      <c r="Z2" s="165"/>
-      <c r="AA2" s="165"/>
-      <c r="AB2" s="165"/>
-      <c r="AC2" s="165"/>
-      <c r="AD2" s="166"/>
-      <c r="AE2" s="157" t="s">
+      <c r="H2" s="146"/>
+      <c r="I2" s="146"/>
+      <c r="J2" s="146"/>
+      <c r="K2" s="146"/>
+      <c r="L2" s="146"/>
+      <c r="M2" s="146"/>
+      <c r="N2" s="146"/>
+      <c r="O2" s="146"/>
+      <c r="P2" s="146"/>
+      <c r="Q2" s="146"/>
+      <c r="R2" s="146"/>
+      <c r="S2" s="146"/>
+      <c r="T2" s="146"/>
+      <c r="U2" s="146"/>
+      <c r="V2" s="146"/>
+      <c r="W2" s="146"/>
+      <c r="X2" s="146"/>
+      <c r="Y2" s="146"/>
+      <c r="Z2" s="146"/>
+      <c r="AA2" s="146"/>
+      <c r="AB2" s="146"/>
+      <c r="AC2" s="146"/>
+      <c r="AD2" s="147"/>
+      <c r="AE2" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="AF2" s="158"/>
-      <c r="AG2" s="158"/>
-      <c r="AH2" s="159"/>
-      <c r="AI2" s="132">
+      <c r="AF2" s="135"/>
+      <c r="AG2" s="135"/>
+      <c r="AH2" s="136"/>
+      <c r="AI2" s="140">
         <f>DATE(2017,1,30)</f>
         <v>42765</v>
       </c>
-      <c r="AJ2" s="132"/>
-      <c r="AK2" s="132"/>
-      <c r="AL2" s="133"/>
-      <c r="AM2" s="132">
+      <c r="AJ2" s="140"/>
+      <c r="AK2" s="140"/>
+      <c r="AL2" s="141"/>
+      <c r="AM2" s="140">
         <f>DATE(2017,2,2)</f>
         <v>42768</v>
       </c>
-      <c r="AN2" s="132"/>
-      <c r="AO2" s="132"/>
-      <c r="AP2" s="133"/>
+      <c r="AN2" s="140"/>
+      <c r="AO2" s="140"/>
+      <c r="AP2" s="141"/>
     </row>
     <row r="3" spans="1:42">
-      <c r="A3" s="163"/>
-      <c r="B3" s="163"/>
-      <c r="C3" s="163"/>
-      <c r="D3" s="163"/>
-      <c r="E3" s="163"/>
-      <c r="F3" s="163"/>
-      <c r="G3" s="167"/>
-      <c r="H3" s="168"/>
-      <c r="I3" s="168"/>
-      <c r="J3" s="168"/>
-      <c r="K3" s="168"/>
-      <c r="L3" s="168"/>
-      <c r="M3" s="168"/>
-      <c r="N3" s="168"/>
-      <c r="O3" s="168"/>
-      <c r="P3" s="168"/>
-      <c r="Q3" s="168"/>
-      <c r="R3" s="168"/>
-      <c r="S3" s="168"/>
-      <c r="T3" s="168"/>
-      <c r="U3" s="168"/>
-      <c r="V3" s="168"/>
-      <c r="W3" s="168"/>
-      <c r="X3" s="168"/>
-      <c r="Y3" s="168"/>
-      <c r="Z3" s="168"/>
-      <c r="AA3" s="168"/>
-      <c r="AB3" s="168"/>
-      <c r="AC3" s="168"/>
-      <c r="AD3" s="169"/>
-      <c r="AE3" s="160"/>
-      <c r="AF3" s="161"/>
-      <c r="AG3" s="161"/>
-      <c r="AH3" s="162"/>
-      <c r="AI3" s="134"/>
-      <c r="AJ3" s="134"/>
-      <c r="AK3" s="134"/>
-      <c r="AL3" s="135"/>
-      <c r="AM3" s="134"/>
-      <c r="AN3" s="134"/>
-      <c r="AO3" s="134"/>
-      <c r="AP3" s="135"/>
+      <c r="A3" s="144"/>
+      <c r="B3" s="144"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="148"/>
+      <c r="H3" s="149"/>
+      <c r="I3" s="149"/>
+      <c r="J3" s="149"/>
+      <c r="K3" s="149"/>
+      <c r="L3" s="149"/>
+      <c r="M3" s="149"/>
+      <c r="N3" s="149"/>
+      <c r="O3" s="149"/>
+      <c r="P3" s="149"/>
+      <c r="Q3" s="149"/>
+      <c r="R3" s="149"/>
+      <c r="S3" s="149"/>
+      <c r="T3" s="149"/>
+      <c r="U3" s="149"/>
+      <c r="V3" s="149"/>
+      <c r="W3" s="149"/>
+      <c r="X3" s="149"/>
+      <c r="Y3" s="149"/>
+      <c r="Z3" s="149"/>
+      <c r="AA3" s="149"/>
+      <c r="AB3" s="149"/>
+      <c r="AC3" s="149"/>
+      <c r="AD3" s="150"/>
+      <c r="AE3" s="137"/>
+      <c r="AF3" s="138"/>
+      <c r="AG3" s="138"/>
+      <c r="AH3" s="139"/>
+      <c r="AI3" s="142"/>
+      <c r="AJ3" s="142"/>
+      <c r="AK3" s="142"/>
+      <c r="AL3" s="143"/>
+      <c r="AM3" s="142"/>
+      <c r="AN3" s="142"/>
+      <c r="AO3" s="142"/>
+      <c r="AP3" s="143"/>
     </row>
     <row r="4" spans="1:42">
       <c r="A4" s="54"/>
@@ -10715,181 +10715,181 @@
     </row>
     <row r="7" spans="1:42" ht="12.75" customHeight="1">
       <c r="A7" s="54"/>
-      <c r="B7" s="170" t="s">
+      <c r="B7" s="151" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="171"/>
-      <c r="D7" s="171"/>
-      <c r="E7" s="171"/>
-      <c r="F7" s="171"/>
-      <c r="G7" s="171"/>
-      <c r="H7" s="171"/>
-      <c r="I7" s="171"/>
-      <c r="J7" s="171"/>
-      <c r="K7" s="171"/>
-      <c r="L7" s="171"/>
-      <c r="M7" s="171"/>
-      <c r="N7" s="171"/>
-      <c r="O7" s="171"/>
-      <c r="P7" s="171"/>
-      <c r="Q7" s="171"/>
-      <c r="R7" s="171"/>
-      <c r="S7" s="171"/>
-      <c r="T7" s="171"/>
-      <c r="U7" s="171"/>
-      <c r="V7" s="171"/>
-      <c r="W7" s="171"/>
-      <c r="X7" s="171"/>
-      <c r="Y7" s="171"/>
-      <c r="Z7" s="171"/>
-      <c r="AA7" s="171"/>
-      <c r="AB7" s="171"/>
-      <c r="AC7" s="171"/>
-      <c r="AD7" s="171"/>
-      <c r="AE7" s="171"/>
-      <c r="AF7" s="171"/>
-      <c r="AG7" s="171"/>
-      <c r="AH7" s="171"/>
-      <c r="AI7" s="171"/>
-      <c r="AJ7" s="171"/>
-      <c r="AK7" s="171"/>
-      <c r="AL7" s="171"/>
-      <c r="AM7" s="171"/>
-      <c r="AN7" s="171"/>
-      <c r="AO7" s="171"/>
-      <c r="AP7" s="172"/>
+      <c r="C7" s="152"/>
+      <c r="D7" s="152"/>
+      <c r="E7" s="152"/>
+      <c r="F7" s="152"/>
+      <c r="G7" s="152"/>
+      <c r="H7" s="152"/>
+      <c r="I7" s="152"/>
+      <c r="J7" s="152"/>
+      <c r="K7" s="152"/>
+      <c r="L7" s="152"/>
+      <c r="M7" s="152"/>
+      <c r="N7" s="152"/>
+      <c r="O7" s="152"/>
+      <c r="P7" s="152"/>
+      <c r="Q7" s="152"/>
+      <c r="R7" s="152"/>
+      <c r="S7" s="152"/>
+      <c r="T7" s="152"/>
+      <c r="U7" s="152"/>
+      <c r="V7" s="152"/>
+      <c r="W7" s="152"/>
+      <c r="X7" s="152"/>
+      <c r="Y7" s="152"/>
+      <c r="Z7" s="152"/>
+      <c r="AA7" s="152"/>
+      <c r="AB7" s="152"/>
+      <c r="AC7" s="152"/>
+      <c r="AD7" s="152"/>
+      <c r="AE7" s="152"/>
+      <c r="AF7" s="152"/>
+      <c r="AG7" s="152"/>
+      <c r="AH7" s="152"/>
+      <c r="AI7" s="152"/>
+      <c r="AJ7" s="152"/>
+      <c r="AK7" s="152"/>
+      <c r="AL7" s="152"/>
+      <c r="AM7" s="152"/>
+      <c r="AN7" s="152"/>
+      <c r="AO7" s="152"/>
+      <c r="AP7" s="153"/>
     </row>
     <row r="8" spans="1:42" ht="12.75" customHeight="1">
       <c r="A8" s="54"/>
-      <c r="B8" s="171"/>
-      <c r="C8" s="171"/>
-      <c r="D8" s="171"/>
-      <c r="E8" s="171"/>
-      <c r="F8" s="171"/>
-      <c r="G8" s="171"/>
-      <c r="H8" s="171"/>
-      <c r="I8" s="171"/>
-      <c r="J8" s="171"/>
-      <c r="K8" s="171"/>
-      <c r="L8" s="171"/>
-      <c r="M8" s="171"/>
-      <c r="N8" s="171"/>
-      <c r="O8" s="171"/>
-      <c r="P8" s="171"/>
-      <c r="Q8" s="171"/>
-      <c r="R8" s="171"/>
-      <c r="S8" s="171"/>
-      <c r="T8" s="171"/>
-      <c r="U8" s="171"/>
-      <c r="V8" s="171"/>
-      <c r="W8" s="171"/>
-      <c r="X8" s="171"/>
-      <c r="Y8" s="171"/>
-      <c r="Z8" s="171"/>
-      <c r="AA8" s="171"/>
-      <c r="AB8" s="171"/>
-      <c r="AC8" s="171"/>
-      <c r="AD8" s="171"/>
-      <c r="AE8" s="171"/>
-      <c r="AF8" s="171"/>
-      <c r="AG8" s="171"/>
-      <c r="AH8" s="171"/>
-      <c r="AI8" s="171"/>
-      <c r="AJ8" s="171"/>
-      <c r="AK8" s="171"/>
-      <c r="AL8" s="171"/>
-      <c r="AM8" s="171"/>
-      <c r="AN8" s="171"/>
-      <c r="AO8" s="171"/>
-      <c r="AP8" s="172"/>
+      <c r="B8" s="152"/>
+      <c r="C8" s="152"/>
+      <c r="D8" s="152"/>
+      <c r="E8" s="152"/>
+      <c r="F8" s="152"/>
+      <c r="G8" s="152"/>
+      <c r="H8" s="152"/>
+      <c r="I8" s="152"/>
+      <c r="J8" s="152"/>
+      <c r="K8" s="152"/>
+      <c r="L8" s="152"/>
+      <c r="M8" s="152"/>
+      <c r="N8" s="152"/>
+      <c r="O8" s="152"/>
+      <c r="P8" s="152"/>
+      <c r="Q8" s="152"/>
+      <c r="R8" s="152"/>
+      <c r="S8" s="152"/>
+      <c r="T8" s="152"/>
+      <c r="U8" s="152"/>
+      <c r="V8" s="152"/>
+      <c r="W8" s="152"/>
+      <c r="X8" s="152"/>
+      <c r="Y8" s="152"/>
+      <c r="Z8" s="152"/>
+      <c r="AA8" s="152"/>
+      <c r="AB8" s="152"/>
+      <c r="AC8" s="152"/>
+      <c r="AD8" s="152"/>
+      <c r="AE8" s="152"/>
+      <c r="AF8" s="152"/>
+      <c r="AG8" s="152"/>
+      <c r="AH8" s="152"/>
+      <c r="AI8" s="152"/>
+      <c r="AJ8" s="152"/>
+      <c r="AK8" s="152"/>
+      <c r="AL8" s="152"/>
+      <c r="AM8" s="152"/>
+      <c r="AN8" s="152"/>
+      <c r="AO8" s="152"/>
+      <c r="AP8" s="153"/>
     </row>
     <row r="9" spans="1:42" ht="12.75" customHeight="1">
       <c r="A9" s="54"/>
-      <c r="B9" s="171"/>
-      <c r="C9" s="171"/>
-      <c r="D9" s="171"/>
-      <c r="E9" s="171"/>
-      <c r="F9" s="171"/>
-      <c r="G9" s="171"/>
-      <c r="H9" s="171"/>
-      <c r="I9" s="171"/>
-      <c r="J9" s="171"/>
-      <c r="K9" s="171"/>
-      <c r="L9" s="171"/>
-      <c r="M9" s="171"/>
-      <c r="N9" s="171"/>
-      <c r="O9" s="171"/>
-      <c r="P9" s="171"/>
-      <c r="Q9" s="171"/>
-      <c r="R9" s="171"/>
-      <c r="S9" s="171"/>
-      <c r="T9" s="171"/>
-      <c r="U9" s="171"/>
-      <c r="V9" s="171"/>
-      <c r="W9" s="171"/>
-      <c r="X9" s="171"/>
-      <c r="Y9" s="171"/>
-      <c r="Z9" s="171"/>
-      <c r="AA9" s="171"/>
-      <c r="AB9" s="171"/>
-      <c r="AC9" s="171"/>
-      <c r="AD9" s="171"/>
-      <c r="AE9" s="171"/>
-      <c r="AF9" s="171"/>
-      <c r="AG9" s="171"/>
-      <c r="AH9" s="171"/>
-      <c r="AI9" s="171"/>
-      <c r="AJ9" s="171"/>
-      <c r="AK9" s="171"/>
-      <c r="AL9" s="171"/>
-      <c r="AM9" s="171"/>
-      <c r="AN9" s="171"/>
-      <c r="AO9" s="171"/>
-      <c r="AP9" s="172"/>
+      <c r="B9" s="152"/>
+      <c r="C9" s="152"/>
+      <c r="D9" s="152"/>
+      <c r="E9" s="152"/>
+      <c r="F9" s="152"/>
+      <c r="G9" s="152"/>
+      <c r="H9" s="152"/>
+      <c r="I9" s="152"/>
+      <c r="J9" s="152"/>
+      <c r="K9" s="152"/>
+      <c r="L9" s="152"/>
+      <c r="M9" s="152"/>
+      <c r="N9" s="152"/>
+      <c r="O9" s="152"/>
+      <c r="P9" s="152"/>
+      <c r="Q9" s="152"/>
+      <c r="R9" s="152"/>
+      <c r="S9" s="152"/>
+      <c r="T9" s="152"/>
+      <c r="U9" s="152"/>
+      <c r="V9" s="152"/>
+      <c r="W9" s="152"/>
+      <c r="X9" s="152"/>
+      <c r="Y9" s="152"/>
+      <c r="Z9" s="152"/>
+      <c r="AA9" s="152"/>
+      <c r="AB9" s="152"/>
+      <c r="AC9" s="152"/>
+      <c r="AD9" s="152"/>
+      <c r="AE9" s="152"/>
+      <c r="AF9" s="152"/>
+      <c r="AG9" s="152"/>
+      <c r="AH9" s="152"/>
+      <c r="AI9" s="152"/>
+      <c r="AJ9" s="152"/>
+      <c r="AK9" s="152"/>
+      <c r="AL9" s="152"/>
+      <c r="AM9" s="152"/>
+      <c r="AN9" s="152"/>
+      <c r="AO9" s="152"/>
+      <c r="AP9" s="153"/>
     </row>
     <row r="10" spans="1:42" ht="12.75" customHeight="1">
       <c r="A10" s="54"/>
-      <c r="B10" s="171"/>
-      <c r="C10" s="171"/>
-      <c r="D10" s="171"/>
-      <c r="E10" s="171"/>
-      <c r="F10" s="171"/>
-      <c r="G10" s="171"/>
-      <c r="H10" s="171"/>
-      <c r="I10" s="171"/>
-      <c r="J10" s="171"/>
-      <c r="K10" s="171"/>
-      <c r="L10" s="171"/>
-      <c r="M10" s="171"/>
-      <c r="N10" s="171"/>
-      <c r="O10" s="171"/>
-      <c r="P10" s="171"/>
-      <c r="Q10" s="171"/>
-      <c r="R10" s="171"/>
-      <c r="S10" s="171"/>
-      <c r="T10" s="171"/>
-      <c r="U10" s="171"/>
-      <c r="V10" s="171"/>
-      <c r="W10" s="171"/>
-      <c r="X10" s="171"/>
-      <c r="Y10" s="171"/>
-      <c r="Z10" s="171"/>
-      <c r="AA10" s="171"/>
-      <c r="AB10" s="171"/>
-      <c r="AC10" s="171"/>
-      <c r="AD10" s="171"/>
-      <c r="AE10" s="171"/>
-      <c r="AF10" s="171"/>
-      <c r="AG10" s="171"/>
-      <c r="AH10" s="171"/>
-      <c r="AI10" s="171"/>
-      <c r="AJ10" s="171"/>
-      <c r="AK10" s="171"/>
-      <c r="AL10" s="171"/>
-      <c r="AM10" s="171"/>
-      <c r="AN10" s="171"/>
-      <c r="AO10" s="171"/>
-      <c r="AP10" s="172"/>
+      <c r="B10" s="152"/>
+      <c r="C10" s="152"/>
+      <c r="D10" s="152"/>
+      <c r="E10" s="152"/>
+      <c r="F10" s="152"/>
+      <c r="G10" s="152"/>
+      <c r="H10" s="152"/>
+      <c r="I10" s="152"/>
+      <c r="J10" s="152"/>
+      <c r="K10" s="152"/>
+      <c r="L10" s="152"/>
+      <c r="M10" s="152"/>
+      <c r="N10" s="152"/>
+      <c r="O10" s="152"/>
+      <c r="P10" s="152"/>
+      <c r="Q10" s="152"/>
+      <c r="R10" s="152"/>
+      <c r="S10" s="152"/>
+      <c r="T10" s="152"/>
+      <c r="U10" s="152"/>
+      <c r="V10" s="152"/>
+      <c r="W10" s="152"/>
+      <c r="X10" s="152"/>
+      <c r="Y10" s="152"/>
+      <c r="Z10" s="152"/>
+      <c r="AA10" s="152"/>
+      <c r="AB10" s="152"/>
+      <c r="AC10" s="152"/>
+      <c r="AD10" s="152"/>
+      <c r="AE10" s="152"/>
+      <c r="AF10" s="152"/>
+      <c r="AG10" s="152"/>
+      <c r="AH10" s="152"/>
+      <c r="AI10" s="152"/>
+      <c r="AJ10" s="152"/>
+      <c r="AK10" s="152"/>
+      <c r="AL10" s="152"/>
+      <c r="AM10" s="152"/>
+      <c r="AN10" s="152"/>
+      <c r="AO10" s="152"/>
+      <c r="AP10" s="153"/>
     </row>
     <row r="11" spans="1:42">
       <c r="A11" s="54"/>
@@ -12711,46 +12711,46 @@
       <c r="C52" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="D52" s="128" t="s">
+      <c r="D52" s="169" t="s">
         <v>24</v>
       </c>
-      <c r="E52" s="128"/>
-      <c r="F52" s="128"/>
-      <c r="G52" s="128"/>
-      <c r="H52" s="128" t="s">
+      <c r="E52" s="169"/>
+      <c r="F52" s="169"/>
+      <c r="G52" s="169"/>
+      <c r="H52" s="169" t="s">
         <v>25</v>
       </c>
-      <c r="I52" s="128"/>
-      <c r="J52" s="128"/>
-      <c r="K52" s="128"/>
-      <c r="L52" s="128"/>
-      <c r="M52" s="128"/>
-      <c r="N52" s="128"/>
-      <c r="O52" s="128"/>
-      <c r="P52" s="128"/>
-      <c r="Q52" s="128"/>
-      <c r="R52" s="128"/>
-      <c r="S52" s="128"/>
-      <c r="T52" s="128"/>
-      <c r="U52" s="128"/>
-      <c r="V52" s="128"/>
-      <c r="W52" s="129" t="s">
+      <c r="I52" s="169"/>
+      <c r="J52" s="169"/>
+      <c r="K52" s="169"/>
+      <c r="L52" s="169"/>
+      <c r="M52" s="169"/>
+      <c r="N52" s="169"/>
+      <c r="O52" s="169"/>
+      <c r="P52" s="169"/>
+      <c r="Q52" s="169"/>
+      <c r="R52" s="169"/>
+      <c r="S52" s="169"/>
+      <c r="T52" s="169"/>
+      <c r="U52" s="169"/>
+      <c r="V52" s="169"/>
+      <c r="W52" s="170" t="s">
         <v>26</v>
       </c>
-      <c r="X52" s="130"/>
-      <c r="Y52" s="130"/>
-      <c r="Z52" s="130"/>
-      <c r="AA52" s="130"/>
-      <c r="AB52" s="130"/>
-      <c r="AC52" s="130"/>
-      <c r="AD52" s="130"/>
-      <c r="AE52" s="130"/>
-      <c r="AF52" s="130"/>
-      <c r="AG52" s="130"/>
-      <c r="AH52" s="130"/>
-      <c r="AI52" s="130"/>
-      <c r="AJ52" s="130"/>
-      <c r="AK52" s="131"/>
+      <c r="X52" s="171"/>
+      <c r="Y52" s="171"/>
+      <c r="Z52" s="171"/>
+      <c r="AA52" s="171"/>
+      <c r="AB52" s="171"/>
+      <c r="AC52" s="171"/>
+      <c r="AD52" s="171"/>
+      <c r="AE52" s="171"/>
+      <c r="AF52" s="171"/>
+      <c r="AG52" s="171"/>
+      <c r="AH52" s="171"/>
+      <c r="AI52" s="171"/>
+      <c r="AJ52" s="171"/>
+      <c r="AK52" s="172"/>
       <c r="AL52" s="5"/>
       <c r="AM52" s="5"/>
       <c r="AN52" s="5"/>
@@ -12763,46 +12763,46 @@
       <c r="C53" s="80">
         <v>1</v>
       </c>
-      <c r="D53" s="136" t="s">
+      <c r="D53" s="158" t="s">
         <v>27</v>
       </c>
-      <c r="E53" s="136"/>
-      <c r="F53" s="136"/>
-      <c r="G53" s="136"/>
-      <c r="H53" s="137" t="s">
+      <c r="E53" s="158"/>
+      <c r="F53" s="158"/>
+      <c r="G53" s="158"/>
+      <c r="H53" s="163" t="s">
         <v>28</v>
       </c>
-      <c r="I53" s="138"/>
-      <c r="J53" s="138"/>
-      <c r="K53" s="138"/>
-      <c r="L53" s="138"/>
-      <c r="M53" s="138"/>
-      <c r="N53" s="138"/>
-      <c r="O53" s="138"/>
-      <c r="P53" s="138"/>
-      <c r="Q53" s="138"/>
-      <c r="R53" s="138"/>
-      <c r="S53" s="138"/>
-      <c r="T53" s="138"/>
-      <c r="U53" s="138"/>
-      <c r="V53" s="139"/>
-      <c r="W53" s="140" t="s">
+      <c r="I53" s="164"/>
+      <c r="J53" s="164"/>
+      <c r="K53" s="164"/>
+      <c r="L53" s="164"/>
+      <c r="M53" s="164"/>
+      <c r="N53" s="164"/>
+      <c r="O53" s="164"/>
+      <c r="P53" s="164"/>
+      <c r="Q53" s="164"/>
+      <c r="R53" s="164"/>
+      <c r="S53" s="164"/>
+      <c r="T53" s="164"/>
+      <c r="U53" s="164"/>
+      <c r="V53" s="165"/>
+      <c r="W53" s="159" t="s">
         <v>29</v>
       </c>
-      <c r="X53" s="141"/>
-      <c r="Y53" s="141"/>
-      <c r="Z53" s="141"/>
-      <c r="AA53" s="141"/>
-      <c r="AB53" s="141"/>
-      <c r="AC53" s="141"/>
-      <c r="AD53" s="141"/>
-      <c r="AE53" s="141"/>
-      <c r="AF53" s="141"/>
-      <c r="AG53" s="141"/>
-      <c r="AH53" s="141"/>
-      <c r="AI53" s="141"/>
-      <c r="AJ53" s="141"/>
-      <c r="AK53" s="142"/>
+      <c r="X53" s="160"/>
+      <c r="Y53" s="160"/>
+      <c r="Z53" s="160"/>
+      <c r="AA53" s="160"/>
+      <c r="AB53" s="160"/>
+      <c r="AC53" s="160"/>
+      <c r="AD53" s="160"/>
+      <c r="AE53" s="160"/>
+      <c r="AF53" s="160"/>
+      <c r="AG53" s="160"/>
+      <c r="AH53" s="160"/>
+      <c r="AI53" s="160"/>
+      <c r="AJ53" s="160"/>
+      <c r="AK53" s="161"/>
       <c r="AL53" s="5"/>
       <c r="AM53" s="5"/>
       <c r="AN53" s="5"/>
@@ -12815,46 +12815,46 @@
       <c r="C54" s="80">
         <v>2</v>
       </c>
-      <c r="D54" s="143" t="s">
+      <c r="D54" s="157" t="s">
         <v>30</v>
       </c>
-      <c r="E54" s="136"/>
-      <c r="F54" s="136"/>
-      <c r="G54" s="136"/>
-      <c r="H54" s="137" t="s">
+      <c r="E54" s="158"/>
+      <c r="F54" s="158"/>
+      <c r="G54" s="158"/>
+      <c r="H54" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="I54" s="138"/>
-      <c r="J54" s="138"/>
-      <c r="K54" s="138"/>
-      <c r="L54" s="138"/>
-      <c r="M54" s="138"/>
-      <c r="N54" s="138"/>
-      <c r="O54" s="138"/>
-      <c r="P54" s="138"/>
-      <c r="Q54" s="138"/>
-      <c r="R54" s="138"/>
-      <c r="S54" s="138"/>
-      <c r="T54" s="138"/>
-      <c r="U54" s="138"/>
-      <c r="V54" s="139"/>
-      <c r="W54" s="140" t="s">
+      <c r="I54" s="164"/>
+      <c r="J54" s="164"/>
+      <c r="K54" s="164"/>
+      <c r="L54" s="164"/>
+      <c r="M54" s="164"/>
+      <c r="N54" s="164"/>
+      <c r="O54" s="164"/>
+      <c r="P54" s="164"/>
+      <c r="Q54" s="164"/>
+      <c r="R54" s="164"/>
+      <c r="S54" s="164"/>
+      <c r="T54" s="164"/>
+      <c r="U54" s="164"/>
+      <c r="V54" s="165"/>
+      <c r="W54" s="159" t="s">
         <v>32</v>
       </c>
-      <c r="X54" s="141"/>
-      <c r="Y54" s="141"/>
-      <c r="Z54" s="141"/>
-      <c r="AA54" s="141"/>
-      <c r="AB54" s="141"/>
-      <c r="AC54" s="141"/>
-      <c r="AD54" s="141"/>
-      <c r="AE54" s="141"/>
-      <c r="AF54" s="141"/>
-      <c r="AG54" s="141"/>
-      <c r="AH54" s="141"/>
-      <c r="AI54" s="141"/>
-      <c r="AJ54" s="141"/>
-      <c r="AK54" s="142"/>
+      <c r="X54" s="160"/>
+      <c r="Y54" s="160"/>
+      <c r="Z54" s="160"/>
+      <c r="AA54" s="160"/>
+      <c r="AB54" s="160"/>
+      <c r="AC54" s="160"/>
+      <c r="AD54" s="160"/>
+      <c r="AE54" s="160"/>
+      <c r="AF54" s="160"/>
+      <c r="AG54" s="160"/>
+      <c r="AH54" s="160"/>
+      <c r="AI54" s="160"/>
+      <c r="AJ54" s="160"/>
+      <c r="AK54" s="161"/>
       <c r="AL54" s="5"/>
       <c r="AM54" s="5"/>
       <c r="AN54" s="5"/>
@@ -12867,46 +12867,46 @@
       <c r="C55" s="80">
         <v>3</v>
       </c>
-      <c r="D55" s="143" t="s">
+      <c r="D55" s="157" t="s">
         <v>33</v>
       </c>
-      <c r="E55" s="136"/>
-      <c r="F55" s="136"/>
-      <c r="G55" s="136"/>
-      <c r="H55" s="137" t="s">
+      <c r="E55" s="158"/>
+      <c r="F55" s="158"/>
+      <c r="G55" s="158"/>
+      <c r="H55" s="163" t="s">
         <v>34</v>
       </c>
-      <c r="I55" s="138"/>
-      <c r="J55" s="138"/>
-      <c r="K55" s="138"/>
-      <c r="L55" s="138"/>
-      <c r="M55" s="138"/>
-      <c r="N55" s="138"/>
-      <c r="O55" s="138"/>
-      <c r="P55" s="138"/>
-      <c r="Q55" s="138"/>
-      <c r="R55" s="138"/>
-      <c r="S55" s="138"/>
-      <c r="T55" s="138"/>
-      <c r="U55" s="138"/>
-      <c r="V55" s="139"/>
-      <c r="W55" s="140" t="s">
+      <c r="I55" s="164"/>
+      <c r="J55" s="164"/>
+      <c r="K55" s="164"/>
+      <c r="L55" s="164"/>
+      <c r="M55" s="164"/>
+      <c r="N55" s="164"/>
+      <c r="O55" s="164"/>
+      <c r="P55" s="164"/>
+      <c r="Q55" s="164"/>
+      <c r="R55" s="164"/>
+      <c r="S55" s="164"/>
+      <c r="T55" s="164"/>
+      <c r="U55" s="164"/>
+      <c r="V55" s="165"/>
+      <c r="W55" s="159" t="s">
         <v>35</v>
       </c>
-      <c r="X55" s="141"/>
-      <c r="Y55" s="141"/>
-      <c r="Z55" s="141"/>
-      <c r="AA55" s="141"/>
-      <c r="AB55" s="141"/>
-      <c r="AC55" s="141"/>
-      <c r="AD55" s="141"/>
-      <c r="AE55" s="141"/>
-      <c r="AF55" s="141"/>
-      <c r="AG55" s="141"/>
-      <c r="AH55" s="141"/>
-      <c r="AI55" s="141"/>
-      <c r="AJ55" s="141"/>
-      <c r="AK55" s="142"/>
+      <c r="X55" s="160"/>
+      <c r="Y55" s="160"/>
+      <c r="Z55" s="160"/>
+      <c r="AA55" s="160"/>
+      <c r="AB55" s="160"/>
+      <c r="AC55" s="160"/>
+      <c r="AD55" s="160"/>
+      <c r="AE55" s="160"/>
+      <c r="AF55" s="160"/>
+      <c r="AG55" s="160"/>
+      <c r="AH55" s="160"/>
+      <c r="AI55" s="160"/>
+      <c r="AJ55" s="160"/>
+      <c r="AK55" s="161"/>
       <c r="AL55" s="5"/>
       <c r="AM55" s="5"/>
       <c r="AN55" s="5"/>
@@ -12919,46 +12919,46 @@
       <c r="C56" s="80">
         <v>4</v>
       </c>
-      <c r="D56" s="143" t="s">
+      <c r="D56" s="157" t="s">
         <v>36</v>
       </c>
-      <c r="E56" s="136"/>
-      <c r="F56" s="136"/>
-      <c r="G56" s="136"/>
-      <c r="H56" s="137" t="s">
+      <c r="E56" s="158"/>
+      <c r="F56" s="158"/>
+      <c r="G56" s="158"/>
+      <c r="H56" s="163" t="s">
         <v>37</v>
       </c>
-      <c r="I56" s="138"/>
-      <c r="J56" s="138"/>
-      <c r="K56" s="138"/>
-      <c r="L56" s="138"/>
-      <c r="M56" s="138"/>
-      <c r="N56" s="138"/>
-      <c r="O56" s="138"/>
-      <c r="P56" s="138"/>
-      <c r="Q56" s="138"/>
-      <c r="R56" s="138"/>
-      <c r="S56" s="138"/>
-      <c r="T56" s="138"/>
-      <c r="U56" s="138"/>
-      <c r="V56" s="139"/>
-      <c r="W56" s="140" t="s">
+      <c r="I56" s="164"/>
+      <c r="J56" s="164"/>
+      <c r="K56" s="164"/>
+      <c r="L56" s="164"/>
+      <c r="M56" s="164"/>
+      <c r="N56" s="164"/>
+      <c r="O56" s="164"/>
+      <c r="P56" s="164"/>
+      <c r="Q56" s="164"/>
+      <c r="R56" s="164"/>
+      <c r="S56" s="164"/>
+      <c r="T56" s="164"/>
+      <c r="U56" s="164"/>
+      <c r="V56" s="165"/>
+      <c r="W56" s="159" t="s">
         <v>38</v>
       </c>
-      <c r="X56" s="141"/>
-      <c r="Y56" s="141"/>
-      <c r="Z56" s="141"/>
-      <c r="AA56" s="141"/>
-      <c r="AB56" s="141"/>
-      <c r="AC56" s="141"/>
-      <c r="AD56" s="141"/>
-      <c r="AE56" s="141"/>
-      <c r="AF56" s="141"/>
-      <c r="AG56" s="141"/>
-      <c r="AH56" s="141"/>
-      <c r="AI56" s="141"/>
-      <c r="AJ56" s="141"/>
-      <c r="AK56" s="142"/>
+      <c r="X56" s="160"/>
+      <c r="Y56" s="160"/>
+      <c r="Z56" s="160"/>
+      <c r="AA56" s="160"/>
+      <c r="AB56" s="160"/>
+      <c r="AC56" s="160"/>
+      <c r="AD56" s="160"/>
+      <c r="AE56" s="160"/>
+      <c r="AF56" s="160"/>
+      <c r="AG56" s="160"/>
+      <c r="AH56" s="160"/>
+      <c r="AI56" s="160"/>
+      <c r="AJ56" s="160"/>
+      <c r="AK56" s="161"/>
       <c r="AL56" s="5"/>
       <c r="AM56" s="5"/>
       <c r="AN56" s="5"/>
@@ -12971,46 +12971,46 @@
       <c r="C57" s="80">
         <v>5</v>
       </c>
-      <c r="D57" s="143" t="s">
+      <c r="D57" s="157" t="s">
         <v>39</v>
       </c>
-      <c r="E57" s="136"/>
-      <c r="F57" s="136"/>
-      <c r="G57" s="136"/>
-      <c r="H57" s="140" t="s">
+      <c r="E57" s="158"/>
+      <c r="F57" s="158"/>
+      <c r="G57" s="158"/>
+      <c r="H57" s="159" t="s">
         <v>40</v>
       </c>
-      <c r="I57" s="141"/>
-      <c r="J57" s="141"/>
-      <c r="K57" s="141"/>
-      <c r="L57" s="141"/>
-      <c r="M57" s="141"/>
-      <c r="N57" s="141"/>
-      <c r="O57" s="141"/>
-      <c r="P57" s="141"/>
-      <c r="Q57" s="141"/>
-      <c r="R57" s="141"/>
-      <c r="S57" s="141"/>
-      <c r="T57" s="141"/>
-      <c r="U57" s="141"/>
-      <c r="V57" s="142"/>
-      <c r="W57" s="140" t="s">
+      <c r="I57" s="160"/>
+      <c r="J57" s="160"/>
+      <c r="K57" s="160"/>
+      <c r="L57" s="160"/>
+      <c r="M57" s="160"/>
+      <c r="N57" s="160"/>
+      <c r="O57" s="160"/>
+      <c r="P57" s="160"/>
+      <c r="Q57" s="160"/>
+      <c r="R57" s="160"/>
+      <c r="S57" s="160"/>
+      <c r="T57" s="160"/>
+      <c r="U57" s="160"/>
+      <c r="V57" s="161"/>
+      <c r="W57" s="159" t="s">
         <v>41</v>
       </c>
-      <c r="X57" s="141"/>
-      <c r="Y57" s="141"/>
-      <c r="Z57" s="141"/>
-      <c r="AA57" s="141"/>
-      <c r="AB57" s="141"/>
-      <c r="AC57" s="141"/>
-      <c r="AD57" s="141"/>
-      <c r="AE57" s="141"/>
-      <c r="AF57" s="141"/>
-      <c r="AG57" s="141"/>
-      <c r="AH57" s="141"/>
-      <c r="AI57" s="141"/>
-      <c r="AJ57" s="141"/>
-      <c r="AK57" s="142"/>
+      <c r="X57" s="160"/>
+      <c r="Y57" s="160"/>
+      <c r="Z57" s="160"/>
+      <c r="AA57" s="160"/>
+      <c r="AB57" s="160"/>
+      <c r="AC57" s="160"/>
+      <c r="AD57" s="160"/>
+      <c r="AE57" s="160"/>
+      <c r="AF57" s="160"/>
+      <c r="AG57" s="160"/>
+      <c r="AH57" s="160"/>
+      <c r="AI57" s="160"/>
+      <c r="AJ57" s="160"/>
+      <c r="AK57" s="161"/>
       <c r="AL57" s="5"/>
       <c r="AM57" s="5"/>
       <c r="AN57" s="5"/>
@@ -13112,45 +13112,45 @@
       <c r="B60" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="144" t="s">
+      <c r="C60" s="162" t="s">
         <v>43</v>
       </c>
-      <c r="D60" s="144"/>
-      <c r="E60" s="144"/>
-      <c r="F60" s="144"/>
-      <c r="G60" s="144"/>
-      <c r="H60" s="144" t="s">
+      <c r="D60" s="162"/>
+      <c r="E60" s="162"/>
+      <c r="F60" s="162"/>
+      <c r="G60" s="162"/>
+      <c r="H60" s="162" t="s">
         <v>44</v>
       </c>
-      <c r="I60" s="144"/>
-      <c r="J60" s="144"/>
-      <c r="K60" s="144"/>
-      <c r="L60" s="144"/>
-      <c r="M60" s="144"/>
-      <c r="N60" s="144"/>
-      <c r="O60" s="144"/>
-      <c r="P60" s="144"/>
-      <c r="Q60" s="144"/>
-      <c r="R60" s="144" t="s">
+      <c r="I60" s="162"/>
+      <c r="J60" s="162"/>
+      <c r="K60" s="162"/>
+      <c r="L60" s="162"/>
+      <c r="M60" s="162"/>
+      <c r="N60" s="162"/>
+      <c r="O60" s="162"/>
+      <c r="P60" s="162"/>
+      <c r="Q60" s="162"/>
+      <c r="R60" s="162" t="s">
         <v>45</v>
       </c>
-      <c r="S60" s="144"/>
-      <c r="T60" s="144"/>
-      <c r="U60" s="144"/>
-      <c r="V60" s="144"/>
-      <c r="W60" s="144"/>
-      <c r="X60" s="144"/>
-      <c r="Y60" s="144"/>
-      <c r="Z60" s="144"/>
-      <c r="AA60" s="144"/>
-      <c r="AB60" s="144"/>
-      <c r="AC60" s="144"/>
-      <c r="AD60" s="144"/>
-      <c r="AE60" s="144"/>
-      <c r="AF60" s="144"/>
-      <c r="AG60" s="144"/>
-      <c r="AH60" s="144"/>
-      <c r="AI60" s="144"/>
+      <c r="S60" s="162"/>
+      <c r="T60" s="162"/>
+      <c r="U60" s="162"/>
+      <c r="V60" s="162"/>
+      <c r="W60" s="162"/>
+      <c r="X60" s="162"/>
+      <c r="Y60" s="162"/>
+      <c r="Z60" s="162"/>
+      <c r="AA60" s="162"/>
+      <c r="AB60" s="162"/>
+      <c r="AC60" s="162"/>
+      <c r="AD60" s="162"/>
+      <c r="AE60" s="162"/>
+      <c r="AF60" s="162"/>
+      <c r="AG60" s="162"/>
+      <c r="AH60" s="162"/>
+      <c r="AI60" s="162"/>
       <c r="AJ60" s="64"/>
       <c r="AK60" s="64"/>
       <c r="AL60" s="64"/>
@@ -13164,13 +13164,13 @@
       <c r="B61" s="83">
         <v>1</v>
       </c>
-      <c r="C61" s="148" t="s">
+      <c r="C61" s="125" t="s">
         <v>46</v>
       </c>
-      <c r="D61" s="149"/>
-      <c r="E61" s="149"/>
-      <c r="F61" s="149"/>
-      <c r="G61" s="150"/>
+      <c r="D61" s="126"/>
+      <c r="E61" s="126"/>
+      <c r="F61" s="126"/>
+      <c r="G61" s="127"/>
       <c r="H61" s="84" t="s">
         <v>47</v>
       </c>
@@ -13183,26 +13183,26 @@
       <c r="O61" s="88"/>
       <c r="P61" s="88"/>
       <c r="Q61" s="88"/>
-      <c r="R61" s="145" t="s">
+      <c r="R61" s="154" t="s">
         <v>48</v>
       </c>
-      <c r="S61" s="146"/>
-      <c r="T61" s="146"/>
-      <c r="U61" s="146"/>
-      <c r="V61" s="146"/>
-      <c r="W61" s="146"/>
-      <c r="X61" s="146"/>
-      <c r="Y61" s="146"/>
-      <c r="Z61" s="146"/>
-      <c r="AA61" s="146"/>
-      <c r="AB61" s="146"/>
-      <c r="AC61" s="146"/>
-      <c r="AD61" s="146"/>
-      <c r="AE61" s="146"/>
-      <c r="AF61" s="146"/>
-      <c r="AG61" s="146"/>
-      <c r="AH61" s="146"/>
-      <c r="AI61" s="147"/>
+      <c r="S61" s="155"/>
+      <c r="T61" s="155"/>
+      <c r="U61" s="155"/>
+      <c r="V61" s="155"/>
+      <c r="W61" s="155"/>
+      <c r="X61" s="155"/>
+      <c r="Y61" s="155"/>
+      <c r="Z61" s="155"/>
+      <c r="AA61" s="155"/>
+      <c r="AB61" s="155"/>
+      <c r="AC61" s="155"/>
+      <c r="AD61" s="155"/>
+      <c r="AE61" s="155"/>
+      <c r="AF61" s="155"/>
+      <c r="AG61" s="155"/>
+      <c r="AH61" s="155"/>
+      <c r="AI61" s="156"/>
       <c r="AJ61" s="5"/>
       <c r="AK61" s="5"/>
       <c r="AL61" s="5"/>
@@ -13216,13 +13216,13 @@
       <c r="B62" s="86">
         <v>2</v>
       </c>
-      <c r="C62" s="148" t="s">
+      <c r="C62" s="125" t="s">
         <v>49</v>
       </c>
-      <c r="D62" s="149"/>
-      <c r="E62" s="149"/>
-      <c r="F62" s="149"/>
-      <c r="G62" s="150"/>
+      <c r="D62" s="126"/>
+      <c r="E62" s="126"/>
+      <c r="F62" s="126"/>
+      <c r="G62" s="127"/>
       <c r="H62" s="87" t="s">
         <v>50</v>
       </c>
@@ -13235,26 +13235,26 @@
       <c r="O62" s="90"/>
       <c r="P62" s="90"/>
       <c r="Q62" s="90"/>
-      <c r="R62" s="151" t="s">
+      <c r="R62" s="128" t="s">
         <v>51</v>
       </c>
-      <c r="S62" s="152"/>
-      <c r="T62" s="152"/>
-      <c r="U62" s="152"/>
-      <c r="V62" s="152"/>
-      <c r="W62" s="152"/>
-      <c r="X62" s="152"/>
-      <c r="Y62" s="152"/>
-      <c r="Z62" s="152"/>
-      <c r="AA62" s="152"/>
-      <c r="AB62" s="152"/>
-      <c r="AC62" s="152"/>
-      <c r="AD62" s="152"/>
-      <c r="AE62" s="152"/>
-      <c r="AF62" s="152"/>
-      <c r="AG62" s="152"/>
-      <c r="AH62" s="152"/>
-      <c r="AI62" s="153"/>
+      <c r="S62" s="129"/>
+      <c r="T62" s="129"/>
+      <c r="U62" s="129"/>
+      <c r="V62" s="129"/>
+      <c r="W62" s="129"/>
+      <c r="X62" s="129"/>
+      <c r="Y62" s="129"/>
+      <c r="Z62" s="129"/>
+      <c r="AA62" s="129"/>
+      <c r="AB62" s="129"/>
+      <c r="AC62" s="129"/>
+      <c r="AD62" s="129"/>
+      <c r="AE62" s="129"/>
+      <c r="AF62" s="129"/>
+      <c r="AG62" s="129"/>
+      <c r="AH62" s="129"/>
+      <c r="AI62" s="130"/>
       <c r="AJ62" s="55"/>
       <c r="AK62" s="55"/>
       <c r="AL62" s="55"/>
@@ -13268,13 +13268,13 @@
       <c r="B63" s="86">
         <v>3</v>
       </c>
-      <c r="C63" s="148" t="s">
+      <c r="C63" s="125" t="s">
         <v>52</v>
       </c>
-      <c r="D63" s="149"/>
-      <c r="E63" s="149"/>
-      <c r="F63" s="149"/>
-      <c r="G63" s="150"/>
+      <c r="D63" s="126"/>
+      <c r="E63" s="126"/>
+      <c r="F63" s="126"/>
+      <c r="G63" s="127"/>
       <c r="H63" s="87" t="s">
         <v>53</v>
       </c>
@@ -13287,26 +13287,26 @@
       <c r="O63" s="90"/>
       <c r="P63" s="90"/>
       <c r="Q63" s="90"/>
-      <c r="R63" s="151" t="s">
+      <c r="R63" s="128" t="s">
         <v>54</v>
       </c>
-      <c r="S63" s="152"/>
-      <c r="T63" s="152"/>
-      <c r="U63" s="152"/>
-      <c r="V63" s="152"/>
-      <c r="W63" s="152"/>
-      <c r="X63" s="152"/>
-      <c r="Y63" s="152"/>
-      <c r="Z63" s="152"/>
-      <c r="AA63" s="152"/>
-      <c r="AB63" s="152"/>
-      <c r="AC63" s="152"/>
-      <c r="AD63" s="152"/>
-      <c r="AE63" s="152"/>
-      <c r="AF63" s="152"/>
-      <c r="AG63" s="152"/>
-      <c r="AH63" s="152"/>
-      <c r="AI63" s="153"/>
+      <c r="S63" s="129"/>
+      <c r="T63" s="129"/>
+      <c r="U63" s="129"/>
+      <c r="V63" s="129"/>
+      <c r="W63" s="129"/>
+      <c r="X63" s="129"/>
+      <c r="Y63" s="129"/>
+      <c r="Z63" s="129"/>
+      <c r="AA63" s="129"/>
+      <c r="AB63" s="129"/>
+      <c r="AC63" s="129"/>
+      <c r="AD63" s="129"/>
+      <c r="AE63" s="129"/>
+      <c r="AF63" s="129"/>
+      <c r="AG63" s="129"/>
+      <c r="AH63" s="129"/>
+      <c r="AI63" s="130"/>
       <c r="AJ63" s="55"/>
       <c r="AK63" s="55"/>
       <c r="AL63" s="55"/>
@@ -13326,13 +13326,13 @@
       <c r="B64" s="86">
         <v>4</v>
       </c>
-      <c r="C64" s="148" t="s">
+      <c r="C64" s="125" t="s">
         <v>55</v>
       </c>
-      <c r="D64" s="149"/>
-      <c r="E64" s="149"/>
-      <c r="F64" s="149"/>
-      <c r="G64" s="150"/>
+      <c r="D64" s="126"/>
+      <c r="E64" s="126"/>
+      <c r="F64" s="126"/>
+      <c r="G64" s="127"/>
       <c r="H64" s="87" t="s">
         <v>56</v>
       </c>
@@ -13345,26 +13345,26 @@
       <c r="O64" s="90"/>
       <c r="P64" s="90"/>
       <c r="Q64" s="90"/>
-      <c r="R64" s="151" t="s">
+      <c r="R64" s="128" t="s">
         <v>57</v>
       </c>
-      <c r="S64" s="152"/>
-      <c r="T64" s="152"/>
-      <c r="U64" s="152"/>
-      <c r="V64" s="152"/>
-      <c r="W64" s="152"/>
-      <c r="X64" s="152"/>
-      <c r="Y64" s="152"/>
-      <c r="Z64" s="152"/>
-      <c r="AA64" s="152"/>
-      <c r="AB64" s="152"/>
-      <c r="AC64" s="152"/>
-      <c r="AD64" s="152"/>
-      <c r="AE64" s="152"/>
-      <c r="AF64" s="152"/>
-      <c r="AG64" s="152"/>
-      <c r="AH64" s="152"/>
-      <c r="AI64" s="153"/>
+      <c r="S64" s="129"/>
+      <c r="T64" s="129"/>
+      <c r="U64" s="129"/>
+      <c r="V64" s="129"/>
+      <c r="W64" s="129"/>
+      <c r="X64" s="129"/>
+      <c r="Y64" s="129"/>
+      <c r="Z64" s="129"/>
+      <c r="AA64" s="129"/>
+      <c r="AB64" s="129"/>
+      <c r="AC64" s="129"/>
+      <c r="AD64" s="129"/>
+      <c r="AE64" s="129"/>
+      <c r="AF64" s="129"/>
+      <c r="AG64" s="129"/>
+      <c r="AH64" s="129"/>
+      <c r="AI64" s="130"/>
       <c r="AJ64" s="55"/>
       <c r="AK64" s="55"/>
       <c r="AL64" s="55"/>
@@ -13384,13 +13384,13 @@
       <c r="B65" s="86">
         <v>5</v>
       </c>
-      <c r="C65" s="148" t="s">
+      <c r="C65" s="125" t="s">
         <v>58</v>
       </c>
-      <c r="D65" s="149"/>
-      <c r="E65" s="149"/>
-      <c r="F65" s="149"/>
-      <c r="G65" s="150"/>
+      <c r="D65" s="126"/>
+      <c r="E65" s="126"/>
+      <c r="F65" s="126"/>
+      <c r="G65" s="127"/>
       <c r="H65" s="87" t="s">
         <v>59</v>
       </c>
@@ -13403,26 +13403,26 @@
       <c r="O65" s="90"/>
       <c r="P65" s="90"/>
       <c r="Q65" s="90"/>
-      <c r="R65" s="151" t="s">
+      <c r="R65" s="128" t="s">
         <v>60</v>
       </c>
-      <c r="S65" s="152"/>
-      <c r="T65" s="152"/>
-      <c r="U65" s="152"/>
-      <c r="V65" s="152"/>
-      <c r="W65" s="152"/>
-      <c r="X65" s="152"/>
-      <c r="Y65" s="152"/>
-      <c r="Z65" s="152"/>
-      <c r="AA65" s="152"/>
-      <c r="AB65" s="152"/>
-      <c r="AC65" s="152"/>
-      <c r="AD65" s="152"/>
-      <c r="AE65" s="152"/>
-      <c r="AF65" s="152"/>
-      <c r="AG65" s="152"/>
-      <c r="AH65" s="152"/>
-      <c r="AI65" s="153"/>
+      <c r="S65" s="129"/>
+      <c r="T65" s="129"/>
+      <c r="U65" s="129"/>
+      <c r="V65" s="129"/>
+      <c r="W65" s="129"/>
+      <c r="X65" s="129"/>
+      <c r="Y65" s="129"/>
+      <c r="Z65" s="129"/>
+      <c r="AA65" s="129"/>
+      <c r="AB65" s="129"/>
+      <c r="AC65" s="129"/>
+      <c r="AD65" s="129"/>
+      <c r="AE65" s="129"/>
+      <c r="AF65" s="129"/>
+      <c r="AG65" s="129"/>
+      <c r="AH65" s="129"/>
+      <c r="AI65" s="130"/>
       <c r="AJ65" s="55"/>
       <c r="AK65" s="55"/>
       <c r="AL65" s="55"/>
@@ -13442,13 +13442,13 @@
       <c r="B66" s="86">
         <v>6</v>
       </c>
-      <c r="C66" s="148" t="s">
+      <c r="C66" s="125" t="s">
         <v>61</v>
       </c>
-      <c r="D66" s="149"/>
-      <c r="E66" s="149"/>
-      <c r="F66" s="149"/>
-      <c r="G66" s="150"/>
+      <c r="D66" s="126"/>
+      <c r="E66" s="126"/>
+      <c r="F66" s="126"/>
+      <c r="G66" s="127"/>
       <c r="H66" s="87" t="s">
         <v>62</v>
       </c>
@@ -13461,26 +13461,26 @@
       <c r="O66" s="90"/>
       <c r="P66" s="90"/>
       <c r="Q66" s="90"/>
-      <c r="R66" s="151" t="s">
+      <c r="R66" s="128" t="s">
         <v>63</v>
       </c>
-      <c r="S66" s="152"/>
-      <c r="T66" s="152"/>
-      <c r="U66" s="152"/>
-      <c r="V66" s="152"/>
-      <c r="W66" s="152"/>
-      <c r="X66" s="152"/>
-      <c r="Y66" s="152"/>
-      <c r="Z66" s="152"/>
-      <c r="AA66" s="152"/>
-      <c r="AB66" s="152"/>
-      <c r="AC66" s="152"/>
-      <c r="AD66" s="152"/>
-      <c r="AE66" s="152"/>
-      <c r="AF66" s="152"/>
-      <c r="AG66" s="152"/>
-      <c r="AH66" s="152"/>
-      <c r="AI66" s="153"/>
+      <c r="S66" s="129"/>
+      <c r="T66" s="129"/>
+      <c r="U66" s="129"/>
+      <c r="V66" s="129"/>
+      <c r="W66" s="129"/>
+      <c r="X66" s="129"/>
+      <c r="Y66" s="129"/>
+      <c r="Z66" s="129"/>
+      <c r="AA66" s="129"/>
+      <c r="AB66" s="129"/>
+      <c r="AC66" s="129"/>
+      <c r="AD66" s="129"/>
+      <c r="AE66" s="129"/>
+      <c r="AF66" s="129"/>
+      <c r="AG66" s="129"/>
+      <c r="AH66" s="129"/>
+      <c r="AI66" s="130"/>
       <c r="AJ66" s="55"/>
       <c r="AK66" s="55"/>
       <c r="AL66" s="55"/>
@@ -13500,11 +13500,11 @@
       <c r="B67" s="86">
         <v>7</v>
       </c>
-      <c r="C67" s="148"/>
-      <c r="D67" s="149"/>
-      <c r="E67" s="149"/>
-      <c r="F67" s="149"/>
-      <c r="G67" s="150"/>
+      <c r="C67" s="125"/>
+      <c r="D67" s="126"/>
+      <c r="E67" s="126"/>
+      <c r="F67" s="126"/>
+      <c r="G67" s="127"/>
       <c r="H67" s="87"/>
       <c r="I67" s="90"/>
       <c r="J67" s="90"/>
@@ -13515,24 +13515,24 @@
       <c r="O67" s="90"/>
       <c r="P67" s="90"/>
       <c r="Q67" s="90"/>
-      <c r="R67" s="151"/>
-      <c r="S67" s="152"/>
-      <c r="T67" s="152"/>
-      <c r="U67" s="152"/>
-      <c r="V67" s="152"/>
-      <c r="W67" s="152"/>
-      <c r="X67" s="152"/>
-      <c r="Y67" s="152"/>
-      <c r="Z67" s="152"/>
-      <c r="AA67" s="152"/>
-      <c r="AB67" s="152"/>
-      <c r="AC67" s="152"/>
-      <c r="AD67" s="152"/>
-      <c r="AE67" s="152"/>
-      <c r="AF67" s="152"/>
-      <c r="AG67" s="152"/>
-      <c r="AH67" s="152"/>
-      <c r="AI67" s="153"/>
+      <c r="R67" s="128"/>
+      <c r="S67" s="129"/>
+      <c r="T67" s="129"/>
+      <c r="U67" s="129"/>
+      <c r="V67" s="129"/>
+      <c r="W67" s="129"/>
+      <c r="X67" s="129"/>
+      <c r="Y67" s="129"/>
+      <c r="Z67" s="129"/>
+      <c r="AA67" s="129"/>
+      <c r="AB67" s="129"/>
+      <c r="AC67" s="129"/>
+      <c r="AD67" s="129"/>
+      <c r="AE67" s="129"/>
+      <c r="AF67" s="129"/>
+      <c r="AG67" s="129"/>
+      <c r="AH67" s="129"/>
+      <c r="AI67" s="130"/>
       <c r="AJ67" s="55"/>
       <c r="AK67" s="55"/>
       <c r="AL67" s="55"/>
@@ -13552,11 +13552,11 @@
       <c r="B68" s="97">
         <v>8</v>
       </c>
-      <c r="C68" s="148"/>
-      <c r="D68" s="149"/>
-      <c r="E68" s="149"/>
-      <c r="F68" s="149"/>
-      <c r="G68" s="150"/>
+      <c r="C68" s="125"/>
+      <c r="D68" s="126"/>
+      <c r="E68" s="126"/>
+      <c r="F68" s="126"/>
+      <c r="G68" s="127"/>
       <c r="H68" s="98"/>
       <c r="I68" s="99"/>
       <c r="J68" s="99"/>
@@ -13567,24 +13567,24 @@
       <c r="O68" s="99"/>
       <c r="P68" s="99"/>
       <c r="Q68" s="99"/>
-      <c r="R68" s="154"/>
-      <c r="S68" s="155"/>
-      <c r="T68" s="155"/>
-      <c r="U68" s="155"/>
-      <c r="V68" s="155"/>
-      <c r="W68" s="155"/>
-      <c r="X68" s="155"/>
-      <c r="Y68" s="155"/>
-      <c r="Z68" s="155"/>
-      <c r="AA68" s="155"/>
-      <c r="AB68" s="155"/>
-      <c r="AC68" s="155"/>
-      <c r="AD68" s="155"/>
-      <c r="AE68" s="155"/>
-      <c r="AF68" s="155"/>
-      <c r="AG68" s="155"/>
-      <c r="AH68" s="155"/>
-      <c r="AI68" s="156"/>
+      <c r="R68" s="131"/>
+      <c r="S68" s="132"/>
+      <c r="T68" s="132"/>
+      <c r="U68" s="132"/>
+      <c r="V68" s="132"/>
+      <c r="W68" s="132"/>
+      <c r="X68" s="132"/>
+      <c r="Y68" s="132"/>
+      <c r="Z68" s="132"/>
+      <c r="AA68" s="132"/>
+      <c r="AB68" s="132"/>
+      <c r="AC68" s="132"/>
+      <c r="AD68" s="132"/>
+      <c r="AE68" s="132"/>
+      <c r="AF68" s="132"/>
+      <c r="AG68" s="132"/>
+      <c r="AH68" s="132"/>
+      <c r="AI68" s="133"/>
       <c r="AJ68" s="55"/>
       <c r="AK68" s="55"/>
       <c r="AL68" s="55"/>
@@ -14832,6 +14832,37 @@
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="G1:AD1"/>
+    <mergeCell ref="AE1:AH1"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="AM1:AP1"/>
+    <mergeCell ref="D52:G52"/>
+    <mergeCell ref="H52:V52"/>
+    <mergeCell ref="W52:AK52"/>
+    <mergeCell ref="AM2:AP3"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="H53:V53"/>
+    <mergeCell ref="W53:AK53"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="H54:V54"/>
+    <mergeCell ref="W54:AK54"/>
+    <mergeCell ref="D55:G55"/>
+    <mergeCell ref="H55:V55"/>
+    <mergeCell ref="W55:AK55"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="H56:V56"/>
+    <mergeCell ref="W56:AK56"/>
+    <mergeCell ref="D57:G57"/>
+    <mergeCell ref="H57:V57"/>
+    <mergeCell ref="W57:AK57"/>
+    <mergeCell ref="C60:G60"/>
+    <mergeCell ref="H60:Q60"/>
+    <mergeCell ref="R60:AI60"/>
+    <mergeCell ref="R61:AI61"/>
+    <mergeCell ref="C62:G62"/>
+    <mergeCell ref="R62:AI62"/>
+    <mergeCell ref="C63:G63"/>
+    <mergeCell ref="R63:AI63"/>
     <mergeCell ref="C67:G67"/>
     <mergeCell ref="R67:AI67"/>
     <mergeCell ref="C68:G68"/>
@@ -14848,37 +14879,6 @@
     <mergeCell ref="C66:G66"/>
     <mergeCell ref="R66:AI66"/>
     <mergeCell ref="C61:G61"/>
-    <mergeCell ref="R61:AI61"/>
-    <mergeCell ref="C62:G62"/>
-    <mergeCell ref="R62:AI62"/>
-    <mergeCell ref="C63:G63"/>
-    <mergeCell ref="R63:AI63"/>
-    <mergeCell ref="D57:G57"/>
-    <mergeCell ref="H57:V57"/>
-    <mergeCell ref="W57:AK57"/>
-    <mergeCell ref="C60:G60"/>
-    <mergeCell ref="H60:Q60"/>
-    <mergeCell ref="R60:AI60"/>
-    <mergeCell ref="D55:G55"/>
-    <mergeCell ref="H55:V55"/>
-    <mergeCell ref="W55:AK55"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="H56:V56"/>
-    <mergeCell ref="W56:AK56"/>
-    <mergeCell ref="D53:G53"/>
-    <mergeCell ref="H53:V53"/>
-    <mergeCell ref="W53:AK53"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="H54:V54"/>
-    <mergeCell ref="W54:AK54"/>
-    <mergeCell ref="G1:AD1"/>
-    <mergeCell ref="AE1:AH1"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="AM1:AP1"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="H52:V52"/>
-    <mergeCell ref="W52:AK52"/>
-    <mergeCell ref="AM2:AP3"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="77" orientation="landscape"/>
@@ -14924,173 +14924,173 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" s="1" customFormat="1">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="144" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="125" t="s">
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
+      <c r="G1" s="166" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="127"/>
-      <c r="L1" s="174" t="s">
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="168"/>
+      <c r="L1" s="177" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="174"/>
-      <c r="N1" s="174"/>
-      <c r="O1" s="174"/>
-      <c r="P1" s="174"/>
-      <c r="Q1" s="174"/>
-      <c r="R1" s="174"/>
-      <c r="S1" s="174"/>
-      <c r="T1" s="174" t="s">
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
+      <c r="P1" s="177"/>
+      <c r="Q1" s="177"/>
+      <c r="R1" s="177"/>
+      <c r="S1" s="177"/>
+      <c r="T1" s="177" t="s">
         <v>71</v>
       </c>
-      <c r="U1" s="174"/>
-      <c r="V1" s="174"/>
-      <c r="W1" s="174"/>
-      <c r="X1" s="174"/>
-      <c r="Y1" s="174"/>
-      <c r="Z1" s="174"/>
-      <c r="AA1" s="174"/>
-      <c r="AB1" s="174"/>
-      <c r="AC1" s="174"/>
-      <c r="AD1" s="174"/>
-      <c r="AE1" s="174"/>
-      <c r="AF1" s="174"/>
-      <c r="AG1" s="125" t="s">
+      <c r="U1" s="177"/>
+      <c r="V1" s="177"/>
+      <c r="W1" s="177"/>
+      <c r="X1" s="177"/>
+      <c r="Y1" s="177"/>
+      <c r="Z1" s="177"/>
+      <c r="AA1" s="177"/>
+      <c r="AB1" s="177"/>
+      <c r="AC1" s="177"/>
+      <c r="AD1" s="177"/>
+      <c r="AE1" s="177"/>
+      <c r="AF1" s="177"/>
+      <c r="AG1" s="166" t="s">
         <v>13</v>
       </c>
-      <c r="AH1" s="126"/>
-      <c r="AI1" s="126"/>
-      <c r="AJ1" s="127"/>
-      <c r="AK1" s="126" t="s">
+      <c r="AH1" s="167"/>
+      <c r="AI1" s="167"/>
+      <c r="AJ1" s="168"/>
+      <c r="AK1" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="AL1" s="126"/>
-      <c r="AM1" s="126"/>
-      <c r="AN1" s="127"/>
-      <c r="AO1" s="125" t="s">
+      <c r="AL1" s="167"/>
+      <c r="AM1" s="167"/>
+      <c r="AN1" s="168"/>
+      <c r="AO1" s="166" t="s">
         <v>15</v>
       </c>
-      <c r="AP1" s="126"/>
-      <c r="AQ1" s="126"/>
-      <c r="AR1" s="127"/>
+      <c r="AP1" s="167"/>
+      <c r="AQ1" s="167"/>
+      <c r="AR1" s="168"/>
     </row>
     <row r="2" spans="1:44" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="163"/>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="157" t="str">
+      <c r="A2" s="144"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="134" t="str">
         <f>T2</f>
         <v>Đăng kí thẻ</v>
       </c>
-      <c r="H2" s="158"/>
-      <c r="I2" s="158"/>
-      <c r="J2" s="158"/>
-      <c r="K2" s="159"/>
-      <c r="L2" s="173" t="str">
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="176" t="str">
         <f>Cover!C61</f>
         <v>UC_001</v>
       </c>
-      <c r="M2" s="173"/>
-      <c r="N2" s="173"/>
-      <c r="O2" s="173"/>
-      <c r="P2" s="173"/>
-      <c r="Q2" s="173"/>
-      <c r="R2" s="173"/>
-      <c r="S2" s="173"/>
-      <c r="T2" s="173" t="str">
+      <c r="M2" s="176"/>
+      <c r="N2" s="176"/>
+      <c r="O2" s="176"/>
+      <c r="P2" s="176"/>
+      <c r="Q2" s="176"/>
+      <c r="R2" s="176"/>
+      <c r="S2" s="176"/>
+      <c r="T2" s="176" t="str">
         <f>Cover!H61</f>
         <v>Đăng kí thẻ</v>
       </c>
-      <c r="U2" s="173"/>
-      <c r="V2" s="173"/>
-      <c r="W2" s="173"/>
-      <c r="X2" s="173"/>
-      <c r="Y2" s="173"/>
-      <c r="Z2" s="173"/>
-      <c r="AA2" s="173"/>
-      <c r="AB2" s="173"/>
-      <c r="AC2" s="173"/>
-      <c r="AD2" s="173"/>
-      <c r="AE2" s="173"/>
-      <c r="AF2" s="173"/>
-      <c r="AG2" s="157" t="s">
+      <c r="U2" s="176"/>
+      <c r="V2" s="176"/>
+      <c r="W2" s="176"/>
+      <c r="X2" s="176"/>
+      <c r="Y2" s="176"/>
+      <c r="Z2" s="176"/>
+      <c r="AA2" s="176"/>
+      <c r="AB2" s="176"/>
+      <c r="AC2" s="176"/>
+      <c r="AD2" s="176"/>
+      <c r="AE2" s="176"/>
+      <c r="AF2" s="176"/>
+      <c r="AG2" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="AH2" s="158"/>
-      <c r="AI2" s="158"/>
-      <c r="AJ2" s="159"/>
-      <c r="AK2" s="132">
+      <c r="AH2" s="135"/>
+      <c r="AI2" s="135"/>
+      <c r="AJ2" s="136"/>
+      <c r="AK2" s="140">
         <f>DATE(2016,2,3)</f>
         <v>42403</v>
       </c>
-      <c r="AL2" s="132"/>
-      <c r="AM2" s="132"/>
-      <c r="AN2" s="133"/>
-      <c r="AO2" s="132">
+      <c r="AL2" s="140"/>
+      <c r="AM2" s="140"/>
+      <c r="AN2" s="141"/>
+      <c r="AO2" s="140">
         <f>DATE(2017,2,12)</f>
         <v>42778</v>
       </c>
-      <c r="AP2" s="132"/>
-      <c r="AQ2" s="132"/>
-      <c r="AR2" s="133"/>
+      <c r="AP2" s="140"/>
+      <c r="AQ2" s="140"/>
+      <c r="AR2" s="141"/>
     </row>
     <row r="3" spans="1:44" s="1" customFormat="1">
-      <c r="A3" s="163"/>
-      <c r="B3" s="163"/>
-      <c r="C3" s="163"/>
-      <c r="D3" s="163"/>
-      <c r="E3" s="163"/>
-      <c r="F3" s="163"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="161"/>
-      <c r="I3" s="161"/>
-      <c r="J3" s="161"/>
-      <c r="K3" s="162"/>
-      <c r="L3" s="173"/>
-      <c r="M3" s="173"/>
-      <c r="N3" s="173"/>
-      <c r="O3" s="173"/>
-      <c r="P3" s="173"/>
-      <c r="Q3" s="173"/>
-      <c r="R3" s="173"/>
-      <c r="S3" s="173"/>
-      <c r="T3" s="173"/>
-      <c r="U3" s="173"/>
-      <c r="V3" s="173"/>
-      <c r="W3" s="173"/>
-      <c r="X3" s="173"/>
-      <c r="Y3" s="173"/>
-      <c r="Z3" s="173"/>
-      <c r="AA3" s="173"/>
-      <c r="AB3" s="173"/>
-      <c r="AC3" s="173"/>
-      <c r="AD3" s="173"/>
-      <c r="AE3" s="173"/>
-      <c r="AF3" s="173"/>
-      <c r="AG3" s="160"/>
-      <c r="AH3" s="161"/>
-      <c r="AI3" s="161"/>
-      <c r="AJ3" s="162"/>
-      <c r="AK3" s="134"/>
-      <c r="AL3" s="134"/>
-      <c r="AM3" s="134"/>
-      <c r="AN3" s="135"/>
-      <c r="AO3" s="134"/>
-      <c r="AP3" s="134"/>
-      <c r="AQ3" s="134"/>
-      <c r="AR3" s="135"/>
+      <c r="A3" s="144"/>
+      <c r="B3" s="144"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="138"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="139"/>
+      <c r="L3" s="176"/>
+      <c r="M3" s="176"/>
+      <c r="N3" s="176"/>
+      <c r="O3" s="176"/>
+      <c r="P3" s="176"/>
+      <c r="Q3" s="176"/>
+      <c r="R3" s="176"/>
+      <c r="S3" s="176"/>
+      <c r="T3" s="176"/>
+      <c r="U3" s="176"/>
+      <c r="V3" s="176"/>
+      <c r="W3" s="176"/>
+      <c r="X3" s="176"/>
+      <c r="Y3" s="176"/>
+      <c r="Z3" s="176"/>
+      <c r="AA3" s="176"/>
+      <c r="AB3" s="176"/>
+      <c r="AC3" s="176"/>
+      <c r="AD3" s="176"/>
+      <c r="AE3" s="176"/>
+      <c r="AF3" s="176"/>
+      <c r="AG3" s="137"/>
+      <c r="AH3" s="138"/>
+      <c r="AI3" s="138"/>
+      <c r="AJ3" s="139"/>
+      <c r="AK3" s="142"/>
+      <c r="AL3" s="142"/>
+      <c r="AM3" s="142"/>
+      <c r="AN3" s="143"/>
+      <c r="AO3" s="142"/>
+      <c r="AP3" s="142"/>
+      <c r="AQ3" s="142"/>
+      <c r="AR3" s="143"/>
     </row>
     <row r="4" spans="1:44">
       <c r="A4" s="4"/>
@@ -16791,9 +16791,9 @@
       <c r="AJ39" s="28"/>
       <c r="AK39" s="28"/>
       <c r="AL39" s="28"/>
-      <c r="AM39" s="176"/>
-      <c r="AN39" s="176"/>
-      <c r="AO39" s="176"/>
+      <c r="AM39" s="173"/>
+      <c r="AN39" s="173"/>
+      <c r="AO39" s="173"/>
       <c r="AP39" s="28"/>
       <c r="AQ39" s="5"/>
       <c r="AR39" s="23"/>
@@ -16837,9 +16837,9 @@
       <c r="AJ40" s="28"/>
       <c r="AK40" s="28"/>
       <c r="AL40" s="28"/>
-      <c r="AM40" s="176"/>
-      <c r="AN40" s="176"/>
-      <c r="AO40" s="176"/>
+      <c r="AM40" s="173"/>
+      <c r="AN40" s="173"/>
+      <c r="AO40" s="173"/>
       <c r="AP40" s="28"/>
       <c r="AQ40" s="5"/>
       <c r="AR40" s="23"/>
@@ -16944,33 +16944,33 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="177"/>
-      <c r="I43" s="177"/>
-      <c r="J43" s="177"/>
-      <c r="K43" s="177"/>
-      <c r="L43" s="177"/>
-      <c r="M43" s="177"/>
-      <c r="N43" s="177"/>
-      <c r="O43" s="177"/>
-      <c r="P43" s="177"/>
-      <c r="Q43" s="177"/>
-      <c r="R43" s="177"/>
-      <c r="S43" s="177"/>
-      <c r="T43" s="177"/>
-      <c r="U43" s="177"/>
-      <c r="V43" s="177"/>
-      <c r="W43" s="177"/>
-      <c r="X43" s="177"/>
-      <c r="Y43" s="177"/>
-      <c r="Z43" s="177"/>
-      <c r="AA43" s="177"/>
-      <c r="AB43" s="177"/>
-      <c r="AC43" s="177"/>
-      <c r="AD43" s="177"/>
-      <c r="AE43" s="177"/>
-      <c r="AF43" s="177"/>
-      <c r="AG43" s="177"/>
-      <c r="AH43" s="177"/>
+      <c r="H43" s="174"/>
+      <c r="I43" s="174"/>
+      <c r="J43" s="174"/>
+      <c r="K43" s="174"/>
+      <c r="L43" s="174"/>
+      <c r="M43" s="174"/>
+      <c r="N43" s="174"/>
+      <c r="O43" s="174"/>
+      <c r="P43" s="174"/>
+      <c r="Q43" s="174"/>
+      <c r="R43" s="174"/>
+      <c r="S43" s="174"/>
+      <c r="T43" s="174"/>
+      <c r="U43" s="174"/>
+      <c r="V43" s="174"/>
+      <c r="W43" s="174"/>
+      <c r="X43" s="174"/>
+      <c r="Y43" s="174"/>
+      <c r="Z43" s="174"/>
+      <c r="AA43" s="174"/>
+      <c r="AB43" s="174"/>
+      <c r="AC43" s="174"/>
+      <c r="AD43" s="174"/>
+      <c r="AE43" s="174"/>
+      <c r="AF43" s="174"/>
+      <c r="AG43" s="174"/>
+      <c r="AH43" s="174"/>
       <c r="AI43" s="53"/>
       <c r="AJ43" s="28"/>
       <c r="AK43" s="28"/>
@@ -16990,33 +16990,33 @@
       <c r="E44" s="28"/>
       <c r="F44" s="28"/>
       <c r="G44" s="28"/>
-      <c r="H44" s="177"/>
-      <c r="I44" s="177"/>
-      <c r="J44" s="177"/>
-      <c r="K44" s="177"/>
-      <c r="L44" s="177"/>
-      <c r="M44" s="177"/>
-      <c r="N44" s="177"/>
-      <c r="O44" s="177"/>
-      <c r="P44" s="177"/>
-      <c r="Q44" s="177"/>
-      <c r="R44" s="177"/>
-      <c r="S44" s="177"/>
-      <c r="T44" s="177"/>
-      <c r="U44" s="177"/>
-      <c r="V44" s="177"/>
-      <c r="W44" s="177"/>
-      <c r="X44" s="177"/>
-      <c r="Y44" s="177"/>
-      <c r="Z44" s="177"/>
-      <c r="AA44" s="177"/>
-      <c r="AB44" s="177"/>
-      <c r="AC44" s="177"/>
-      <c r="AD44" s="177"/>
-      <c r="AE44" s="177"/>
-      <c r="AF44" s="177"/>
-      <c r="AG44" s="177"/>
-      <c r="AH44" s="177"/>
+      <c r="H44" s="174"/>
+      <c r="I44" s="174"/>
+      <c r="J44" s="174"/>
+      <c r="K44" s="174"/>
+      <c r="L44" s="174"/>
+      <c r="M44" s="174"/>
+      <c r="N44" s="174"/>
+      <c r="O44" s="174"/>
+      <c r="P44" s="174"/>
+      <c r="Q44" s="174"/>
+      <c r="R44" s="174"/>
+      <c r="S44" s="174"/>
+      <c r="T44" s="174"/>
+      <c r="U44" s="174"/>
+      <c r="V44" s="174"/>
+      <c r="W44" s="174"/>
+      <c r="X44" s="174"/>
+      <c r="Y44" s="174"/>
+      <c r="Z44" s="174"/>
+      <c r="AA44" s="174"/>
+      <c r="AB44" s="174"/>
+      <c r="AC44" s="174"/>
+      <c r="AD44" s="174"/>
+      <c r="AE44" s="174"/>
+      <c r="AF44" s="174"/>
+      <c r="AG44" s="174"/>
+      <c r="AH44" s="174"/>
       <c r="AI44" s="28"/>
       <c r="AJ44" s="28"/>
       <c r="AK44" s="28"/>
@@ -18318,18 +18318,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="AM39:AO40"/>
-    <mergeCell ref="H43:K44"/>
-    <mergeCell ref="L43:O44"/>
-    <mergeCell ref="P43:T44"/>
-    <mergeCell ref="U43:Y44"/>
-    <mergeCell ref="Z43:AD44"/>
-    <mergeCell ref="AE43:AH44"/>
-    <mergeCell ref="A1:F3"/>
-    <mergeCell ref="H39:K40"/>
-    <mergeCell ref="L39:O40"/>
-    <mergeCell ref="P39:S40"/>
-    <mergeCell ref="T39:W40"/>
     <mergeCell ref="AO1:AR1"/>
     <mergeCell ref="AG2:AJ3"/>
     <mergeCell ref="AK2:AN3"/>
@@ -18342,6 +18330,18 @@
     <mergeCell ref="T1:AF1"/>
     <mergeCell ref="AG1:AJ1"/>
     <mergeCell ref="AK1:AN1"/>
+    <mergeCell ref="A1:F3"/>
+    <mergeCell ref="H39:K40"/>
+    <mergeCell ref="L39:O40"/>
+    <mergeCell ref="P39:S40"/>
+    <mergeCell ref="T39:W40"/>
+    <mergeCell ref="AM39:AO40"/>
+    <mergeCell ref="H43:K44"/>
+    <mergeCell ref="L43:O44"/>
+    <mergeCell ref="P43:T44"/>
+    <mergeCell ref="U43:Y44"/>
+    <mergeCell ref="Z43:AD44"/>
+    <mergeCell ref="AE43:AH44"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="80" fitToHeight="0" orientation="landscape"/>
@@ -18359,8 +18359,8 @@
   </sheetPr>
   <dimension ref="A1:AR97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AX1" sqref="AX1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.42578125" defaultRowHeight="12.75"/>
@@ -18372,170 +18372,170 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" s="1" customFormat="1">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="144" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="125" t="s">
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
+      <c r="G1" s="166" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="127"/>
-      <c r="L1" s="174" t="s">
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="168"/>
+      <c r="L1" s="177" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="174"/>
-      <c r="N1" s="174"/>
-      <c r="O1" s="174"/>
-      <c r="P1" s="174"/>
-      <c r="Q1" s="174"/>
-      <c r="R1" s="174"/>
-      <c r="S1" s="174"/>
-      <c r="T1" s="174" t="s">
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
+      <c r="P1" s="177"/>
+      <c r="Q1" s="177"/>
+      <c r="R1" s="177"/>
+      <c r="S1" s="177"/>
+      <c r="T1" s="177" t="s">
         <v>71</v>
       </c>
-      <c r="U1" s="174"/>
-      <c r="V1" s="174"/>
-      <c r="W1" s="174"/>
-      <c r="X1" s="174"/>
-      <c r="Y1" s="174"/>
-      <c r="Z1" s="174"/>
-      <c r="AA1" s="174"/>
-      <c r="AB1" s="174"/>
-      <c r="AC1" s="174"/>
-      <c r="AD1" s="174"/>
-      <c r="AE1" s="174"/>
-      <c r="AF1" s="174"/>
-      <c r="AG1" s="125" t="s">
+      <c r="U1" s="177"/>
+      <c r="V1" s="177"/>
+      <c r="W1" s="177"/>
+      <c r="X1" s="177"/>
+      <c r="Y1" s="177"/>
+      <c r="Z1" s="177"/>
+      <c r="AA1" s="177"/>
+      <c r="AB1" s="177"/>
+      <c r="AC1" s="177"/>
+      <c r="AD1" s="177"/>
+      <c r="AE1" s="177"/>
+      <c r="AF1" s="177"/>
+      <c r="AG1" s="166" t="s">
         <v>13</v>
       </c>
-      <c r="AH1" s="126"/>
-      <c r="AI1" s="126"/>
-      <c r="AJ1" s="127"/>
-      <c r="AK1" s="126" t="s">
+      <c r="AH1" s="167"/>
+      <c r="AI1" s="167"/>
+      <c r="AJ1" s="168"/>
+      <c r="AK1" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="AL1" s="126"/>
-      <c r="AM1" s="126"/>
-      <c r="AN1" s="127"/>
-      <c r="AO1" s="125" t="s">
+      <c r="AL1" s="167"/>
+      <c r="AM1" s="167"/>
+      <c r="AN1" s="168"/>
+      <c r="AO1" s="166" t="s">
         <v>15</v>
       </c>
-      <c r="AP1" s="126"/>
-      <c r="AQ1" s="126"/>
-      <c r="AR1" s="127"/>
+      <c r="AP1" s="167"/>
+      <c r="AQ1" s="167"/>
+      <c r="AR1" s="168"/>
     </row>
     <row r="2" spans="1:44" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="163"/>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="157" t="str">
+      <c r="A2" s="144"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="134" t="str">
         <f>T2</f>
         <v>Đọc tên</v>
       </c>
-      <c r="H2" s="158"/>
-      <c r="I2" s="158"/>
-      <c r="J2" s="158"/>
-      <c r="K2" s="159"/>
-      <c r="L2" s="173" t="str">
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="176" t="str">
         <f>Cover!C62</f>
         <v>UC_002</v>
       </c>
-      <c r="M2" s="173"/>
-      <c r="N2" s="173"/>
-      <c r="O2" s="173"/>
-      <c r="P2" s="173"/>
-      <c r="Q2" s="173"/>
-      <c r="R2" s="173"/>
-      <c r="S2" s="173"/>
-      <c r="T2" s="173" t="str">
+      <c r="M2" s="176"/>
+      <c r="N2" s="176"/>
+      <c r="O2" s="176"/>
+      <c r="P2" s="176"/>
+      <c r="Q2" s="176"/>
+      <c r="R2" s="176"/>
+      <c r="S2" s="176"/>
+      <c r="T2" s="176" t="str">
         <f>Cover!H62</f>
         <v>Đọc tên</v>
       </c>
-      <c r="U2" s="173"/>
-      <c r="V2" s="173"/>
-      <c r="W2" s="173"/>
-      <c r="X2" s="173"/>
-      <c r="Y2" s="173"/>
-      <c r="Z2" s="173"/>
-      <c r="AA2" s="173"/>
-      <c r="AB2" s="173"/>
-      <c r="AC2" s="173"/>
-      <c r="AD2" s="173"/>
-      <c r="AE2" s="173"/>
-      <c r="AF2" s="173"/>
-      <c r="AG2" s="157" t="s">
+      <c r="U2" s="176"/>
+      <c r="V2" s="176"/>
+      <c r="W2" s="176"/>
+      <c r="X2" s="176"/>
+      <c r="Y2" s="176"/>
+      <c r="Z2" s="176"/>
+      <c r="AA2" s="176"/>
+      <c r="AB2" s="176"/>
+      <c r="AC2" s="176"/>
+      <c r="AD2" s="176"/>
+      <c r="AE2" s="176"/>
+      <c r="AF2" s="176"/>
+      <c r="AG2" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="AH2" s="158"/>
-      <c r="AI2" s="158"/>
-      <c r="AJ2" s="159"/>
-      <c r="AK2" s="132">
+      <c r="AH2" s="135"/>
+      <c r="AI2" s="135"/>
+      <c r="AJ2" s="136"/>
+      <c r="AK2" s="140">
         <f>DATE(2017,2,12)</f>
         <v>42778</v>
       </c>
-      <c r="AL2" s="132"/>
-      <c r="AM2" s="132"/>
-      <c r="AN2" s="133"/>
-      <c r="AO2" s="132"/>
-      <c r="AP2" s="132"/>
-      <c r="AQ2" s="132"/>
-      <c r="AR2" s="133"/>
+      <c r="AL2" s="140"/>
+      <c r="AM2" s="140"/>
+      <c r="AN2" s="141"/>
+      <c r="AO2" s="140"/>
+      <c r="AP2" s="140"/>
+      <c r="AQ2" s="140"/>
+      <c r="AR2" s="141"/>
     </row>
     <row r="3" spans="1:44" s="1" customFormat="1">
-      <c r="A3" s="163"/>
-      <c r="B3" s="163"/>
-      <c r="C3" s="163"/>
-      <c r="D3" s="163"/>
-      <c r="E3" s="163"/>
-      <c r="F3" s="163"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="161"/>
-      <c r="I3" s="161"/>
-      <c r="J3" s="161"/>
-      <c r="K3" s="162"/>
-      <c r="L3" s="173"/>
-      <c r="M3" s="173"/>
-      <c r="N3" s="173"/>
-      <c r="O3" s="173"/>
-      <c r="P3" s="173"/>
-      <c r="Q3" s="173"/>
-      <c r="R3" s="173"/>
-      <c r="S3" s="173"/>
-      <c r="T3" s="173"/>
-      <c r="U3" s="173"/>
-      <c r="V3" s="173"/>
-      <c r="W3" s="173"/>
-      <c r="X3" s="173"/>
-      <c r="Y3" s="173"/>
-      <c r="Z3" s="173"/>
-      <c r="AA3" s="173"/>
-      <c r="AB3" s="173"/>
-      <c r="AC3" s="173"/>
-      <c r="AD3" s="173"/>
-      <c r="AE3" s="173"/>
-      <c r="AF3" s="173"/>
-      <c r="AG3" s="160"/>
-      <c r="AH3" s="161"/>
-      <c r="AI3" s="161"/>
-      <c r="AJ3" s="162"/>
-      <c r="AK3" s="134"/>
-      <c r="AL3" s="134"/>
-      <c r="AM3" s="134"/>
-      <c r="AN3" s="135"/>
-      <c r="AO3" s="134"/>
-      <c r="AP3" s="134"/>
-      <c r="AQ3" s="134"/>
-      <c r="AR3" s="135"/>
+      <c r="A3" s="144"/>
+      <c r="B3" s="144"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="138"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="139"/>
+      <c r="L3" s="176"/>
+      <c r="M3" s="176"/>
+      <c r="N3" s="176"/>
+      <c r="O3" s="176"/>
+      <c r="P3" s="176"/>
+      <c r="Q3" s="176"/>
+      <c r="R3" s="176"/>
+      <c r="S3" s="176"/>
+      <c r="T3" s="176"/>
+      <c r="U3" s="176"/>
+      <c r="V3" s="176"/>
+      <c r="W3" s="176"/>
+      <c r="X3" s="176"/>
+      <c r="Y3" s="176"/>
+      <c r="Z3" s="176"/>
+      <c r="AA3" s="176"/>
+      <c r="AB3" s="176"/>
+      <c r="AC3" s="176"/>
+      <c r="AD3" s="176"/>
+      <c r="AE3" s="176"/>
+      <c r="AF3" s="176"/>
+      <c r="AG3" s="137"/>
+      <c r="AH3" s="138"/>
+      <c r="AI3" s="138"/>
+      <c r="AJ3" s="139"/>
+      <c r="AK3" s="142"/>
+      <c r="AL3" s="142"/>
+      <c r="AM3" s="142"/>
+      <c r="AN3" s="143"/>
+      <c r="AO3" s="142"/>
+      <c r="AP3" s="142"/>
+      <c r="AQ3" s="142"/>
+      <c r="AR3" s="143"/>
     </row>
     <row r="4" spans="1:44">
       <c r="A4" s="4"/>
@@ -22944,102 +22944,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" s="1" customFormat="1">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="144" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="125" t="s">
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144"/>
+      <c r="G1" s="166" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="127"/>
-      <c r="L1" s="174" t="s">
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="168"/>
+      <c r="L1" s="177" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="174"/>
-      <c r="N1" s="174"/>
-      <c r="O1" s="174"/>
-      <c r="P1" s="174"/>
-      <c r="Q1" s="174"/>
-      <c r="R1" s="174"/>
-      <c r="S1" s="174"/>
-      <c r="T1" s="174" t="s">
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
+      <c r="P1" s="177"/>
+      <c r="Q1" s="177"/>
+      <c r="R1" s="177"/>
+      <c r="S1" s="177"/>
+      <c r="T1" s="177" t="s">
         <v>71</v>
       </c>
-      <c r="U1" s="174"/>
-      <c r="V1" s="174"/>
-      <c r="W1" s="174"/>
-      <c r="X1" s="174"/>
-      <c r="Y1" s="174"/>
-      <c r="Z1" s="174"/>
-      <c r="AA1" s="174"/>
-      <c r="AB1" s="174"/>
-      <c r="AC1" s="174"/>
-      <c r="AD1" s="174"/>
-      <c r="AE1" s="174"/>
-      <c r="AF1" s="174"/>
-      <c r="AG1" s="125" t="s">
+      <c r="U1" s="177"/>
+      <c r="V1" s="177"/>
+      <c r="W1" s="177"/>
+      <c r="X1" s="177"/>
+      <c r="Y1" s="177"/>
+      <c r="Z1" s="177"/>
+      <c r="AA1" s="177"/>
+      <c r="AB1" s="177"/>
+      <c r="AC1" s="177"/>
+      <c r="AD1" s="177"/>
+      <c r="AE1" s="177"/>
+      <c r="AF1" s="177"/>
+      <c r="AG1" s="166" t="s">
         <v>13</v>
       </c>
-      <c r="AH1" s="126"/>
-      <c r="AI1" s="126"/>
-      <c r="AJ1" s="127"/>
-      <c r="AK1" s="126" t="s">
+      <c r="AH1" s="167"/>
+      <c r="AI1" s="167"/>
+      <c r="AJ1" s="168"/>
+      <c r="AK1" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="AL1" s="126"/>
-      <c r="AM1" s="126"/>
-      <c r="AN1" s="127"/>
-      <c r="AO1" s="125" t="s">
+      <c r="AL1" s="167"/>
+      <c r="AM1" s="167"/>
+      <c r="AN1" s="168"/>
+      <c r="AO1" s="166" t="s">
         <v>15</v>
       </c>
-      <c r="AP1" s="126"/>
-      <c r="AQ1" s="126"/>
-      <c r="AR1" s="127"/>
+      <c r="AP1" s="167"/>
+      <c r="AQ1" s="167"/>
+      <c r="AR1" s="168"/>
     </row>
     <row r="2" spans="1:44" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="163"/>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="157"/>
-      <c r="H2" s="158"/>
-      <c r="I2" s="158"/>
-      <c r="J2" s="158"/>
-      <c r="K2" s="159"/>
-      <c r="L2" s="173"/>
-      <c r="M2" s="173"/>
-      <c r="N2" s="173"/>
-      <c r="O2" s="173"/>
-      <c r="P2" s="173"/>
-      <c r="Q2" s="173"/>
-      <c r="R2" s="173"/>
-      <c r="S2" s="173"/>
-      <c r="T2" s="173"/>
-      <c r="U2" s="173"/>
-      <c r="V2" s="173"/>
-      <c r="W2" s="173"/>
-      <c r="X2" s="173"/>
-      <c r="Y2" s="173"/>
-      <c r="Z2" s="173"/>
-      <c r="AA2" s="173"/>
-      <c r="AB2" s="173"/>
-      <c r="AC2" s="173"/>
-      <c r="AD2" s="173"/>
-      <c r="AE2" s="173"/>
-      <c r="AF2" s="173"/>
-      <c r="AG2" s="157"/>
-      <c r="AH2" s="158"/>
-      <c r="AI2" s="158"/>
-      <c r="AJ2" s="159"/>
+      <c r="A2" s="144"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="176"/>
+      <c r="M2" s="176"/>
+      <c r="N2" s="176"/>
+      <c r="O2" s="176"/>
+      <c r="P2" s="176"/>
+      <c r="Q2" s="176"/>
+      <c r="R2" s="176"/>
+      <c r="S2" s="176"/>
+      <c r="T2" s="176"/>
+      <c r="U2" s="176"/>
+      <c r="V2" s="176"/>
+      <c r="W2" s="176"/>
+      <c r="X2" s="176"/>
+      <c r="Y2" s="176"/>
+      <c r="Z2" s="176"/>
+      <c r="AA2" s="176"/>
+      <c r="AB2" s="176"/>
+      <c r="AC2" s="176"/>
+      <c r="AD2" s="176"/>
+      <c r="AE2" s="176"/>
+      <c r="AF2" s="176"/>
+      <c r="AG2" s="134"/>
+      <c r="AH2" s="135"/>
+      <c r="AI2" s="135"/>
+      <c r="AJ2" s="136"/>
       <c r="AK2" s="178"/>
       <c r="AL2" s="178"/>
       <c r="AM2" s="178"/>
@@ -23050,42 +23050,42 @@
       <c r="AR2" s="179"/>
     </row>
     <row r="3" spans="1:44" s="1" customFormat="1">
-      <c r="A3" s="163"/>
-      <c r="B3" s="163"/>
-      <c r="C3" s="163"/>
-      <c r="D3" s="163"/>
-      <c r="E3" s="163"/>
-      <c r="F3" s="163"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="161"/>
-      <c r="I3" s="161"/>
-      <c r="J3" s="161"/>
-      <c r="K3" s="162"/>
-      <c r="L3" s="173"/>
-      <c r="M3" s="173"/>
-      <c r="N3" s="173"/>
-      <c r="O3" s="173"/>
-      <c r="P3" s="173"/>
-      <c r="Q3" s="173"/>
-      <c r="R3" s="173"/>
-      <c r="S3" s="173"/>
-      <c r="T3" s="173"/>
-      <c r="U3" s="173"/>
-      <c r="V3" s="173"/>
-      <c r="W3" s="173"/>
-      <c r="X3" s="173"/>
-      <c r="Y3" s="173"/>
-      <c r="Z3" s="173"/>
-      <c r="AA3" s="173"/>
-      <c r="AB3" s="173"/>
-      <c r="AC3" s="173"/>
-      <c r="AD3" s="173"/>
-      <c r="AE3" s="173"/>
-      <c r="AF3" s="173"/>
-      <c r="AG3" s="160"/>
-      <c r="AH3" s="161"/>
-      <c r="AI3" s="161"/>
-      <c r="AJ3" s="162"/>
+      <c r="A3" s="144"/>
+      <c r="B3" s="144"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="138"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="139"/>
+      <c r="L3" s="176"/>
+      <c r="M3" s="176"/>
+      <c r="N3" s="176"/>
+      <c r="O3" s="176"/>
+      <c r="P3" s="176"/>
+      <c r="Q3" s="176"/>
+      <c r="R3" s="176"/>
+      <c r="S3" s="176"/>
+      <c r="T3" s="176"/>
+      <c r="U3" s="176"/>
+      <c r="V3" s="176"/>
+      <c r="W3" s="176"/>
+      <c r="X3" s="176"/>
+      <c r="Y3" s="176"/>
+      <c r="Z3" s="176"/>
+      <c r="AA3" s="176"/>
+      <c r="AB3" s="176"/>
+      <c r="AC3" s="176"/>
+      <c r="AD3" s="176"/>
+      <c r="AE3" s="176"/>
+      <c r="AF3" s="176"/>
+      <c r="AG3" s="137"/>
+      <c r="AH3" s="138"/>
+      <c r="AI3" s="138"/>
+      <c r="AJ3" s="139"/>
       <c r="AK3" s="180"/>
       <c r="AL3" s="180"/>
       <c r="AM3" s="180"/>

</xml_diff>